<commit_message>
set up PDA daily script and cleaned up repo
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24BDE44-9045-4B55-B3F7-53EDBF6B261F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E37E9F-AB05-4E24-ABDD-644EA5988FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="23" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -470,7 +470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,6 +668,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -830,7 +836,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -845,6 +851,7 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -906,7 +913,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.880152199075" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.923933101854" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
@@ -4706,7 +4713,7 @@
     <n v="0.45440000000000003"/>
     <s v="Playing At:  Vancouver Canucks   Home"/>
     <x v="4"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -4745,86 +4752,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L3:N10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item h="1" x="6"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -5278,6 +5206,85 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L3:N10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item h="1" x="6"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5578,23 +5585,23 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -5602,7 +5609,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5610,7 +5617,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -5627,17 +5634,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
       <c r="G4" s="10"/>
       <c r="L4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="13">
         <v>66</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="13">
         <v>38</v>
       </c>
       <c r="O4" s="4">
@@ -5645,7 +5652,7 @@
         <v>0.5757575757575758</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -5670,10 +5677,10 @@
       <c r="L5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="13">
         <v>54</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="13">
         <v>31</v>
       </c>
       <c r="O5" s="4">
@@ -5681,14 +5688,14 @@
         <v>0.57407407407407407</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>3</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="13">
         <v>3</v>
       </c>
       <c r="D6" s="5">
@@ -5710,10 +5717,10 @@
       <c r="L6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="13">
         <v>36</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="13">
         <v>24</v>
       </c>
       <c r="O6" s="4">
@@ -5721,14 +5728,14 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="13">
         <v>10</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="13">
         <v>10</v>
       </c>
       <c r="D7" s="5">
@@ -5737,7 +5744,7 @@
       </c>
       <c r="E7" s="8">
         <f>SUM(C9:C11)</f>
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="6">
         <f>SUM(C6:C8)</f>
@@ -5750,10 +5757,10 @@
       <c r="L7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="13">
         <v>57</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="13">
         <v>35</v>
       </c>
       <c r="O7" s="4">
@@ -5761,14 +5768,14 @@
         <v>0.61403508771929827</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="13">
         <v>72</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="13">
         <v>45</v>
       </c>
       <c r="D8" s="5">
@@ -5777,7 +5784,7 @@
       </c>
       <c r="E8" s="9">
         <f>E7/E6</f>
-        <v>0.56888888888888889</v>
+        <v>0.56444444444444442</v>
       </c>
       <c r="F8" s="7">
         <f>F7/F6</f>
@@ -5790,10 +5797,10 @@
       <c r="L8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="13">
         <v>48</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="13">
         <v>24</v>
       </c>
       <c r="O8" s="4">
@@ -5801,14 +5808,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="13">
         <v>98</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="13">
         <v>58</v>
       </c>
       <c r="D9" s="5">
@@ -5818,25 +5825,25 @@
       <c r="L9" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="13">
         <v>49</v>
       </c>
-      <c r="N9" s="12">
-        <v>34</v>
+      <c r="N9" s="13">
+        <v>33</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="0"/>
-        <v>0.69387755102040816</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.67346938775510201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="13">
         <v>62</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="13">
         <v>34</v>
       </c>
       <c r="D10" s="5">
@@ -5846,49 +5853,49 @@
       <c r="L10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="13">
         <v>310</v>
       </c>
-      <c r="N10" s="12">
-        <v>186</v>
+      <c r="N10" s="13">
+        <v>185</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.59677419354838712</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="13">
         <v>65</v>
       </c>
-      <c r="C11" s="12">
-        <v>36</v>
+      <c r="C11" s="13">
+        <v>35</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="1"/>
-        <v>0.55384615384615388</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="O11" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="13">
         <v>310</v>
       </c>
-      <c r="C12" s="12">
-        <v>186</v>
+      <c r="C12" s="13">
+        <v>185</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.59677419354838712</v>
       </c>
     </row>
   </sheetData>
@@ -5901,24 +5908,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I311"/>
   <sheetViews>
-    <sheetView topLeftCell="A269" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G286" sqref="G286"/>
+    <sheetView topLeftCell="A290" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I311" sqref="I311"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -5947,7 +5954,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -5976,7 +5983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -6005,7 +6012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -6034,7 +6041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -6063,7 +6070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -6092,7 +6099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -6121,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -6150,7 +6157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -6179,7 +6186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -6208,7 +6215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -6237,7 +6244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -6266,7 +6273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -6295,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -6324,7 +6331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -6353,7 +6360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -6382,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -6411,7 +6418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -6440,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -6469,7 +6476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -6498,7 +6505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -6527,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -6556,7 +6563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -6585,7 +6592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -6614,7 +6621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -6643,7 +6650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -6672,7 +6679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -6701,7 +6708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -6730,7 +6737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -6759,7 +6766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -6788,7 +6795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -6817,7 +6824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -6846,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -6875,7 +6882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -6904,7 +6911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -6933,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -6962,7 +6969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -6991,7 +6998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -7020,7 +7027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -7049,7 +7056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -7078,7 +7085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -7107,7 +7114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -7136,7 +7143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -7165,7 +7172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -7194,7 +7201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -7223,7 +7230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -7252,7 +7259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -7281,7 +7288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -7310,7 +7317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -7339,7 +7346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -7368,7 +7375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -7397,7 +7404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -7426,7 +7433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -7455,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -7484,7 +7491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -7513,7 +7520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -7542,7 +7549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -7571,7 +7578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -7600,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -7629,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -7658,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -7687,7 +7694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -7716,7 +7723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -7745,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>87</v>
       </c>
@@ -7774,7 +7781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>87</v>
       </c>
@@ -7803,7 +7810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -7832,7 +7839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -7861,7 +7868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -7890,7 +7897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -7919,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -7948,7 +7955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -7977,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>88</v>
       </c>
@@ -8006,7 +8013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -8035,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -8064,7 +8071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -8093,7 +8100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -8122,7 +8129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -8151,7 +8158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -8180,7 +8187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -8209,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -8238,7 +8245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -8267,7 +8274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -8296,7 +8303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -8325,7 +8332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -8354,7 +8361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -8383,7 +8390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -8412,7 +8419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -8441,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -8470,7 +8477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -8499,7 +8506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -8528,7 +8535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -8557,7 +8564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -8586,7 +8593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>88</v>
       </c>
@@ -8615,7 +8622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>88</v>
       </c>
@@ -8644,7 +8651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -8673,7 +8680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>88</v>
       </c>
@@ -8702,7 +8709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>88</v>
       </c>
@@ -8731,7 +8738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>88</v>
       </c>
@@ -8760,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>88</v>
       </c>
@@ -8789,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -8818,7 +8825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>88</v>
       </c>
@@ -8847,7 +8854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -8876,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>88</v>
       </c>
@@ -8905,7 +8912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>88</v>
       </c>
@@ -8934,7 +8941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>88</v>
       </c>
@@ -8963,7 +8970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>88</v>
       </c>
@@ -8992,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>88</v>
       </c>
@@ -9021,7 +9028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>88</v>
       </c>
@@ -9050,7 +9057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>88</v>
       </c>
@@ -9079,7 +9086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>88</v>
       </c>
@@ -9108,7 +9115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>88</v>
       </c>
@@ -9137,7 +9144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>88</v>
       </c>
@@ -9166,7 +9173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>88</v>
       </c>
@@ -9195,7 +9202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>88</v>
       </c>
@@ -9224,7 +9231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>88</v>
       </c>
@@ -9253,7 +9260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>88</v>
       </c>
@@ -9282,7 +9289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>88</v>
       </c>
@@ -9311,7 +9318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>88</v>
       </c>
@@ -9340,7 +9347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>88</v>
       </c>
@@ -9369,7 +9376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>88</v>
       </c>
@@ -9398,7 +9405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>88</v>
       </c>
@@ -9427,7 +9434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>89</v>
       </c>
@@ -9456,7 +9463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>89</v>
       </c>
@@ -9485,7 +9492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>89</v>
       </c>
@@ -9514,7 +9521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>89</v>
       </c>
@@ -9543,7 +9550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>89</v>
       </c>
@@ -9572,7 +9579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>89</v>
       </c>
@@ -9601,7 +9608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>89</v>
       </c>
@@ -9630,7 +9637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>89</v>
       </c>
@@ -9659,7 +9666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>89</v>
       </c>
@@ -9688,7 +9695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>89</v>
       </c>
@@ -9717,7 +9724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>89</v>
       </c>
@@ -9746,7 +9753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>89</v>
       </c>
@@ -9775,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>89</v>
       </c>
@@ -9804,7 +9811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>89</v>
       </c>
@@ -9833,7 +9840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>89</v>
       </c>
@@ -9862,7 +9869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>89</v>
       </c>
@@ -9891,7 +9898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>89</v>
       </c>
@@ -9920,7 +9927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>89</v>
       </c>
@@ -9949,7 +9956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>89</v>
       </c>
@@ -9978,7 +9985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>89</v>
       </c>
@@ -10007,7 +10014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>89</v>
       </c>
@@ -10036,7 +10043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>89</v>
       </c>
@@ -10065,7 +10072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>89</v>
       </c>
@@ -10094,7 +10101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>89</v>
       </c>
@@ -10123,7 +10130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>89</v>
       </c>
@@ -10152,7 +10159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>89</v>
       </c>
@@ -10181,7 +10188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>89</v>
       </c>
@@ -10210,7 +10217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>89</v>
       </c>
@@ -10239,7 +10246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>89</v>
       </c>
@@ -10268,7 +10275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>89</v>
       </c>
@@ -10297,7 +10304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>89</v>
       </c>
@@ -10326,7 +10333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>89</v>
       </c>
@@ -10355,7 +10362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>89</v>
       </c>
@@ -10384,7 +10391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>89</v>
       </c>
@@ -10413,7 +10420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>89</v>
       </c>
@@ -10442,7 +10449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>89</v>
       </c>
@@ -10471,7 +10478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>90</v>
       </c>
@@ -10500,7 +10507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>90</v>
       </c>
@@ -10529,7 +10536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>90</v>
       </c>
@@ -10558,7 +10565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>90</v>
       </c>
@@ -10587,7 +10594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>90</v>
       </c>
@@ -10616,7 +10623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>90</v>
       </c>
@@ -10645,7 +10652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>90</v>
       </c>
@@ -10674,7 +10681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>90</v>
       </c>
@@ -10703,7 +10710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>90</v>
       </c>
@@ -10732,7 +10739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>90</v>
       </c>
@@ -10761,7 +10768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>90</v>
       </c>
@@ -10790,7 +10797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>90</v>
       </c>
@@ -10819,7 +10826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>90</v>
       </c>
@@ -10848,7 +10855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>90</v>
       </c>
@@ -10877,7 +10884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>90</v>
       </c>
@@ -10906,7 +10913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>90</v>
       </c>
@@ -10935,7 +10942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>90</v>
       </c>
@@ -10964,7 +10971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>90</v>
       </c>
@@ -10993,7 +11000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>90</v>
       </c>
@@ -11022,7 +11029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>90</v>
       </c>
@@ -11051,7 +11058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>90</v>
       </c>
@@ -11080,7 +11087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>90</v>
       </c>
@@ -11109,7 +11116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>90</v>
       </c>
@@ -11138,7 +11145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>90</v>
       </c>
@@ -11167,7 +11174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>90</v>
       </c>
@@ -11196,7 +11203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>90</v>
       </c>
@@ -11225,7 +11232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>90</v>
       </c>
@@ -11254,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>90</v>
       </c>
@@ -11283,7 +11290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>90</v>
       </c>
@@ -11312,7 +11319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>90</v>
       </c>
@@ -11341,7 +11348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>90</v>
       </c>
@@ -11370,7 +11377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>90</v>
       </c>
@@ -11399,7 +11406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>90</v>
       </c>
@@ -11428,7 +11435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>90</v>
       </c>
@@ -11457,7 +11464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>90</v>
       </c>
@@ -11486,7 +11493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>90</v>
       </c>
@@ -11515,7 +11522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>90</v>
       </c>
@@ -11544,7 +11551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>90</v>
       </c>
@@ -11573,7 +11580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>90</v>
       </c>
@@ -11602,7 +11609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>90</v>
       </c>
@@ -11631,7 +11638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>90</v>
       </c>
@@ -11660,7 +11667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>90</v>
       </c>
@@ -11689,7 +11696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>90</v>
       </c>
@@ -11718,7 +11725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>90</v>
       </c>
@@ -11747,7 +11754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>90</v>
       </c>
@@ -11776,7 +11783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>90</v>
       </c>
@@ -11805,7 +11812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>90</v>
       </c>
@@ -11834,7 +11841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>90</v>
       </c>
@@ -11863,7 +11870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>90</v>
       </c>
@@ -11892,7 +11899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>90</v>
       </c>
@@ -11921,7 +11928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>90</v>
       </c>
@@ -11950,7 +11957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>90</v>
       </c>
@@ -11979,7 +11986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>90</v>
       </c>
@@ -12008,7 +12015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>90</v>
       </c>
@@ -12037,7 +12044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>90</v>
       </c>
@@ -12066,7 +12073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>90</v>
       </c>
@@ -12095,7 +12102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>90</v>
       </c>
@@ -12124,7 +12131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>92</v>
       </c>
@@ -12153,7 +12160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>92</v>
       </c>
@@ -12182,7 +12189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>92</v>
       </c>
@@ -12211,7 +12218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>92</v>
       </c>
@@ -12240,7 +12247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>92</v>
       </c>
@@ -12269,7 +12276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>92</v>
       </c>
@@ -12298,7 +12305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>92</v>
       </c>
@@ -12327,7 +12334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>92</v>
       </c>
@@ -12356,7 +12363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>92</v>
       </c>
@@ -12385,7 +12392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>92</v>
       </c>
@@ -12414,7 +12421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>92</v>
       </c>
@@ -12443,7 +12450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>92</v>
       </c>
@@ -12472,7 +12479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>92</v>
       </c>
@@ -12501,7 +12508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>92</v>
       </c>
@@ -12530,7 +12537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>92</v>
       </c>
@@ -12559,7 +12566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>92</v>
       </c>
@@ -12588,7 +12595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>92</v>
       </c>
@@ -12617,7 +12624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>92</v>
       </c>
@@ -12646,7 +12653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>92</v>
       </c>
@@ -12675,7 +12682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>92</v>
       </c>
@@ -12704,7 +12711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>92</v>
       </c>
@@ -12733,7 +12740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>92</v>
       </c>
@@ -12762,7 +12769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>92</v>
       </c>
@@ -12791,7 +12798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>92</v>
       </c>
@@ -12820,7 +12827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>92</v>
       </c>
@@ -12849,7 +12856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>92</v>
       </c>
@@ -12878,7 +12885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>92</v>
       </c>
@@ -12907,7 +12914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>92</v>
       </c>
@@ -12936,7 +12943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>92</v>
       </c>
@@ -12965,7 +12972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>92</v>
       </c>
@@ -12994,7 +13001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>92</v>
       </c>
@@ -13023,7 +13030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>92</v>
       </c>
@@ -13052,7 +13059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>92</v>
       </c>
@@ -13081,7 +13088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>92</v>
       </c>
@@ -13110,7 +13117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>92</v>
       </c>
@@ -13139,7 +13146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>92</v>
       </c>
@@ -13168,7 +13175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>92</v>
       </c>
@@ -13197,7 +13204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>92</v>
       </c>
@@ -13226,7 +13233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>92</v>
       </c>
@@ -13255,7 +13262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>92</v>
       </c>
@@ -13284,7 +13291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>92</v>
       </c>
@@ -13313,7 +13320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>92</v>
       </c>
@@ -13342,7 +13349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>92</v>
       </c>
@@ -13371,7 +13378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>92</v>
       </c>
@@ -13400,7 +13407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>92</v>
       </c>
@@ -13429,7 +13436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>92</v>
       </c>
@@ -13458,7 +13465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>92</v>
       </c>
@@ -13487,7 +13494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>92</v>
       </c>
@@ -13516,7 +13523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>91</v>
       </c>
@@ -13545,7 +13552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>91</v>
       </c>
@@ -13574,7 +13581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>91</v>
       </c>
@@ -13603,7 +13610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>91</v>
       </c>
@@ -13632,7 +13639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>91</v>
       </c>
@@ -13661,7 +13668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>91</v>
       </c>
@@ -13690,7 +13697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>91</v>
       </c>
@@ -13719,7 +13726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>91</v>
       </c>
@@ -13748,7 +13755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>91</v>
       </c>
@@ -13777,7 +13784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>91</v>
       </c>
@@ -13806,7 +13813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>91</v>
       </c>
@@ -13835,7 +13842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>91</v>
       </c>
@@ -13864,7 +13871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>91</v>
       </c>
@@ -13893,7 +13900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>91</v>
       </c>
@@ -13922,7 +13929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>91</v>
       </c>
@@ -13951,7 +13958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>91</v>
       </c>
@@ -13980,7 +13987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>91</v>
       </c>
@@ -14009,7 +14016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>91</v>
       </c>
@@ -14038,7 +14045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>91</v>
       </c>
@@ -14067,7 +14074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>91</v>
       </c>
@@ -14096,7 +14103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>91</v>
       </c>
@@ -14125,7 +14132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>91</v>
       </c>
@@ -14154,7 +14161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>91</v>
       </c>
@@ -14183,7 +14190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>91</v>
       </c>
@@ -14212,7 +14219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>91</v>
       </c>
@@ -14241,7 +14248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>91</v>
       </c>
@@ -14270,7 +14277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>91</v>
       </c>
@@ -14299,7 +14306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>91</v>
       </c>
@@ -14328,7 +14335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>91</v>
       </c>
@@ -14357,7 +14364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>91</v>
       </c>
@@ -14386,7 +14393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>91</v>
       </c>
@@ -14415,7 +14422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>91</v>
       </c>
@@ -14444,7 +14451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>91</v>
       </c>
@@ -14473,7 +14480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>91</v>
       </c>
@@ -14502,7 +14509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>91</v>
       </c>
@@ -14531,7 +14538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>91</v>
       </c>
@@ -14560,7 +14567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>91</v>
       </c>
@@ -14589,7 +14596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>91</v>
       </c>
@@ -14618,7 +14625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>91</v>
       </c>
@@ -14643,11 +14650,11 @@
       <c r="H301" t="s">
         <v>51</v>
       </c>
-      <c r="I301">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I301" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>91</v>
       </c>
@@ -14672,11 +14679,11 @@
       <c r="H302" t="s">
         <v>52</v>
       </c>
-      <c r="I302">
+      <c r="I302" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>91</v>
       </c>
@@ -14701,11 +14708,11 @@
       <c r="H303" t="s">
         <v>52</v>
       </c>
-      <c r="I303">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I303" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>91</v>
       </c>
@@ -14734,7 +14741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>91</v>
       </c>
@@ -14763,7 +14770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>91</v>
       </c>
@@ -14788,11 +14795,11 @@
       <c r="H306" t="s">
         <v>85</v>
       </c>
-      <c r="I306">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I306" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>91</v>
       </c>
@@ -14817,11 +14824,11 @@
       <c r="H307" t="s">
         <v>85</v>
       </c>
-      <c r="I307">
+      <c r="I307" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>91</v>
       </c>
@@ -14850,7 +14857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>91</v>
       </c>
@@ -14875,11 +14882,11 @@
       <c r="H309" t="s">
         <v>86</v>
       </c>
-      <c r="I309">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I309" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>91</v>
       </c>
@@ -14908,7 +14915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
cleaned up code/retrained model/updated predictions
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EB57FE-9A4A-4A72-AE8B-D1963A56AA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EF15BB-48D1-49BD-8A99-06D2AEADFEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="14" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>75% or greater</t>
+  </si>
+  <si>
+    <t>PDA7</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -866,10 +869,12 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -930,24 +935,25 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.949893287034" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45312.431761342596" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="318" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Model Used" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
+      <sharedItems containsBlank="1" count="8">
         <s v="PDA1"/>
         <s v="PDA2"/>
         <s v="PDA3"/>
         <s v="PDA4"/>
         <s v="PDA5"/>
         <s v="PDA6"/>
+        <s v="PDA7"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-21T00:00:00" count="41">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-22T00:00:00" count="42">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -988,14 +994,15 @@
         <d v="2024-01-18T00:00:00"/>
         <d v="2024-01-19T00:00:00"/>
         <d v="2024-01-20T00:00:00"/>
+        <d v="2024-01-21T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Winner1" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Winner Probability" numFmtId="164">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.50009999999999999" maxValue="0.87610539305886403" count="608">
+    <cacheField name="Winner Probability" numFmtId="0">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.50009999999999999" maxValue="0.87610539305886403" count="614">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1294,6 +1301,12 @@
         <n v="0.55630000000000002"/>
         <n v="0.52470000000000006"/>
         <n v="0.52190000000000003"/>
+        <n v="0.77761999999999998"/>
+        <n v="0.62456999999999996"/>
+        <n v="0.58115000000000006"/>
+        <n v="0.58060999999999996"/>
+        <n v="0.54981999999999998"/>
+        <n v="0.52839000000000003"/>
         <m/>
         <n v="0.87610539305886403" u="1"/>
         <n v="0.78056782297496197" u="1"/>
@@ -1609,7 +1622,7 @@
     <cacheField name="Loser1" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Loser Probability" numFmtId="164">
+    <cacheField name="Loser Probability" numFmtId="0">
       <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.1239" maxValue="0.49990000000000001"/>
     </cacheField>
     <cacheField name="Site" numFmtId="0">
@@ -1642,7 +1655,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="311">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="318">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -5018,7 +5031,7 @@
     <n v="0.43780000000000002"/>
     <s v="Playing At:  San Jose Sharks   Home"/>
     <x v="3"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -5029,7 +5042,7 @@
     <n v="0.44369999999999998"/>
     <s v="Playing At:  Los Angeles Kings   Home"/>
     <x v="3"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -5056,30 +5069,108 @@
   <r>
     <x v="6"/>
     <x v="40"/>
+    <s v="New York Rangers"/>
+    <x v="298"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.22237999999999999"/>
+    <s v="Playing At:  Anaheim Ducks   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="40"/>
+    <s v="Carolina Hurricanes"/>
+    <x v="299"/>
+    <s v="Minnesota Wild"/>
+    <n v="0.37542999999999999"/>
+    <s v="Playing At:  Carolina Hurricanes   Home"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="40"/>
+    <s v="Tampa Bay Lightning"/>
+    <x v="300"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.41885"/>
+    <s v="Playing At:  Detroit Red Wings   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="40"/>
+    <s v="Dallas Stars"/>
+    <x v="301"/>
+    <s v="New York Islanders"/>
+    <n v="0.41938999999999999"/>
+    <s v="Playing At:  New York Islanders   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="40"/>
+    <s v="Toronto Maple Leafs"/>
+    <x v="302"/>
+    <s v="Seattle Kraken"/>
+    <n v="0.45018000000000002"/>
+    <s v="Playing At:  Seattle Kraken   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="40"/>
+    <s v="Ottawa Senators"/>
+    <x v="303"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.47160999999999997"/>
+    <s v="Playing At:  Philadelphia Flyers   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
     <m/>
-    <x v="298"/>
+    <x v="304"/>
     <m/>
     <m/>
     <m/>
     <x v="7"/>
     <m/>
   </r>
+  <r>
+    <x v="7"/>
+    <x v="41"/>
+    <m/>
+    <x v="304"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="7"/>
+    <m/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L3:N10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item h="1" x="6"/>
+      <items count="9">
+        <item h="1" x="7"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item h="1" x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5147,23 +5238,24 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="8">
-        <item x="6"/>
+      <items count="9">
+        <item x="7"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="42">
+      <items count="43">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -5203,21 +5295,16 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
+        <item x="41"/>
+        <item x="39"/>
         <item x="40"/>
-        <item x="39"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="609">
-        <item x="298"/>
-        <item m="1" x="299"/>
-        <item m="1" x="300"/>
-        <item m="1" x="301"/>
-        <item m="1" x="302"/>
-        <item m="1" x="303"/>
-        <item m="1" x="304"/>
+      <items count="615">
+        <item x="304"/>
         <item m="1" x="305"/>
         <item m="1" x="306"/>
         <item m="1" x="307"/>
@@ -5520,8 +5607,14 @@
         <item m="1" x="604"/>
         <item m="1" x="605"/>
         <item m="1" x="606"/>
+        <item m="1" x="607"/>
+        <item m="1" x="608"/>
+        <item m="1" x="609"/>
+        <item m="1" x="610"/>
+        <item m="1" x="611"/>
+        <item m="1" x="612"/>
         <item x="9"/>
-        <item m="1" x="607"/>
+        <item m="1" x="613"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -5819,6 +5912,12 @@
         <item x="283"/>
         <item x="284"/>
         <item x="285"/>
+        <item x="298"/>
+        <item x="299"/>
+        <item x="300"/>
+        <item x="301"/>
+        <item x="302"/>
+        <item x="303"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6202,8 +6301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6256,15 +6355,15 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="10"/>
       <c r="L4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="16">
         <v>66</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="16">
         <v>38</v>
       </c>
       <c r="O4" s="4">
@@ -6291,7 +6390,7 @@
       <c r="F5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>98</v>
       </c>
       <c r="H5" s="10" t="s">
@@ -6300,10 +6399,10 @@
       <c r="L5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="16">
         <v>54</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="16">
         <v>31</v>
       </c>
       <c r="O5" s="4">
@@ -6315,10 +6414,10 @@
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="16">
         <v>4</v>
       </c>
       <c r="D6" s="5">
@@ -6327,15 +6426,15 @@
       </c>
       <c r="E6" s="8">
         <f>SUM(B10:B12)</f>
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F6" s="6">
         <f>SUM(B6:B9)</f>
-        <v>85</v>
-      </c>
-      <c r="G6" s="13">
+        <v>86</v>
+      </c>
+      <c r="G6" s="12">
         <f>SUM(B6:B8)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H6" s="10">
         <f>SUM(B6:B7)</f>
@@ -6344,10 +6443,10 @@
       <c r="L6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="16">
         <v>36</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="16">
         <v>24</v>
       </c>
       <c r="O6" s="4">
@@ -6359,10 +6458,10 @@
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="16">
         <v>9</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="16">
         <v>9</v>
       </c>
       <c r="D7" s="5">
@@ -6371,15 +6470,15 @@
       </c>
       <c r="E7" s="8">
         <f>SUM(C10:C12)</f>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F7" s="6">
         <f>SUM(C6:C9)</f>
-        <v>58</v>
-      </c>
-      <c r="G7" s="13">
+        <v>59</v>
+      </c>
+      <c r="G7" s="12">
         <f>SUM(C6:C8)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="10">
         <f>SUM(C6:C7)</f>
@@ -6388,10 +6487,10 @@
       <c r="L7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="16">
         <v>57</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="16">
         <v>35</v>
       </c>
       <c r="O7" s="4">
@@ -6403,27 +6502,27 @@
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="12">
-        <v>33</v>
-      </c>
-      <c r="C8" s="12">
-        <v>19</v>
+      <c r="B8" s="16">
+        <v>34</v>
+      </c>
+      <c r="C8" s="16">
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="1"/>
-        <v>0.5757575757575758</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="E8" s="9">
         <f>E7/E6</f>
-        <v>0.56444444444444442</v>
+        <v>0.55652173913043479</v>
       </c>
       <c r="F8" s="7">
         <f>F7/F6</f>
-        <v>0.68235294117647061</v>
-      </c>
-      <c r="G8" s="14">
+        <v>0.68604651162790697</v>
+      </c>
+      <c r="G8" s="13">
         <f>G7/G6</f>
-        <v>0.69565217391304346</v>
+        <v>0.7021276595744681</v>
       </c>
       <c r="H8" s="11">
         <f>H7/H6</f>
@@ -6432,10 +6531,10 @@
       <c r="L8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="16">
         <v>48</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="16">
         <v>24</v>
       </c>
       <c r="O8" s="4">
@@ -6447,10 +6546,10 @@
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="16">
         <v>39</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="16">
         <v>26</v>
       </c>
       <c r="D9" s="5">
@@ -6460,58 +6559,58 @@
       <c r="L9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="16">
         <v>49</v>
       </c>
-      <c r="N9" s="12">
-        <v>33</v>
+      <c r="N9" s="16">
+        <v>31</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="0"/>
-        <v>0.67346938775510201</v>
+        <v>0.63265306122448983</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="12">
-        <v>98</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B10" s="16">
+        <v>99</v>
+      </c>
+      <c r="C10" s="16">
         <v>58</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="1"/>
-        <v>0.59183673469387754</v>
+        <v>0.58585858585858586</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="16">
         <v>310</v>
       </c>
-      <c r="N10" s="12">
-        <v>185</v>
+      <c r="N10" s="16">
+        <v>183</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="0"/>
-        <v>0.59677419354838712</v>
+        <v>0.5903225806451613</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="12">
-        <v>64</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B11" s="16">
+        <v>66</v>
+      </c>
+      <c r="C11" s="16">
         <v>36</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="1"/>
-        <v>0.5625</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="O11" s="4" t="e">
         <f t="shared" si="0"/>
@@ -6522,30 +6621,30 @@
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="12">
-        <v>63</v>
-      </c>
-      <c r="C12" s="12">
-        <v>33</v>
+      <c r="B12" s="16">
+        <v>65</v>
+      </c>
+      <c r="C12" s="16">
+        <v>34</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="1"/>
-        <v>0.52380952380952384</v>
+        <v>0.52307692307692311</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="12">
-        <v>310</v>
-      </c>
-      <c r="C13" s="12">
-        <v>185</v>
+      <c r="B13" s="16">
+        <v>316</v>
+      </c>
+      <c r="C13" s="16">
+        <v>187</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="1"/>
-        <v>0.59677419354838712</v>
+        <v>0.59177215189873422</v>
       </c>
     </row>
   </sheetData>
@@ -6556,10 +6655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I311"/>
+  <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C315" sqref="C315"/>
+    <sheetView topLeftCell="A293" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A312" sqref="A312:XFD312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12299,7 +12398,7 @@
       <c r="C198" t="s">
         <v>43</v>
       </c>
-      <c r="D198" s="15" t="s">
+      <c r="D198" s="14" t="s">
         <v>95</v>
       </c>
       <c r="E198" t="s">
@@ -13436,7 +13535,7 @@
       <c r="E237" t="s">
         <v>37</v>
       </c>
-      <c r="F237" s="15" t="s">
+      <c r="F237" s="14" t="s">
         <v>96</v>
       </c>
       <c r="G237" t="s">
@@ -14184,7 +14283,7 @@
       <c r="C263" t="s">
         <v>25</v>
       </c>
-      <c r="D263" s="15" t="s">
+      <c r="D263" s="14" t="s">
         <v>97</v>
       </c>
       <c r="E263" t="s">
@@ -15272,7 +15371,7 @@
       <c r="H300" t="s">
         <v>61</v>
       </c>
-      <c r="I300" s="13">
+      <c r="I300" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15301,7 +15400,7 @@
       <c r="H301" t="s">
         <v>94</v>
       </c>
-      <c r="I301" s="13">
+      <c r="I301" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15330,7 +15429,7 @@
       <c r="H302" t="s">
         <v>51</v>
       </c>
-      <c r="I302" s="13">
+      <c r="I302" s="15">
         <v>0</v>
       </c>
     </row>
@@ -15359,7 +15458,7 @@
       <c r="H303" t="s">
         <v>51</v>
       </c>
-      <c r="I303">
+      <c r="I303" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15388,7 +15487,7 @@
       <c r="H304" t="s">
         <v>51</v>
       </c>
-      <c r="I304">
+      <c r="I304" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15417,7 +15516,7 @@
       <c r="H305" t="s">
         <v>51</v>
       </c>
-      <c r="I305" s="13">
+      <c r="I305" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15446,7 +15545,7 @@
       <c r="H306" t="s">
         <v>84</v>
       </c>
-      <c r="I306" s="13">
+      <c r="I306" s="15">
         <v>1</v>
       </c>
     </row>
@@ -15475,7 +15574,7 @@
       <c r="H307" t="s">
         <v>84</v>
       </c>
-      <c r="I307" s="13">
+      <c r="I307" s="15">
         <v>0</v>
       </c>
     </row>
@@ -15504,8 +15603,8 @@
       <c r="H308" t="s">
         <v>84</v>
       </c>
-      <c r="I308">
-        <v>1</v>
+      <c r="I308" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.35">
@@ -15533,8 +15632,8 @@
       <c r="H309" t="s">
         <v>84</v>
       </c>
-      <c r="I309">
-        <v>1</v>
+      <c r="I309" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.35">
@@ -15562,7 +15661,7 @@
       <c r="H310" t="s">
         <v>85</v>
       </c>
-      <c r="I310" s="13">
+      <c r="I310" s="15">
         <v>0</v>
       </c>
     </row>
@@ -15591,8 +15690,182 @@
       <c r="H311" t="s">
         <v>85</v>
       </c>
-      <c r="I311" s="13">
-        <v>1</v>
+      <c r="I311" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>99</v>
+      </c>
+      <c r="B312" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C312" t="s">
+        <v>25</v>
+      </c>
+      <c r="D312" s="17">
+        <v>0.77761999999999998</v>
+      </c>
+      <c r="E312" t="s">
+        <v>17</v>
+      </c>
+      <c r="F312" s="17">
+        <v>0.22237999999999999</v>
+      </c>
+      <c r="G312" t="s">
+        <v>18</v>
+      </c>
+      <c r="H312" t="s">
+        <v>93</v>
+      </c>
+      <c r="I312" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>99</v>
+      </c>
+      <c r="B313" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C313" t="s">
+        <v>43</v>
+      </c>
+      <c r="D313" s="17">
+        <v>0.62456999999999996</v>
+      </c>
+      <c r="E313" t="s">
+        <v>58</v>
+      </c>
+      <c r="F313" s="17">
+        <v>0.37542999999999999</v>
+      </c>
+      <c r="G313" t="s">
+        <v>74</v>
+      </c>
+      <c r="H313" t="s">
+        <v>51</v>
+      </c>
+      <c r="I313" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>99</v>
+      </c>
+      <c r="B314" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C314" t="s">
+        <v>22</v>
+      </c>
+      <c r="D314" s="17">
+        <v>0.58115000000000006</v>
+      </c>
+      <c r="E314" t="s">
+        <v>37</v>
+      </c>
+      <c r="F314" s="17">
+        <v>0.41885</v>
+      </c>
+      <c r="G314" t="s">
+        <v>38</v>
+      </c>
+      <c r="H314" t="s">
+        <v>84</v>
+      </c>
+      <c r="I314" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>99</v>
+      </c>
+      <c r="B315" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C315" t="s">
+        <v>28</v>
+      </c>
+      <c r="D315" s="17">
+        <v>0.58060999999999996</v>
+      </c>
+      <c r="E315" t="s">
+        <v>39</v>
+      </c>
+      <c r="F315" s="17">
+        <v>0.41938999999999999</v>
+      </c>
+      <c r="G315" t="s">
+        <v>41</v>
+      </c>
+      <c r="H315" t="s">
+        <v>84</v>
+      </c>
+      <c r="I315" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>99</v>
+      </c>
+      <c r="B316" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C316" t="s">
+        <v>19</v>
+      </c>
+      <c r="D316" s="17">
+        <v>0.54981999999999998</v>
+      </c>
+      <c r="E316" t="s">
+        <v>23</v>
+      </c>
+      <c r="F316" s="17">
+        <v>0.45018000000000002</v>
+      </c>
+      <c r="G316" t="s">
+        <v>24</v>
+      </c>
+      <c r="H316" t="s">
+        <v>85</v>
+      </c>
+      <c r="I316" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>99</v>
+      </c>
+      <c r="B317" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C317" t="s">
+        <v>36</v>
+      </c>
+      <c r="D317" s="17">
+        <v>0.52839000000000003</v>
+      </c>
+      <c r="E317" t="s">
+        <v>8</v>
+      </c>
+      <c r="F317" s="17">
+        <v>0.47160999999999997</v>
+      </c>
+      <c r="G317" t="s">
+        <v>73</v>
+      </c>
+      <c r="H317" t="s">
+        <v>85</v>
+      </c>
+      <c r="I317" s="15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated predictions/messing around with EDA
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA42F25A-506B-452B-8C4C-A52C4FE5EA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5BF79B-737D-4289-BCBB-E95DCE80AE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="35" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -359,6 +359,9 @@
   <si>
     <t>PDA7 Total</t>
   </si>
+  <si>
+    <t>% Of Predictions</t>
+  </si>
 </sst>
 </file>
 
@@ -509,7 +512,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +716,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -875,7 +884,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -893,6 +902,7 @@
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -954,7 +964,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45315.3350587963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="339" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45316.94707858796" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="348" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
@@ -972,7 +982,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-25T00:00:00" count="45">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-26T00:00:00" count="46">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1017,6 +1027,7 @@
         <d v="2024-01-22T00:00:00"/>
         <d v="2024-01-23T00:00:00"/>
         <d v="2024-01-24T00:00:00"/>
+        <d v="2024-01-25T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1024,7 +1035,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="634">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="642">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1350,6 +1361,14 @@
         <n v="0.61480000000000001"/>
         <n v="0.57620000000000005"/>
         <n v="0.50680000000000003"/>
+        <n v="0.78939999999999999"/>
+        <n v="0.75160000000000005"/>
+        <n v="0.74780000000000002"/>
+        <n v="0.71889999999999998"/>
+        <n v="0.64839999999999998"/>
+        <n v="0.55449999999999999"/>
+        <n v="0.53690000000000004"/>
+        <n v="0.52159999999999995"/>
         <m/>
         <n v="0.87610539305886403" u="1"/>
         <n v="0.78056782297496197" u="1"/>
@@ -1697,7 +1716,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="339">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="348">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -5359,7 +5378,7 @@
     <n v="0.32290000000000002"/>
     <s v="Playing At:  Florida Panthers   Home"/>
     <x v="2"/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <x v="6"/>
@@ -5381,7 +5400,7 @@
     <n v="0.38369999999999999"/>
     <s v="Playing At:  Boston Bruins   Home"/>
     <x v="2"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -5403,7 +5422,7 @@
     <n v="0.42380000000000001"/>
     <s v="Playing At:  Vancouver Canucks   Home"/>
     <x v="3"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -5417,10 +5436,109 @@
     <n v="0"/>
   </r>
   <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Edmonton Oilers"/>
+    <x v="325"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.21060000000000001"/>
+    <s v="Playing At:  Edmonton Oilers   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Dallas Stars"/>
+    <x v="326"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.24840000000000001"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Boston Bruins"/>
+    <x v="327"/>
+    <s v="Ottawa Senators"/>
+    <n v="0.25219999999999998"/>
+    <s v="Playing At:  Ottawa Senators   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Calgary Flames"/>
+    <x v="328"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.28110000000000002"/>
+    <s v="Playing At:  Calgary Flames   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Tampa Bay Lightning"/>
+    <x v="284"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.31259999999999999"/>
+    <s v="Playing At:  Tampa Bay Lightning   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="New York Islanders"/>
+    <x v="329"/>
+    <s v="Montreal Canadiens"/>
+    <n v="0.35160000000000002"/>
+    <s v="Playing At:  Montreal Canadiens   Home"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Detroit Red Wings"/>
+    <x v="330"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.44550000000000001"/>
+    <s v="Playing At:  Detroit Red Wings   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="Minnesota Wild"/>
+    <x v="331"/>
+    <s v="Nashville Predators"/>
+    <n v="0.46310000000000001"/>
+    <s v="Playing At:  Minnesota Wild   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="44"/>
+    <s v="New Jersey Devils"/>
+    <x v="332"/>
+    <s v="Carolina Hurricanes"/>
+    <n v="0.47839999999999999"/>
+    <s v="Playing At:  Carolina Hurricanes   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="7"/>
-    <x v="44"/>
+    <x v="45"/>
     <m/>
-    <x v="325"/>
+    <x v="333"/>
     <m/>
     <m/>
     <m/>
@@ -5431,8 +5549,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O33" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O34" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="9">
@@ -5474,7 +5592,7 @@
     <field x="0"/>
     <field x="7"/>
   </rowFields>
-  <rowItems count="30">
+  <rowItems count="31">
     <i>
       <x v="1"/>
       <x v="3"/>
@@ -5561,6 +5679,9 @@
     </i>
     <i>
       <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
       <x v="5"/>
     </i>
     <i r="1">
@@ -5601,7 +5722,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -5618,7 +5739,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="46">
+      <items count="47">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -5658,27 +5779,20 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="44"/>
+        <item x="45"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
         <item x="42"/>
         <item x="43"/>
+        <item x="44"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="635">
-        <item x="325"/>
-        <item m="1" x="326"/>
-        <item m="1" x="327"/>
-        <item m="1" x="328"/>
-        <item m="1" x="329"/>
-        <item m="1" x="330"/>
-        <item m="1" x="331"/>
-        <item m="1" x="332"/>
-        <item m="1" x="333"/>
+      <items count="643">
+        <item x="333"/>
         <item m="1" x="334"/>
         <item m="1" x="335"/>
         <item m="1" x="336"/>
@@ -5973,14 +6087,22 @@
         <item m="1" x="625"/>
         <item m="1" x="626"/>
         <item m="1" x="627"/>
-        <item x="314"/>
         <item m="1" x="628"/>
         <item m="1" x="629"/>
         <item m="1" x="630"/>
         <item m="1" x="631"/>
         <item m="1" x="632"/>
+        <item m="1" x="633"/>
+        <item m="1" x="634"/>
+        <item m="1" x="635"/>
+        <item x="314"/>
+        <item m="1" x="636"/>
+        <item m="1" x="637"/>
+        <item m="1" x="638"/>
+        <item m="1" x="639"/>
+        <item m="1" x="640"/>
         <item x="9"/>
-        <item m="1" x="633"/>
+        <item m="1" x="641"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -6304,6 +6426,14 @@
         <item x="322"/>
         <item x="323"/>
         <item x="324"/>
+        <item x="325"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="330"/>
+        <item x="331"/>
+        <item x="332"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6687,24 +6817,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -6712,7 +6842,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6720,7 +6850,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -6743,17 +6873,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="L4" t="s">
         <v>86</v>
       </c>
       <c r="M4" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="16">
         <v>5</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="16">
         <v>5</v>
       </c>
       <c r="P4" s="4">
@@ -6761,7 +6891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -6789,10 +6919,10 @@
       <c r="M5" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="16">
         <v>7</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="16">
         <v>4</v>
       </c>
       <c r="P5" s="4">
@@ -6800,14 +6930,14 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="16">
         <v>4</v>
       </c>
       <c r="D6" s="4">
@@ -6816,15 +6946,15 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H6" s="9">
         <f>SUM(B6:B7)</f>
@@ -6833,10 +6963,10 @@
       <c r="M6" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="16">
         <v>2</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="16">
         <v>2</v>
       </c>
       <c r="P6" s="4">
@@ -6844,14 +6974,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="16">
         <v>11</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="16">
         <v>10</v>
       </c>
       <c r="D7" s="4">
@@ -6860,15 +6990,15 @@
       </c>
       <c r="E7" s="7">
         <f>SUM(C10:C12)</f>
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F7" s="5">
         <f>SUM(C6:C9)</f>
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H7" s="9">
         <f>SUM(C6:C7)</f>
@@ -6877,10 +7007,10 @@
       <c r="M7" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="15">
-        <v>1</v>
-      </c>
-      <c r="O7" s="15">
+      <c r="N7" s="16">
+        <v>1</v>
+      </c>
+      <c r="O7" s="16">
         <v>1</v>
       </c>
       <c r="P7" s="4">
@@ -6888,31 +7018,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="15">
-        <v>37</v>
-      </c>
-      <c r="C8" s="15">
-        <v>22</v>
+      <c r="B8" s="16">
+        <v>39</v>
+      </c>
+      <c r="C8" s="16">
+        <v>24</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>0.59459459459459463</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.56275303643724695</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.68131868131868134</v>
+        <v>0.69473684210526321</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
-        <v>0.69230769230769229</v>
+        <v>0.70370370370370372</v>
       </c>
       <c r="H8" s="10">
         <f>H7/H6</f>
@@ -6921,10 +7051,10 @@
       <c r="L8" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="16">
         <v>15</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="16">
         <v>12</v>
       </c>
       <c r="P8" s="4">
@@ -6932,19 +7062,31 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="15">
-        <v>39</v>
-      </c>
-      <c r="C9" s="15">
-        <v>26</v>
+      <c r="B9" s="16">
+        <v>41</v>
+      </c>
+      <c r="C9" s="16">
+        <v>28</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.68292682926829273</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="L9" t="s">
         <v>87</v>
@@ -6952,10 +7094,10 @@
       <c r="M9" t="s">
         <v>94</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="16">
         <v>8</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="16">
         <v>5</v>
       </c>
       <c r="P9" s="4">
@@ -6963,27 +7105,43 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="15">
-        <v>107</v>
-      </c>
-      <c r="C10" s="15">
-        <v>63</v>
+      <c r="B10" s="16">
+        <v>109</v>
+      </c>
+      <c r="C10" s="16">
+        <v>64</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>0.58878504672897192</v>
+        <v>0.58715596330275233</v>
+      </c>
+      <c r="E10" s="8">
+        <f>E6/$B$13</f>
+        <v>0.72622478386167144</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" ref="F10:H10" si="2">F6/$B$13</f>
+        <v>0.2737752161383285</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.15561959654178675</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="2"/>
+        <v>4.3227665706051875E-2</v>
       </c>
       <c r="M10" t="s">
         <v>93</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="16">
         <v>6</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="16">
         <v>1</v>
       </c>
       <c r="P10" s="4">
@@ -6991,27 +7149,27 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="15">
-        <v>71</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="16">
+        <v>72</v>
+      </c>
+      <c r="C11" s="16">
         <v>38</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0.53521126760563376</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="M11" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="15">
-        <v>1</v>
-      </c>
-      <c r="O11" s="15">
+      <c r="N11" s="16">
+        <v>1</v>
+      </c>
+      <c r="O11" s="16">
         <v>1</v>
       </c>
       <c r="P11" s="4">
@@ -7019,27 +7177,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="15">
-        <v>69</v>
-      </c>
-      <c r="C12" s="15">
+      <c r="B12" s="16">
+        <v>71</v>
+      </c>
+      <c r="C12" s="16">
         <v>38</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="1"/>
-        <v>0.55072463768115942</v>
+        <v>0.53521126760563376</v>
       </c>
       <c r="L12" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="16">
         <v>15</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="16">
         <v>7</v>
       </c>
       <c r="P12" s="4">
@@ -7047,19 +7205,19 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="15">
-        <v>338</v>
-      </c>
-      <c r="C13" s="15">
-        <v>201</v>
+      <c r="B13" s="16">
+        <v>347</v>
+      </c>
+      <c r="C13" s="16">
+        <v>206</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0.59467455621301779</v>
+        <v>0.59365994236311237</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
@@ -7067,10 +7225,10 @@
       <c r="M13" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="16">
         <v>3</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="16">
         <v>2</v>
       </c>
       <c r="P13" s="4">
@@ -7078,14 +7236,14 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M14" t="s">
         <v>93</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="16">
         <v>7</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O14" s="16">
         <v>4</v>
       </c>
       <c r="P14" s="4">
@@ -7093,14 +7251,14 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M15" t="s">
         <v>50</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="16">
         <v>2</v>
       </c>
-      <c r="O15" s="15">
+      <c r="O15" s="16">
         <v>2</v>
       </c>
       <c r="P15" s="4">
@@ -7108,14 +7266,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="L16" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="16">
         <v>12</v>
       </c>
-      <c r="O16" s="15">
+      <c r="O16" s="16">
         <v>8</v>
       </c>
       <c r="P16" s="4">
@@ -7123,17 +7281,17 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L17" t="s">
         <v>89</v>
       </c>
       <c r="M17" t="s">
         <v>94</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="16">
         <v>9</v>
       </c>
-      <c r="O17" s="15">
+      <c r="O17" s="16">
         <v>5</v>
       </c>
       <c r="P17" s="4">
@@ -7141,14 +7299,14 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M18" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="16">
         <v>4</v>
       </c>
-      <c r="O18" s="15">
+      <c r="O18" s="16">
         <v>4</v>
       </c>
       <c r="P18" s="4">
@@ -7156,14 +7314,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M19" t="s">
         <v>50</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="16">
         <v>3</v>
       </c>
-      <c r="O19" s="15">
+      <c r="O19" s="16">
         <v>3</v>
       </c>
       <c r="P19" s="4">
@@ -7171,14 +7329,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M20" t="s">
         <v>61</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="16">
         <v>2</v>
       </c>
-      <c r="O20" s="15">
+      <c r="O20" s="16">
         <v>2</v>
       </c>
       <c r="P20" s="4">
@@ -7186,14 +7344,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L21" t="s">
         <v>103</v>
       </c>
-      <c r="N21" s="15">
+      <c r="N21" s="16">
         <v>18</v>
       </c>
-      <c r="O21" s="15">
+      <c r="O21" s="16">
         <v>14</v>
       </c>
       <c r="P21" s="4">
@@ -7201,17 +7359,17 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L22" t="s">
         <v>91</v>
       </c>
       <c r="M22" t="s">
         <v>94</v>
       </c>
-      <c r="N22" s="15">
+      <c r="N22" s="16">
         <v>6</v>
       </c>
-      <c r="O22" s="15">
+      <c r="O22" s="16">
         <v>3</v>
       </c>
       <c r="P22" s="4">
@@ -7219,14 +7377,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M23" t="s">
         <v>93</v>
       </c>
-      <c r="N23" s="15">
+      <c r="N23" s="16">
         <v>6</v>
       </c>
-      <c r="O23" s="15">
+      <c r="O23" s="16">
         <v>5</v>
       </c>
       <c r="P23" s="4">
@@ -7234,14 +7392,14 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="24" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M24" t="s">
         <v>50</v>
       </c>
-      <c r="N24" s="15">
-        <v>1</v>
-      </c>
-      <c r="O24" s="15">
+      <c r="N24" s="16">
+        <v>1</v>
+      </c>
+      <c r="O24" s="16">
         <v>1</v>
       </c>
       <c r="P24" s="4">
@@ -7249,14 +7407,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L25" t="s">
         <v>104</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="16">
         <v>13</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="16">
         <v>9</v>
       </c>
       <c r="P25" s="4">
@@ -7264,17 +7422,17 @@
         <v>0.69230769230769229</v>
       </c>
     </row>
-    <row r="26" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L26" t="s">
         <v>90</v>
       </c>
       <c r="M26" t="s">
         <v>94</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N26" s="16">
         <v>8</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="16">
         <v>6</v>
       </c>
       <c r="P26" s="4">
@@ -7282,14 +7440,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M27" t="s">
         <v>93</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="16">
         <v>3</v>
       </c>
-      <c r="O27" s="15">
+      <c r="O27" s="16">
         <v>1</v>
       </c>
       <c r="P27" s="4">
@@ -7297,14 +7455,14 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="28" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M28" t="s">
         <v>61</v>
       </c>
-      <c r="N28" s="15">
-        <v>1</v>
-      </c>
-      <c r="O28" s="15">
+      <c r="N28" s="16">
+        <v>1</v>
+      </c>
+      <c r="O28" s="16">
         <v>1</v>
       </c>
       <c r="P28" s="4">
@@ -7312,14 +7470,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L29" t="s">
         <v>105</v>
       </c>
-      <c r="N29" s="15">
+      <c r="N29" s="16">
         <v>12</v>
       </c>
-      <c r="O29" s="15">
+      <c r="O29" s="16">
         <v>8</v>
       </c>
       <c r="P29" s="4">
@@ -7327,124 +7485,133 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="30" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L30" t="s">
         <v>99</v>
       </c>
       <c r="M30" t="s">
-        <v>93</v>
-      </c>
-      <c r="N30" s="15">
-        <v>4</v>
-      </c>
-      <c r="O30" s="15">
-        <v>3</v>
+        <v>94</v>
+      </c>
+      <c r="N30" s="16">
+        <v>2</v>
+      </c>
+      <c r="O30" s="16">
+        <v>2</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="31" spans="12:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M31" t="s">
-        <v>50</v>
-      </c>
-      <c r="N31" s="15">
-        <v>2</v>
-      </c>
-      <c r="O31" s="15">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="N31" s="16">
+        <v>6</v>
+      </c>
+      <c r="O31" s="16">
+        <v>5</v>
       </c>
       <c r="P31" s="4">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L32" t="s">
-        <v>106</v>
-      </c>
-      <c r="N32" s="15">
-        <v>6</v>
-      </c>
-      <c r="O32" s="15">
-        <v>4</v>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="32" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="M32" t="s">
+        <v>50</v>
+      </c>
+      <c r="N32" s="16">
+        <v>2</v>
+      </c>
+      <c r="O32" s="16">
+        <v>1</v>
       </c>
       <c r="P32" s="4">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="33" spans="12:16" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L33" t="s">
+        <v>106</v>
+      </c>
+      <c r="N33" s="16">
+        <v>10</v>
+      </c>
+      <c r="O33" s="16">
+        <v>8</v>
+      </c>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L34" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="15">
-        <v>91</v>
-      </c>
-      <c r="O33" s="15">
-        <v>62</v>
-      </c>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="N34" s="16">
+        <v>95</v>
+      </c>
+      <c r="O34" s="16">
+        <v>66</v>
+      </c>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P49" s="4"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P53" s="4"/>
     </row>
   </sheetData>
@@ -7515,27 +7682,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I339"/>
+  <dimension ref="A1:I348"/>
   <sheetViews>
-    <sheetView topLeftCell="A278" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I333" sqref="I333:I339"/>
+    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I344" sqref="I344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -7564,7 +7731,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -7593,7 +7760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -7622,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -7651,7 +7818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -7680,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -7709,7 +7876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -7738,7 +7905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -7767,7 +7934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -7796,7 +7963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -7825,7 +7992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -7854,7 +8021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -7883,7 +8050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -7912,7 +8079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -7941,7 +8108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -7970,7 +8137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -7999,7 +8166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -8028,7 +8195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -8057,7 +8224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -8086,7 +8253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -8115,7 +8282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -8144,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -8173,7 +8340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -8202,7 +8369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -8231,7 +8398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -8260,7 +8427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -8289,7 +8456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -8318,7 +8485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -8347,7 +8514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -8376,7 +8543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -8405,7 +8572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -8434,7 +8601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -8463,7 +8630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -8492,7 +8659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -8521,7 +8688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -8550,7 +8717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -8579,7 +8746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -8608,7 +8775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -8637,7 +8804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -8666,7 +8833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -8695,7 +8862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -8724,7 +8891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -8753,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -8782,7 +8949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -8811,7 +8978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -8840,7 +9007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -8869,7 +9036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -8898,7 +9065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -8927,7 +9094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -8956,7 +9123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -8985,7 +9152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -9014,7 +9181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -9043,7 +9210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -9072,7 +9239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -9101,7 +9268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -9130,7 +9297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -9159,7 +9326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -9188,7 +9355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -9217,7 +9384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -9246,7 +9413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -9275,7 +9442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -9304,7 +9471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -9333,7 +9500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -9362,7 +9529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -9391,7 +9558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -9420,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -9449,7 +9616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -9478,7 +9645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -9507,7 +9674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -9536,7 +9703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -9565,7 +9732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -9594,7 +9761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -9623,7 +9790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -9652,7 +9819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -9681,7 +9848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -9710,7 +9877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -9739,7 +9906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -9768,7 +9935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -9797,7 +9964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -9826,7 +9993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -9855,7 +10022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -9884,7 +10051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -9913,7 +10080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -9942,7 +10109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -9971,7 +10138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -10000,7 +10167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -10029,7 +10196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -10058,7 +10225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -10087,7 +10254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -10116,7 +10283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -10145,7 +10312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -10174,7 +10341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -10203,7 +10370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -10232,7 +10399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>87</v>
       </c>
@@ -10261,7 +10428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -10290,7 +10457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -10319,7 +10486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>87</v>
       </c>
@@ -10348,7 +10515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>87</v>
       </c>
@@ -10377,7 +10544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -10406,7 +10573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -10435,7 +10602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>87</v>
       </c>
@@ -10464,7 +10631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>87</v>
       </c>
@@ -10493,7 +10660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>87</v>
       </c>
@@ -10522,7 +10689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>87</v>
       </c>
@@ -10551,7 +10718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>87</v>
       </c>
@@ -10580,7 +10747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>87</v>
       </c>
@@ -10609,7 +10776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>87</v>
       </c>
@@ -10638,7 +10805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>87</v>
       </c>
@@ -10667,7 +10834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>87</v>
       </c>
@@ -10696,7 +10863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>87</v>
       </c>
@@ -10725,7 +10892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>87</v>
       </c>
@@ -10754,7 +10921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>87</v>
       </c>
@@ -10783,7 +10950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>87</v>
       </c>
@@ -10812,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>87</v>
       </c>
@@ -10841,7 +11008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>87</v>
       </c>
@@ -10870,7 +11037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>87</v>
       </c>
@@ -10899,7 +11066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>87</v>
       </c>
@@ -10928,7 +11095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>87</v>
       </c>
@@ -10957,7 +11124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>87</v>
       </c>
@@ -10986,7 +11153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>87</v>
       </c>
@@ -11015,7 +11182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>87</v>
       </c>
@@ -11044,7 +11211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>88</v>
       </c>
@@ -11073,7 +11240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -11102,7 +11269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>88</v>
       </c>
@@ -11131,7 +11298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>88</v>
       </c>
@@ -11160,7 +11327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>88</v>
       </c>
@@ -11189,7 +11356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>88</v>
       </c>
@@ -11218,7 +11385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>88</v>
       </c>
@@ -11247,7 +11414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>88</v>
       </c>
@@ -11276,7 +11443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>88</v>
       </c>
@@ -11305,7 +11472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>88</v>
       </c>
@@ -11334,7 +11501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>88</v>
       </c>
@@ -11363,7 +11530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>88</v>
       </c>
@@ -11392,7 +11559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>88</v>
       </c>
@@ -11421,7 +11588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>88</v>
       </c>
@@ -11450,7 +11617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>88</v>
       </c>
@@ -11479,7 +11646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>88</v>
       </c>
@@ -11508,7 +11675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>88</v>
       </c>
@@ -11537,7 +11704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>88</v>
       </c>
@@ -11566,7 +11733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>88</v>
       </c>
@@ -11595,7 +11762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>88</v>
       </c>
@@ -11624,7 +11791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>88</v>
       </c>
@@ -11653,7 +11820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>88</v>
       </c>
@@ -11682,7 +11849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>88</v>
       </c>
@@ -11711,7 +11878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>88</v>
       </c>
@@ -11740,7 +11907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>88</v>
       </c>
@@ -11769,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>88</v>
       </c>
@@ -11798,7 +11965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>88</v>
       </c>
@@ -11827,7 +11994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>88</v>
       </c>
@@ -11856,7 +12023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>88</v>
       </c>
@@ -11885,7 +12052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -11914,7 +12081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>88</v>
       </c>
@@ -11943,7 +12110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>88</v>
       </c>
@@ -11972,7 +12139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>88</v>
       </c>
@@ -12001,7 +12168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>88</v>
       </c>
@@ -12030,7 +12197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>88</v>
       </c>
@@ -12059,7 +12226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>88</v>
       </c>
@@ -12088,7 +12255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>89</v>
       </c>
@@ -12117,7 +12284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>89</v>
       </c>
@@ -12146,7 +12313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>89</v>
       </c>
@@ -12175,7 +12342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>89</v>
       </c>
@@ -12204,7 +12371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -12233,7 +12400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>89</v>
       </c>
@@ -12262,7 +12429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>89</v>
       </c>
@@ -12291,7 +12458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>89</v>
       </c>
@@ -12320,7 +12487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>89</v>
       </c>
@@ -12349,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>89</v>
       </c>
@@ -12378,7 +12545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>89</v>
       </c>
@@ -12407,7 +12574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>89</v>
       </c>
@@ -12436,7 +12603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>89</v>
       </c>
@@ -12465,7 +12632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>89</v>
       </c>
@@ -12494,7 +12661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>89</v>
       </c>
@@ -12523,7 +12690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>89</v>
       </c>
@@ -12552,7 +12719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>89</v>
       </c>
@@ -12581,7 +12748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>89</v>
       </c>
@@ -12610,7 +12777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>89</v>
       </c>
@@ -12639,7 +12806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>89</v>
       </c>
@@ -12668,7 +12835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>89</v>
       </c>
@@ -12697,7 +12864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>89</v>
       </c>
@@ -12726,7 +12893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>89</v>
       </c>
@@ -12755,7 +12922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>89</v>
       </c>
@@ -12784,7 +12951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>89</v>
       </c>
@@ -12813,7 +12980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>89</v>
       </c>
@@ -12842,7 +13009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>89</v>
       </c>
@@ -12871,7 +13038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>89</v>
       </c>
@@ -12900,7 +13067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>89</v>
       </c>
@@ -12929,7 +13096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>89</v>
       </c>
@@ -12958,7 +13125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>89</v>
       </c>
@@ -12987,7 +13154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>89</v>
       </c>
@@ -13016,7 +13183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>89</v>
       </c>
@@ -13045,7 +13212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>89</v>
       </c>
@@ -13074,7 +13241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>89</v>
       </c>
@@ -13103,7 +13270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>89</v>
       </c>
@@ -13132,7 +13299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>89</v>
       </c>
@@ -13161,7 +13328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>89</v>
       </c>
@@ -13190,7 +13357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>89</v>
       </c>
@@ -13219,7 +13386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>89</v>
       </c>
@@ -13248,7 +13415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>89</v>
       </c>
@@ -13277,7 +13444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>89</v>
       </c>
@@ -13306,7 +13473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>89</v>
       </c>
@@ -13335,7 +13502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>89</v>
       </c>
@@ -13364,7 +13531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>89</v>
       </c>
@@ -13393,7 +13560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>89</v>
       </c>
@@ -13422,7 +13589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>89</v>
       </c>
@@ -13451,7 +13618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>89</v>
       </c>
@@ -13480,7 +13647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>89</v>
       </c>
@@ -13509,7 +13676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>89</v>
       </c>
@@ -13538,7 +13705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>89</v>
       </c>
@@ -13567,7 +13734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>89</v>
       </c>
@@ -13596,7 +13763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>89</v>
       </c>
@@ -13625,7 +13792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>89</v>
       </c>
@@ -13654,7 +13821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>89</v>
       </c>
@@ -13683,7 +13850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>89</v>
       </c>
@@ -13712,7 +13879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>89</v>
       </c>
@@ -13741,7 +13908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>91</v>
       </c>
@@ -13770,7 +13937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>91</v>
       </c>
@@ -13799,7 +13966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>91</v>
       </c>
@@ -13828,7 +13995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>91</v>
       </c>
@@ -13857,7 +14024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>91</v>
       </c>
@@ -13886,7 +14053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -13915,7 +14082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>91</v>
       </c>
@@ -13944,7 +14111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>91</v>
       </c>
@@ -13973,7 +14140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>91</v>
       </c>
@@ -14002,7 +14169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>91</v>
       </c>
@@ -14031,7 +14198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>91</v>
       </c>
@@ -14060,7 +14227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>91</v>
       </c>
@@ -14089,7 +14256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>91</v>
       </c>
@@ -14118,7 +14285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>91</v>
       </c>
@@ -14147,7 +14314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>91</v>
       </c>
@@ -14176,7 +14343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>91</v>
       </c>
@@ -14205,7 +14372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>91</v>
       </c>
@@ -14234,7 +14401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>91</v>
       </c>
@@ -14263,7 +14430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>91</v>
       </c>
@@ -14292,7 +14459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>91</v>
       </c>
@@ -14321,7 +14488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>91</v>
       </c>
@@ -14350,7 +14517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>91</v>
       </c>
@@ -14379,7 +14546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>91</v>
       </c>
@@ -14408,7 +14575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>91</v>
       </c>
@@ -14437,7 +14604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>91</v>
       </c>
@@ -14466,7 +14633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>91</v>
       </c>
@@ -14495,7 +14662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>91</v>
       </c>
@@ -14524,7 +14691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>91</v>
       </c>
@@ -14553,7 +14720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>91</v>
       </c>
@@ -14582,7 +14749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>91</v>
       </c>
@@ -14611,7 +14778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>91</v>
       </c>
@@ -14640,7 +14807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>91</v>
       </c>
@@ -14669,7 +14836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>91</v>
       </c>
@@ -14698,7 +14865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>91</v>
       </c>
@@ -14727,7 +14894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>91</v>
       </c>
@@ -14756,7 +14923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>91</v>
       </c>
@@ -14785,7 +14952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>91</v>
       </c>
@@ -14814,7 +14981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>91</v>
       </c>
@@ -14843,7 +15010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>91</v>
       </c>
@@ -14872,7 +15039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>91</v>
       </c>
@@ -14901,7 +15068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>91</v>
       </c>
@@ -14930,7 +15097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>91</v>
       </c>
@@ -14959,7 +15126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>91</v>
       </c>
@@ -14988,7 +15155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>91</v>
       </c>
@@ -15017,7 +15184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>91</v>
       </c>
@@ -15046,7 +15213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>91</v>
       </c>
@@ -15075,7 +15242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>91</v>
       </c>
@@ -15104,7 +15271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>91</v>
       </c>
@@ -15133,7 +15300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>90</v>
       </c>
@@ -15162,7 +15329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>90</v>
       </c>
@@ -15191,7 +15358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>90</v>
       </c>
@@ -15220,7 +15387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>90</v>
       </c>
@@ -15249,7 +15416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>90</v>
       </c>
@@ -15278,7 +15445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>90</v>
       </c>
@@ -15307,7 +15474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>90</v>
       </c>
@@ -15336,7 +15503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>90</v>
       </c>
@@ -15365,7 +15532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>90</v>
       </c>
@@ -15394,7 +15561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>90</v>
       </c>
@@ -15423,7 +15590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>90</v>
       </c>
@@ -15452,7 +15619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>90</v>
       </c>
@@ -15481,7 +15648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>90</v>
       </c>
@@ -15510,7 +15677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>90</v>
       </c>
@@ -15539,7 +15706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>90</v>
       </c>
@@ -15568,7 +15735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>90</v>
       </c>
@@ -15597,7 +15764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>90</v>
       </c>
@@ -15626,7 +15793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>90</v>
       </c>
@@ -15655,7 +15822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>90</v>
       </c>
@@ -15684,7 +15851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>90</v>
       </c>
@@ -15713,7 +15880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>90</v>
       </c>
@@ -15742,7 +15909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>90</v>
       </c>
@@ -15771,7 +15938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>90</v>
       </c>
@@ -15800,7 +15967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>90</v>
       </c>
@@ -15829,7 +15996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>90</v>
       </c>
@@ -15858,7 +16025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>90</v>
       </c>
@@ -15887,7 +16054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>90</v>
       </c>
@@ -15916,7 +16083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>90</v>
       </c>
@@ -15945,7 +16112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>90</v>
       </c>
@@ -15974,7 +16141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>90</v>
       </c>
@@ -16003,7 +16170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>90</v>
       </c>
@@ -16032,7 +16199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>90</v>
       </c>
@@ -16061,7 +16228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>90</v>
       </c>
@@ -16090,7 +16257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>90</v>
       </c>
@@ -16119,7 +16286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>90</v>
       </c>
@@ -16148,7 +16315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>90</v>
       </c>
@@ -16177,7 +16344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>90</v>
       </c>
@@ -16206,7 +16373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>90</v>
       </c>
@@ -16235,7 +16402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>90</v>
       </c>
@@ -16264,7 +16431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>90</v>
       </c>
@@ -16293,7 +16460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>90</v>
       </c>
@@ -16322,7 +16489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>90</v>
       </c>
@@ -16351,7 +16518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>90</v>
       </c>
@@ -16380,7 +16547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>90</v>
       </c>
@@ -16409,7 +16576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>90</v>
       </c>
@@ -16438,7 +16605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>90</v>
       </c>
@@ -16467,7 +16634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>90</v>
       </c>
@@ -16496,7 +16663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>90</v>
       </c>
@@ -16525,7 +16692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>90</v>
       </c>
@@ -16554,7 +16721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>99</v>
       </c>
@@ -16583,7 +16750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>99</v>
       </c>
@@ -16612,7 +16779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>99</v>
       </c>
@@ -16641,7 +16808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>99</v>
       </c>
@@ -16670,7 +16837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>99</v>
       </c>
@@ -16699,7 +16866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>99</v>
       </c>
@@ -16728,7 +16895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>99</v>
       </c>
@@ -16757,7 +16924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>99</v>
       </c>
@@ -16786,7 +16953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>99</v>
       </c>
@@ -16815,7 +16982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>99</v>
       </c>
@@ -16844,7 +17011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>99</v>
       </c>
@@ -16873,7 +17040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>99</v>
       </c>
@@ -16902,7 +17069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>99</v>
       </c>
@@ -16931,7 +17098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>99</v>
       </c>
@@ -16960,7 +17127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>99</v>
       </c>
@@ -16989,7 +17156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>99</v>
       </c>
@@ -17018,7 +17185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>99</v>
       </c>
@@ -17047,7 +17214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>99</v>
       </c>
@@ -17076,7 +17243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>99</v>
       </c>
@@ -17105,7 +17272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>99</v>
       </c>
@@ -17134,7 +17301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>99</v>
       </c>
@@ -17163,7 +17330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>99</v>
       </c>
@@ -17192,7 +17359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>99</v>
       </c>
@@ -17218,10 +17385,10 @@
         <v>51</v>
       </c>
       <c r="I334">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>99</v>
       </c>
@@ -17250,7 +17417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>99</v>
       </c>
@@ -17276,10 +17443,10 @@
         <v>51</v>
       </c>
       <c r="I336">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>99</v>
       </c>
@@ -17308,7 +17475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>99</v>
       </c>
@@ -17334,10 +17501,10 @@
         <v>84</v>
       </c>
       <c r="I338">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>99</v>
       </c>
@@ -17363,6 +17530,267 @@
         <v>85</v>
       </c>
       <c r="I339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>99</v>
+      </c>
+      <c r="B340" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C340" t="s">
+        <v>10</v>
+      </c>
+      <c r="D340" s="14">
+        <v>0.78939999999999999</v>
+      </c>
+      <c r="E340" t="s">
+        <v>14</v>
+      </c>
+      <c r="F340" s="14">
+        <v>0.21060000000000001</v>
+      </c>
+      <c r="G340" t="s">
+        <v>12</v>
+      </c>
+      <c r="H340" t="s">
+        <v>93</v>
+      </c>
+      <c r="I340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>99</v>
+      </c>
+      <c r="B341" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C341" t="s">
+        <v>28</v>
+      </c>
+      <c r="D341" s="14">
+        <v>0.75160000000000005</v>
+      </c>
+      <c r="E341" t="s">
+        <v>17</v>
+      </c>
+      <c r="F341" s="14">
+        <v>0.24840000000000001</v>
+      </c>
+      <c r="G341" t="s">
+        <v>30</v>
+      </c>
+      <c r="H341" t="s">
+        <v>93</v>
+      </c>
+      <c r="I341" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>99</v>
+      </c>
+      <c r="B342" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C342" t="s">
+        <v>4</v>
+      </c>
+      <c r="D342" s="14">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="E342" t="s">
+        <v>36</v>
+      </c>
+      <c r="F342" s="14">
+        <v>0.25219999999999998</v>
+      </c>
+      <c r="G342" t="s">
+        <v>64</v>
+      </c>
+      <c r="H342" t="s">
+        <v>94</v>
+      </c>
+      <c r="I342" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>99</v>
+      </c>
+      <c r="B343" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C343" t="s">
+        <v>31</v>
+      </c>
+      <c r="D343" s="14">
+        <v>0.71889999999999998</v>
+      </c>
+      <c r="E343" t="s">
+        <v>34</v>
+      </c>
+      <c r="F343" s="14">
+        <v>0.28110000000000002</v>
+      </c>
+      <c r="G343" t="s">
+        <v>32</v>
+      </c>
+      <c r="H343" t="s">
+        <v>94</v>
+      </c>
+      <c r="I343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>99</v>
+      </c>
+      <c r="B344" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C344" t="s">
+        <v>22</v>
+      </c>
+      <c r="D344" s="14">
+        <v>0.68740000000000001</v>
+      </c>
+      <c r="E344" t="s">
+        <v>5</v>
+      </c>
+      <c r="F344" s="14">
+        <v>0.31259999999999999</v>
+      </c>
+      <c r="G344" t="s">
+        <v>77</v>
+      </c>
+      <c r="H344" t="s">
+        <v>51</v>
+      </c>
+      <c r="I344" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>99</v>
+      </c>
+      <c r="B345" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C345" t="s">
+        <v>39</v>
+      </c>
+      <c r="D345" s="14">
+        <v>0.64839999999999998</v>
+      </c>
+      <c r="E345" t="s">
+        <v>45</v>
+      </c>
+      <c r="F345" s="14">
+        <v>0.35160000000000002</v>
+      </c>
+      <c r="G345" t="s">
+        <v>59</v>
+      </c>
+      <c r="H345" t="s">
+        <v>51</v>
+      </c>
+      <c r="I345" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>99</v>
+      </c>
+      <c r="B346" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C346" t="s">
+        <v>37</v>
+      </c>
+      <c r="D346" s="14">
+        <v>0.55449999999999999</v>
+      </c>
+      <c r="E346" t="s">
+        <v>8</v>
+      </c>
+      <c r="F346" s="14">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="G346" t="s">
+        <v>38</v>
+      </c>
+      <c r="H346" t="s">
+        <v>84</v>
+      </c>
+      <c r="I346" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>99</v>
+      </c>
+      <c r="B347" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C347" t="s">
+        <v>58</v>
+      </c>
+      <c r="D347" s="14">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="E347" t="s">
+        <v>20</v>
+      </c>
+      <c r="F347" s="14">
+        <v>0.46310000000000001</v>
+      </c>
+      <c r="G347" t="s">
+        <v>72</v>
+      </c>
+      <c r="H347" t="s">
+        <v>85</v>
+      </c>
+      <c r="I347" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>99</v>
+      </c>
+      <c r="B348" s="1">
+        <v>45316</v>
+      </c>
+      <c r="C348" t="s">
+        <v>11</v>
+      </c>
+      <c r="D348" s="14">
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="E348" t="s">
+        <v>43</v>
+      </c>
+      <c r="F348" s="14">
+        <v>0.47839999999999999</v>
+      </c>
+      <c r="G348" t="s">
+        <v>74</v>
+      </c>
+      <c r="H348" t="s">
+        <v>85</v>
+      </c>
+      <c r="I348" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
retrained model, updated predictions
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1215CCB4-BE6E-4F51-8C51-3F81BB560699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D4D554-21A4-4F90-8306-82ED3810D9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="28" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>% Of Predictions</t>
+  </si>
+  <si>
+    <t>PDA8</t>
+  </si>
+  <si>
+    <t>PDA8 Total</t>
   </si>
 </sst>
 </file>
@@ -878,7 +884,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -897,6 +903,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -957,13 +964,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45318.336384259259" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="366" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45319.363471990742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="368" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Model Used" numFmtId="0">
-      <sharedItems containsBlank="1" count="8">
+      <sharedItems containsBlank="1" count="9">
         <s v="PDA1"/>
         <s v="PDA2"/>
         <s v="PDA3"/>
@@ -971,11 +978,12 @@
         <s v="PDA5"/>
         <s v="PDA6"/>
         <s v="PDA7"/>
+        <s v="PDA8"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-28T00:00:00" count="48">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-29T00:00:00" count="49">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1023,6 +1031,7 @@
         <d v="2024-01-25T00:00:00"/>
         <d v="2024-01-26T00:00:00"/>
         <d v="2024-01-27T00:00:00"/>
+        <d v="2024-01-28T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1030,7 +1039,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="658">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="660">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1380,6 +1389,8 @@
         <n v="0.5887"/>
         <n v="0.51970000000000005"/>
         <n v="0.50490000000000002"/>
+        <n v="0.75"/>
+        <n v="0.56999999999999995"/>
         <m/>
         <n v="0.87610539305886403" u="1"/>
         <n v="0.78056782297496197" u="1"/>
@@ -1727,7 +1738,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="366">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="368">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -5620,7 +5631,7 @@
     <n v="0.25559999999999999"/>
     <s v="Playing At:  Minnesota Wild   Home"/>
     <x v="6"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -5708,7 +5719,7 @@
     <n v="0.4113"/>
     <s v="Playing At:  Detroit Red Wings   Home"/>
     <x v="3"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -5746,8 +5757,30 @@
   <r>
     <x v="7"/>
     <x v="47"/>
+    <s v="Seattle Kraken"/>
+    <x v="349"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.25"/>
+    <s v="Playing At:  Seattle Kraken   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="47"/>
+    <s v="Los Angeles Kings"/>
+    <x v="350"/>
+    <s v="St. Louis Blues"/>
+    <n v="0.43"/>
+    <s v="Playing At:  St. Louis Blues   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="48"/>
     <m/>
-    <x v="349"/>
+    <x v="351"/>
     <m/>
     <m/>
     <m/>
@@ -5758,12 +5791,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O36" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="10">
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item x="7"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="8"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -5771,11 +5804,193 @@
         <item x="4"/>
         <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="33">
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="10">
+        <item x="8"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="49">
+      <items count="50">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -5815,7 +6030,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="47"/>
+        <item x="48"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -5824,15 +6039,14 @@
         <item x="44"/>
         <item x="45"/>
         <item x="46"/>
+        <item x="47"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="659">
-        <item x="349"/>
-        <item m="1" x="350"/>
-        <item m="1" x="351"/>
+      <items count="661">
+        <item x="351"/>
         <item m="1" x="352"/>
         <item m="1" x="353"/>
         <item m="1" x="354"/>
@@ -6133,14 +6347,16 @@
         <item m="1" x="649"/>
         <item m="1" x="650"/>
         <item m="1" x="651"/>
-        <item x="314"/>
         <item m="1" x="652"/>
         <item m="1" x="653"/>
+        <item x="314"/>
         <item m="1" x="654"/>
         <item m="1" x="655"/>
         <item m="1" x="656"/>
+        <item m="1" x="657"/>
+        <item m="1" x="658"/>
         <item x="9"/>
-        <item m="1" x="657"/>
+        <item m="1" x="659"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -6488,6 +6704,8 @@
         <item x="346"/>
         <item x="347"/>
         <item x="348"/>
+        <item x="349"/>
+        <item x="350"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6556,179 +6774,6 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O34" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="9">
-        <item h="1" x="7"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="2"/>
-        <item x="6"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="31">
-    <i>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
@@ -7045,7 +7090,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7153,7 +7198,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" ref="P5:P33" si="0">O5/N5</f>
+        <f t="shared" ref="P5:P35" si="0">O5/N5</f>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -7173,15 +7218,15 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H6" s="9">
         <f>SUM(B6:B7)</f>
@@ -7225,7 +7270,7 @@
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" s="9">
         <f>SUM(C6:C7)</f>
@@ -7250,26 +7295,26 @@
         <v>93</v>
       </c>
       <c r="B8" s="15">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="15">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>0.63414634146341464</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.55849056603773584</v>
+        <v>0.55639097744360899</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.7</v>
+        <v>0.69306930693069302</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
-        <v>0.7142857142857143</v>
+        <v>0.7192982456140351</v>
       </c>
       <c r="H8" s="10">
         <f>H7/H6</f>
@@ -7297,11 +7342,11 @@
         <v>44</v>
       </c>
       <c r="C9" s="15">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>0.68181818181818177</v>
+        <v>0.65909090909090906</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>107</v>
@@ -7348,19 +7393,19 @@
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.72602739726027399</v>
+        <v>0.72479564032697552</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" ref="F10:H10" si="2">F6/$B$13</f>
-        <v>0.27397260273972601</v>
+        <v>0.27520435967302453</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" si="2"/>
-        <v>0.15342465753424658</v>
+        <v>0.15531335149863759</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>4.1095890410958902E-2</v>
+        <v>4.0871934604904632E-2</v>
       </c>
       <c r="M10" t="s">
         <v>93</v>
@@ -7381,14 +7426,14 @@
         <v>84</v>
       </c>
       <c r="B11" s="15">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C11" s="15">
         <v>41</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0.53246753246753242</v>
+        <v>0.52564102564102566</v>
       </c>
       <c r="M11" t="s">
         <v>50</v>
@@ -7437,14 +7482,14 @@
         <v>53</v>
       </c>
       <c r="B13" s="15">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C13" s="15">
         <v>218</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0.59726027397260273</v>
+        <v>0.59400544959128065</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
@@ -7723,11 +7768,11 @@
         <v>5</v>
       </c>
       <c r="O30" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="31" spans="12:16" x14ac:dyDescent="0.25">
@@ -7768,29 +7813,56 @@
         <v>15</v>
       </c>
       <c r="O33" s="15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P33" s="4">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="34" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L34" t="s">
+        <v>108</v>
+      </c>
+      <c r="M34" t="s">
+        <v>93</v>
+      </c>
+      <c r="N34" s="15">
+        <v>1</v>
+      </c>
+      <c r="O34" s="15">
+        <v>1</v>
+      </c>
+      <c r="P34" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>109</v>
+      </c>
+      <c r="N35" s="15">
+        <v>1</v>
+      </c>
+      <c r="O35" s="15">
+        <v>1</v>
+      </c>
+      <c r="P35" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
         <v>53</v>
       </c>
-      <c r="N34" s="15">
-        <v>100</v>
-      </c>
-      <c r="O34" s="15">
+      <c r="N36" s="15">
+        <v>101</v>
+      </c>
+      <c r="O36" s="15">
         <v>70</v>
       </c>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P36" s="4"/>
     </row>
     <row r="37" spans="12:16" x14ac:dyDescent="0.25">
@@ -7859,7 +7931,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P33">
+  <conditionalFormatting sqref="P4:P35">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -7902,7 +7974,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P4:P33</xm:sqref>
+          <xm:sqref>P4:P35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7912,10 +7984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I366"/>
+  <dimension ref="A1:I368"/>
   <sheetViews>
     <sheetView topLeftCell="A325" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I356" sqref="I356"/>
+      <selection activeCell="I369" sqref="I369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18169,7 +18241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>99</v>
       </c>
@@ -18224,7 +18296,7 @@
         <v>94</v>
       </c>
       <c r="I355">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.25">
@@ -18456,7 +18528,7 @@
         <v>84</v>
       </c>
       <c r="I363">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.25">
@@ -18543,6 +18615,64 @@
         <v>85</v>
       </c>
       <c r="I366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>108</v>
+      </c>
+      <c r="B367" s="1">
+        <v>45319</v>
+      </c>
+      <c r="C367" t="s">
+        <v>23</v>
+      </c>
+      <c r="D367" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="E367" t="s">
+        <v>34</v>
+      </c>
+      <c r="F367" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="G367" t="s">
+        <v>24</v>
+      </c>
+      <c r="H367" t="s">
+        <v>93</v>
+      </c>
+      <c r="I367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>108</v>
+      </c>
+      <c r="B368" s="1">
+        <v>45319</v>
+      </c>
+      <c r="C368" t="s">
+        <v>40</v>
+      </c>
+      <c r="D368" s="16">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E368" t="s">
+        <v>13</v>
+      </c>
+      <c r="F368" s="16">
+        <v>0.43</v>
+      </c>
+      <c r="G368" t="s">
+        <v>65</v>
+      </c>
+      <c r="H368" t="s">
+        <v>84</v>
+      </c>
+      <c r="I368">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated predictions, added in schedule analysis
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D4D554-21A4-4F90-8306-82ED3810D9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F805017-830D-4194-BC72-639F5417717A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="14" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -902,8 +902,8 @@
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -964,7 +964,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45319.363471990742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="368" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45320.325966203702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="369" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
@@ -983,7 +983,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-29T00:00:00" count="49">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-30T00:00:00" count="50">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1032,6 +1032,7 @@
         <d v="2024-01-26T00:00:00"/>
         <d v="2024-01-27T00:00:00"/>
         <d v="2024-01-28T00:00:00"/>
+        <d v="2024-01-29T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1039,7 +1040,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="660">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="661">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1391,6 +1392,7 @@
         <n v="0.50490000000000002"/>
         <n v="0.75"/>
         <n v="0.56999999999999995"/>
+        <n v="0.57999999999999996"/>
         <m/>
         <n v="0.87610539305886403" u="1"/>
         <n v="0.78056782297496197" u="1"/>
@@ -1738,7 +1740,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="368">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="369">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -5774,13 +5776,24 @@
     <n v="0.43"/>
     <s v="Playing At:  St. Louis Blues   Home"/>
     <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="48"/>
+    <s v="Nashville Predators"/>
+    <x v="351"/>
+    <s v="Ottawa Senators"/>
+    <n v="0.42"/>
+    <s v="Playing At:  Ottawa Senators   Home"/>
+    <x v="3"/>
     <n v="1"/>
   </r>
   <r>
     <x v="8"/>
-    <x v="48"/>
+    <x v="49"/>
     <m/>
-    <x v="351"/>
+    <x v="352"/>
     <m/>
     <m/>
     <m/>
@@ -5791,188 +5804,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O36" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="8"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="2"/>
-        <item x="6"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="33">
-    <i>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -5990,7 +5822,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="50">
+      <items count="51">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -6030,7 +5862,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="48"/>
+        <item x="49"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -6040,14 +5872,14 @@
         <item x="45"/>
         <item x="46"/>
         <item x="47"/>
+        <item x="48"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="661">
-        <item x="351"/>
-        <item m="1" x="352"/>
+      <items count="662">
+        <item x="352"/>
         <item m="1" x="353"/>
         <item m="1" x="354"/>
         <item m="1" x="355"/>
@@ -6349,14 +6181,15 @@
         <item m="1" x="651"/>
         <item m="1" x="652"/>
         <item m="1" x="653"/>
+        <item m="1" x="654"/>
         <item x="314"/>
-        <item m="1" x="654"/>
         <item m="1" x="655"/>
         <item m="1" x="656"/>
         <item m="1" x="657"/>
         <item m="1" x="658"/>
+        <item m="1" x="659"/>
         <item x="9"/>
-        <item m="1" x="659"/>
+        <item m="1" x="660"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -6706,6 +6539,7 @@
         <item x="348"/>
         <item x="349"/>
         <item x="350"/>
+        <item x="351"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6774,6 +6608,187 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O36" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="8"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="33">
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
@@ -7090,23 +7105,23 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -7114,7 +7129,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7122,7 +7137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -7145,17 +7160,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="L4" t="s">
         <v>86</v>
       </c>
       <c r="M4" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="16">
         <v>5</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="16">
         <v>5</v>
       </c>
       <c r="P4" s="4">
@@ -7163,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -7191,10 +7206,10 @@
       <c r="M5" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="16">
         <v>7</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="16">
         <v>4</v>
       </c>
       <c r="P5" s="4">
@@ -7202,14 +7217,14 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="16">
         <v>4</v>
       </c>
       <c r="D6" s="4">
@@ -7218,7 +7233,7 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
@@ -7235,10 +7250,10 @@
       <c r="M6" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="16">
         <v>2</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="16">
         <v>2</v>
       </c>
       <c r="P6" s="4">
@@ -7246,14 +7261,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="16">
         <v>11</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="16">
         <v>10</v>
       </c>
       <c r="D7" s="4">
@@ -7279,10 +7294,10 @@
       <c r="M7" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="15">
-        <v>1</v>
-      </c>
-      <c r="O7" s="15">
+      <c r="N7" s="16">
+        <v>1</v>
+      </c>
+      <c r="O7" s="16">
         <v>1</v>
       </c>
       <c r="P7" s="4">
@@ -7290,14 +7305,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="16">
         <v>42</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="16">
         <v>27</v>
       </c>
       <c r="D8" s="4">
@@ -7306,7 +7321,7 @@
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.55639097744360899</v>
+        <v>0.55430711610486894</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
@@ -7323,10 +7338,10 @@
       <c r="L8" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="16">
         <v>15</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="16">
         <v>12</v>
       </c>
       <c r="P8" s="4">
@@ -7334,14 +7349,14 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="16">
         <v>44</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="16">
         <v>29</v>
       </c>
       <c r="D9" s="4">
@@ -7366,10 +7381,10 @@
       <c r="M9" t="s">
         <v>94</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="16">
         <v>8</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="16">
         <v>5</v>
       </c>
       <c r="P9" s="4">
@@ -7377,14 +7392,14 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="16">
         <v>113</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="16">
         <v>67</v>
       </c>
       <c r="D10" s="4">
@@ -7393,27 +7408,27 @@
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.72479564032697552</v>
+        <v>0.72554347826086951</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" ref="F10:H10" si="2">F6/$B$13</f>
-        <v>0.27520435967302453</v>
+        <v>0.27445652173913043</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" si="2"/>
-        <v>0.15531335149863759</v>
+        <v>0.15489130434782608</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>4.0871934604904632E-2</v>
+        <v>4.0760869565217392E-2</v>
       </c>
       <c r="M10" t="s">
         <v>93</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="16">
         <v>6</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="16">
         <v>1</v>
       </c>
       <c r="P10" s="4">
@@ -7421,27 +7436,27 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="15">
-        <v>78</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="16">
+        <v>79</v>
+      </c>
+      <c r="C11" s="16">
         <v>41</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0.52564102564102566</v>
+        <v>0.51898734177215189</v>
       </c>
       <c r="M11" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="15">
-        <v>1</v>
-      </c>
-      <c r="O11" s="15">
+      <c r="N11" s="16">
+        <v>1</v>
+      </c>
+      <c r="O11" s="16">
         <v>1</v>
       </c>
       <c r="P11" s="4">
@@ -7449,14 +7464,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="16">
         <v>75</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="16">
         <v>40</v>
       </c>
       <c r="D12" s="4">
@@ -7466,10 +7481,10 @@
       <c r="L12" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="16">
         <v>15</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="16">
         <v>7</v>
       </c>
       <c r="P12" s="4">
@@ -7477,19 +7492,19 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="15">
-        <v>367</v>
-      </c>
-      <c r="C13" s="15">
+      <c r="B13" s="16">
+        <v>368</v>
+      </c>
+      <c r="C13" s="16">
         <v>218</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0.59400544959128065</v>
+        <v>0.59239130434782605</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
@@ -7497,10 +7512,10 @@
       <c r="M13" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="16">
         <v>3</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="16">
         <v>2</v>
       </c>
       <c r="P13" s="4">
@@ -7508,14 +7523,14 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M14" t="s">
         <v>93</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="16">
         <v>7</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O14" s="16">
         <v>4</v>
       </c>
       <c r="P14" s="4">
@@ -7523,14 +7538,14 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="M15" t="s">
         <v>50</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="16">
         <v>2</v>
       </c>
-      <c r="O15" s="15">
+      <c r="O15" s="16">
         <v>2</v>
       </c>
       <c r="P15" s="4">
@@ -7538,14 +7553,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="L16" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="16">
         <v>12</v>
       </c>
-      <c r="O16" s="15">
+      <c r="O16" s="16">
         <v>8</v>
       </c>
       <c r="P16" s="4">
@@ -7553,17 +7568,17 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L17" t="s">
         <v>89</v>
       </c>
       <c r="M17" t="s">
         <v>94</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="16">
         <v>9</v>
       </c>
-      <c r="O17" s="15">
+      <c r="O17" s="16">
         <v>5</v>
       </c>
       <c r="P17" s="4">
@@ -7571,14 +7586,14 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M18" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="16">
         <v>4</v>
       </c>
-      <c r="O18" s="15">
+      <c r="O18" s="16">
         <v>4</v>
       </c>
       <c r="P18" s="4">
@@ -7586,14 +7601,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M19" t="s">
         <v>50</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="16">
         <v>3</v>
       </c>
-      <c r="O19" s="15">
+      <c r="O19" s="16">
         <v>3</v>
       </c>
       <c r="P19" s="4">
@@ -7601,14 +7616,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M20" t="s">
         <v>61</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="16">
         <v>2</v>
       </c>
-      <c r="O20" s="15">
+      <c r="O20" s="16">
         <v>2</v>
       </c>
       <c r="P20" s="4">
@@ -7616,14 +7631,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L21" t="s">
         <v>103</v>
       </c>
-      <c r="N21" s="15">
+      <c r="N21" s="16">
         <v>18</v>
       </c>
-      <c r="O21" s="15">
+      <c r="O21" s="16">
         <v>14</v>
       </c>
       <c r="P21" s="4">
@@ -7631,17 +7646,17 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L22" t="s">
         <v>91</v>
       </c>
       <c r="M22" t="s">
         <v>94</v>
       </c>
-      <c r="N22" s="15">
+      <c r="N22" s="16">
         <v>6</v>
       </c>
-      <c r="O22" s="15">
+      <c r="O22" s="16">
         <v>3</v>
       </c>
       <c r="P22" s="4">
@@ -7649,14 +7664,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M23" t="s">
         <v>93</v>
       </c>
-      <c r="N23" s="15">
+      <c r="N23" s="16">
         <v>6</v>
       </c>
-      <c r="O23" s="15">
+      <c r="O23" s="16">
         <v>5</v>
       </c>
       <c r="P23" s="4">
@@ -7664,14 +7679,14 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="24" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M24" t="s">
         <v>50</v>
       </c>
-      <c r="N24" s="15">
-        <v>1</v>
-      </c>
-      <c r="O24" s="15">
+      <c r="N24" s="16">
+        <v>1</v>
+      </c>
+      <c r="O24" s="16">
         <v>1</v>
       </c>
       <c r="P24" s="4">
@@ -7679,14 +7694,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L25" t="s">
         <v>104</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="16">
         <v>13</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="16">
         <v>9</v>
       </c>
       <c r="P25" s="4">
@@ -7694,17 +7709,17 @@
         <v>0.69230769230769229</v>
       </c>
     </row>
-    <row r="26" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L26" t="s">
         <v>90</v>
       </c>
       <c r="M26" t="s">
         <v>94</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N26" s="16">
         <v>8</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="16">
         <v>6</v>
       </c>
       <c r="P26" s="4">
@@ -7712,14 +7727,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M27" t="s">
         <v>93</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="16">
         <v>3</v>
       </c>
-      <c r="O27" s="15">
+      <c r="O27" s="16">
         <v>1</v>
       </c>
       <c r="P27" s="4">
@@ -7727,14 +7742,14 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="28" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M28" t="s">
         <v>61</v>
       </c>
-      <c r="N28" s="15">
-        <v>1</v>
-      </c>
-      <c r="O28" s="15">
+      <c r="N28" s="16">
+        <v>1</v>
+      </c>
+      <c r="O28" s="16">
         <v>1</v>
       </c>
       <c r="P28" s="4">
@@ -7742,14 +7757,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L29" t="s">
         <v>105</v>
       </c>
-      <c r="N29" s="15">
+      <c r="N29" s="16">
         <v>12</v>
       </c>
-      <c r="O29" s="15">
+      <c r="O29" s="16">
         <v>8</v>
       </c>
       <c r="P29" s="4">
@@ -7757,17 +7772,17 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="30" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L30" t="s">
         <v>99</v>
       </c>
       <c r="M30" t="s">
         <v>94</v>
       </c>
-      <c r="N30" s="15">
+      <c r="N30" s="16">
         <v>5</v>
       </c>
-      <c r="O30" s="15">
+      <c r="O30" s="16">
         <v>3</v>
       </c>
       <c r="P30" s="4">
@@ -7775,14 +7790,14 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M31" t="s">
         <v>93</v>
       </c>
-      <c r="N31" s="15">
+      <c r="N31" s="16">
         <v>8</v>
       </c>
-      <c r="O31" s="15">
+      <c r="O31" s="16">
         <v>7</v>
       </c>
       <c r="P31" s="4">
@@ -7790,14 +7805,14 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="32" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M32" t="s">
         <v>50</v>
       </c>
-      <c r="N32" s="15">
+      <c r="N32" s="16">
         <v>2</v>
       </c>
-      <c r="O32" s="15">
+      <c r="O32" s="16">
         <v>1</v>
       </c>
       <c r="P32" s="4">
@@ -7805,14 +7820,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L33" t="s">
         <v>106</v>
       </c>
-      <c r="N33" s="15">
+      <c r="N33" s="16">
         <v>15</v>
       </c>
-      <c r="O33" s="15">
+      <c r="O33" s="16">
         <v>11</v>
       </c>
       <c r="P33" s="4">
@@ -7820,17 +7835,17 @@
         <v>0.73333333333333328</v>
       </c>
     </row>
-    <row r="34" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L34" t="s">
         <v>108</v>
       </c>
       <c r="M34" t="s">
         <v>93</v>
       </c>
-      <c r="N34" s="15">
-        <v>1</v>
-      </c>
-      <c r="O34" s="15">
+      <c r="N34" s="16">
+        <v>1</v>
+      </c>
+      <c r="O34" s="16">
         <v>1</v>
       </c>
       <c r="P34" s="4">
@@ -7838,14 +7853,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L35" t="s">
         <v>109</v>
       </c>
-      <c r="N35" s="15">
-        <v>1</v>
-      </c>
-      <c r="O35" s="15">
+      <c r="N35" s="16">
+        <v>1</v>
+      </c>
+      <c r="O35" s="16">
         <v>1</v>
       </c>
       <c r="P35" s="4">
@@ -7853,67 +7868,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:16" x14ac:dyDescent="0.35">
       <c r="L36" t="s">
         <v>53</v>
       </c>
-      <c r="N36" s="15">
+      <c r="N36" s="16">
         <v>101</v>
       </c>
-      <c r="O36" s="15">
+      <c r="O36" s="16">
         <v>70</v>
       </c>
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="12:16" x14ac:dyDescent="0.35">
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P49" s="4"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P53" s="4"/>
     </row>
   </sheetData>
@@ -7984,27 +7999,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I368"/>
+  <dimension ref="A1:I369"/>
   <sheetViews>
-    <sheetView topLeftCell="A325" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I369" sqref="I369"/>
+    <sheetView topLeftCell="A351" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I370" sqref="I370"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -8033,7 +8048,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -8062,7 +8077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -8091,7 +8106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -8120,7 +8135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -8149,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -8178,7 +8193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -8207,7 +8222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -8236,7 +8251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -8265,7 +8280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -8294,7 +8309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -8323,7 +8338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -8352,7 +8367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -8381,7 +8396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -8410,7 +8425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -8439,7 +8454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -8468,7 +8483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -8497,7 +8512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -8526,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -8555,7 +8570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -8584,7 +8599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -8613,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -8642,7 +8657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -8671,7 +8686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -8700,7 +8715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -8729,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -8758,7 +8773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -8787,7 +8802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -8816,7 +8831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -8845,7 +8860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -8874,7 +8889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -8903,7 +8918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -8932,7 +8947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -8961,7 +8976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -8990,7 +9005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -9019,7 +9034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -9048,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -9077,7 +9092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -9106,7 +9121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -9135,7 +9150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -9164,7 +9179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -9193,7 +9208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -9222,7 +9237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -9251,7 +9266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -9280,7 +9295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -9309,7 +9324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -9338,7 +9353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -9367,7 +9382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -9396,7 +9411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -9425,7 +9440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -9454,7 +9469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -9483,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -9512,7 +9527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -9541,7 +9556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -9570,7 +9585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -9599,7 +9614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -9628,7 +9643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -9657,7 +9672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -9686,7 +9701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -9715,7 +9730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -9744,7 +9759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -9773,7 +9788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -9802,7 +9817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -9831,7 +9846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -9860,7 +9875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -9889,7 +9904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -9918,7 +9933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -9947,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -9976,7 +9991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -10005,7 +10020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -10034,7 +10049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -10063,7 +10078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -10092,7 +10107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -10121,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -10150,7 +10165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -10179,7 +10194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -10208,7 +10223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -10237,7 +10252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -10266,7 +10281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -10295,7 +10310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -10324,7 +10339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -10353,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -10382,7 +10397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -10411,7 +10426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -10440,7 +10455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -10469,7 +10484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -10498,7 +10513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -10527,7 +10542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -10556,7 +10571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -10585,7 +10600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -10614,7 +10629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -10643,7 +10658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -10672,7 +10687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -10701,7 +10716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>87</v>
       </c>
@@ -10730,7 +10745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -10759,7 +10774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -10788,7 +10803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>87</v>
       </c>
@@ -10817,7 +10832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>87</v>
       </c>
@@ -10846,7 +10861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -10875,7 +10890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -10904,7 +10919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>87</v>
       </c>
@@ -10933,7 +10948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>87</v>
       </c>
@@ -10962,7 +10977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>87</v>
       </c>
@@ -10991,7 +11006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>87</v>
       </c>
@@ -11020,7 +11035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>87</v>
       </c>
@@ -11049,7 +11064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>87</v>
       </c>
@@ -11078,7 +11093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>87</v>
       </c>
@@ -11107,7 +11122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>87</v>
       </c>
@@ -11136,7 +11151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>87</v>
       </c>
@@ -11165,7 +11180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>87</v>
       </c>
@@ -11194,7 +11209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>87</v>
       </c>
@@ -11223,7 +11238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>87</v>
       </c>
@@ -11252,7 +11267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>87</v>
       </c>
@@ -11281,7 +11296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>87</v>
       </c>
@@ -11310,7 +11325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>87</v>
       </c>
@@ -11339,7 +11354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>87</v>
       </c>
@@ -11368,7 +11383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>87</v>
       </c>
@@ -11397,7 +11412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>87</v>
       </c>
@@ -11426,7 +11441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>87</v>
       </c>
@@ -11455,7 +11470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>87</v>
       </c>
@@ -11484,7 +11499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>87</v>
       </c>
@@ -11513,7 +11528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>88</v>
       </c>
@@ -11542,7 +11557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -11571,7 +11586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>88</v>
       </c>
@@ -11600,7 +11615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>88</v>
       </c>
@@ -11629,7 +11644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>88</v>
       </c>
@@ -11658,7 +11673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>88</v>
       </c>
@@ -11687,7 +11702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>88</v>
       </c>
@@ -11716,7 +11731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>88</v>
       </c>
@@ -11745,7 +11760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>88</v>
       </c>
@@ -11774,7 +11789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>88</v>
       </c>
@@ -11803,7 +11818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>88</v>
       </c>
@@ -11832,7 +11847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>88</v>
       </c>
@@ -11861,7 +11876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>88</v>
       </c>
@@ -11890,7 +11905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>88</v>
       </c>
@@ -11919,7 +11934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>88</v>
       </c>
@@ -11948,7 +11963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>88</v>
       </c>
@@ -11977,7 +11992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>88</v>
       </c>
@@ -12006,7 +12021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>88</v>
       </c>
@@ -12035,7 +12050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>88</v>
       </c>
@@ -12064,7 +12079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>88</v>
       </c>
@@ -12093,7 +12108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>88</v>
       </c>
@@ -12122,7 +12137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>88</v>
       </c>
@@ -12151,7 +12166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>88</v>
       </c>
@@ -12180,7 +12195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>88</v>
       </c>
@@ -12209,7 +12224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>88</v>
       </c>
@@ -12238,7 +12253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>88</v>
       </c>
@@ -12267,7 +12282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>88</v>
       </c>
@@ -12296,7 +12311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>88</v>
       </c>
@@ -12325,7 +12340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>88</v>
       </c>
@@ -12354,7 +12369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -12383,7 +12398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>88</v>
       </c>
@@ -12412,7 +12427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>88</v>
       </c>
@@ -12441,7 +12456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>88</v>
       </c>
@@ -12470,7 +12485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>88</v>
       </c>
@@ -12499,7 +12514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>88</v>
       </c>
@@ -12528,7 +12543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>88</v>
       </c>
@@ -12557,7 +12572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>89</v>
       </c>
@@ -12586,7 +12601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>89</v>
       </c>
@@ -12615,7 +12630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>89</v>
       </c>
@@ -12644,7 +12659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>89</v>
       </c>
@@ -12673,7 +12688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -12702,7 +12717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>89</v>
       </c>
@@ -12731,7 +12746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>89</v>
       </c>
@@ -12760,7 +12775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>89</v>
       </c>
@@ -12789,7 +12804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>89</v>
       </c>
@@ -12818,7 +12833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>89</v>
       </c>
@@ -12847,7 +12862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>89</v>
       </c>
@@ -12876,7 +12891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>89</v>
       </c>
@@ -12905,7 +12920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>89</v>
       </c>
@@ -12934,7 +12949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>89</v>
       </c>
@@ -12963,7 +12978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>89</v>
       </c>
@@ -12992,7 +13007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>89</v>
       </c>
@@ -13021,7 +13036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>89</v>
       </c>
@@ -13050,7 +13065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>89</v>
       </c>
@@ -13079,7 +13094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>89</v>
       </c>
@@ -13108,7 +13123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>89</v>
       </c>
@@ -13137,7 +13152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>89</v>
       </c>
@@ -13166,7 +13181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>89</v>
       </c>
@@ -13195,7 +13210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>89</v>
       </c>
@@ -13224,7 +13239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>89</v>
       </c>
@@ -13253,7 +13268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>89</v>
       </c>
@@ -13282,7 +13297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>89</v>
       </c>
@@ -13311,7 +13326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>89</v>
       </c>
@@ -13340,7 +13355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>89</v>
       </c>
@@ -13369,7 +13384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>89</v>
       </c>
@@ -13398,7 +13413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>89</v>
       </c>
@@ -13427,7 +13442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>89</v>
       </c>
@@ -13456,7 +13471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>89</v>
       </c>
@@ -13485,7 +13500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>89</v>
       </c>
@@ -13514,7 +13529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>89</v>
       </c>
@@ -13543,7 +13558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>89</v>
       </c>
@@ -13572,7 +13587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>89</v>
       </c>
@@ -13601,7 +13616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>89</v>
       </c>
@@ -13630,7 +13645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>89</v>
       </c>
@@ -13659,7 +13674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>89</v>
       </c>
@@ -13688,7 +13703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>89</v>
       </c>
@@ -13717,7 +13732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>89</v>
       </c>
@@ -13746,7 +13761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>89</v>
       </c>
@@ -13775,7 +13790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>89</v>
       </c>
@@ -13804,7 +13819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>89</v>
       </c>
@@ -13833,7 +13848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>89</v>
       </c>
@@ -13862,7 +13877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>89</v>
       </c>
@@ -13891,7 +13906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>89</v>
       </c>
@@ -13920,7 +13935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>89</v>
       </c>
@@ -13949,7 +13964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>89</v>
       </c>
@@ -13978,7 +13993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>89</v>
       </c>
@@ -14007,7 +14022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>89</v>
       </c>
@@ -14036,7 +14051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>89</v>
       </c>
@@ -14065,7 +14080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>89</v>
       </c>
@@ -14094,7 +14109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>89</v>
       </c>
@@ -14123,7 +14138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>89</v>
       </c>
@@ -14152,7 +14167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>89</v>
       </c>
@@ -14181,7 +14196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>89</v>
       </c>
@@ -14210,7 +14225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>91</v>
       </c>
@@ -14239,7 +14254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>91</v>
       </c>
@@ -14268,7 +14283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>91</v>
       </c>
@@ -14297,7 +14312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>91</v>
       </c>
@@ -14326,7 +14341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>91</v>
       </c>
@@ -14355,7 +14370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -14384,7 +14399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>91</v>
       </c>
@@ -14413,7 +14428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>91</v>
       </c>
@@ -14442,7 +14457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>91</v>
       </c>
@@ -14471,7 +14486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>91</v>
       </c>
@@ -14500,7 +14515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>91</v>
       </c>
@@ -14529,7 +14544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>91</v>
       </c>
@@ -14558,7 +14573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>91</v>
       </c>
@@ -14587,7 +14602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>91</v>
       </c>
@@ -14616,7 +14631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>91</v>
       </c>
@@ -14645,7 +14660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>91</v>
       </c>
@@ -14674,7 +14689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>91</v>
       </c>
@@ -14703,7 +14718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>91</v>
       </c>
@@ -14732,7 +14747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>91</v>
       </c>
@@ -14761,7 +14776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>91</v>
       </c>
@@ -14790,7 +14805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>91</v>
       </c>
@@ -14819,7 +14834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>91</v>
       </c>
@@ -14848,7 +14863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>91</v>
       </c>
@@ -14877,7 +14892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>91</v>
       </c>
@@ -14906,7 +14921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>91</v>
       </c>
@@ -14935,7 +14950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>91</v>
       </c>
@@ -14964,7 +14979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>91</v>
       </c>
@@ -14993,7 +15008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>91</v>
       </c>
@@ -15022,7 +15037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>91</v>
       </c>
@@ -15051,7 +15066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>91</v>
       </c>
@@ -15080,7 +15095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>91</v>
       </c>
@@ -15109,7 +15124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>91</v>
       </c>
@@ -15138,7 +15153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>91</v>
       </c>
@@ -15167,7 +15182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>91</v>
       </c>
@@ -15196,7 +15211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>91</v>
       </c>
@@ -15225,7 +15240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>91</v>
       </c>
@@ -15254,7 +15269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>91</v>
       </c>
@@ -15283,7 +15298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>91</v>
       </c>
@@ -15312,7 +15327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>91</v>
       </c>
@@ -15341,7 +15356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>91</v>
       </c>
@@ -15370,7 +15385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>91</v>
       </c>
@@ -15399,7 +15414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>91</v>
       </c>
@@ -15428,7 +15443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>91</v>
       </c>
@@ -15457,7 +15472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>91</v>
       </c>
@@ -15486,7 +15501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>91</v>
       </c>
@@ -15515,7 +15530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>91</v>
       </c>
@@ -15544,7 +15559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>91</v>
       </c>
@@ -15573,7 +15588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>91</v>
       </c>
@@ -15602,7 +15617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>90</v>
       </c>
@@ -15631,7 +15646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>90</v>
       </c>
@@ -15660,7 +15675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>90</v>
       </c>
@@ -15689,7 +15704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>90</v>
       </c>
@@ -15718,7 +15733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>90</v>
       </c>
@@ -15747,7 +15762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>90</v>
       </c>
@@ -15776,7 +15791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>90</v>
       </c>
@@ -15805,7 +15820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>90</v>
       </c>
@@ -15834,7 +15849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>90</v>
       </c>
@@ -15863,7 +15878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>90</v>
       </c>
@@ -15892,7 +15907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>90</v>
       </c>
@@ -15921,7 +15936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>90</v>
       </c>
@@ -15950,7 +15965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>90</v>
       </c>
@@ -15979,7 +15994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>90</v>
       </c>
@@ -16008,7 +16023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>90</v>
       </c>
@@ -16037,7 +16052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>90</v>
       </c>
@@ -16066,7 +16081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>90</v>
       </c>
@@ -16095,7 +16110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>90</v>
       </c>
@@ -16124,7 +16139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>90</v>
       </c>
@@ -16153,7 +16168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>90</v>
       </c>
@@ -16182,7 +16197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>90</v>
       </c>
@@ -16211,7 +16226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>90</v>
       </c>
@@ -16240,7 +16255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>90</v>
       </c>
@@ -16269,7 +16284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>90</v>
       </c>
@@ -16298,7 +16313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>90</v>
       </c>
@@ -16327,7 +16342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>90</v>
       </c>
@@ -16356,7 +16371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>90</v>
       </c>
@@ -16385,7 +16400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>90</v>
       </c>
@@ -16414,7 +16429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>90</v>
       </c>
@@ -16443,7 +16458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>90</v>
       </c>
@@ -16472,7 +16487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>90</v>
       </c>
@@ -16501,7 +16516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>90</v>
       </c>
@@ -16530,7 +16545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>90</v>
       </c>
@@ -16559,7 +16574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>90</v>
       </c>
@@ -16588,7 +16603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>90</v>
       </c>
@@ -16617,7 +16632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>90</v>
       </c>
@@ -16646,7 +16661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>90</v>
       </c>
@@ -16675,7 +16690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>90</v>
       </c>
@@ -16704,7 +16719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>90</v>
       </c>
@@ -16733,7 +16748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>90</v>
       </c>
@@ -16762,7 +16777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>90</v>
       </c>
@@ -16791,7 +16806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>90</v>
       </c>
@@ -16820,7 +16835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>90</v>
       </c>
@@ -16849,7 +16864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>90</v>
       </c>
@@ -16878,7 +16893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>90</v>
       </c>
@@ -16907,7 +16922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>90</v>
       </c>
@@ -16936,7 +16951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>90</v>
       </c>
@@ -16965,7 +16980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>90</v>
       </c>
@@ -16994,7 +17009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>90</v>
       </c>
@@ -17023,7 +17038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>99</v>
       </c>
@@ -17052,7 +17067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>99</v>
       </c>
@@ -17081,7 +17096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>99</v>
       </c>
@@ -17110,7 +17125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>99</v>
       </c>
@@ -17139,7 +17154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>99</v>
       </c>
@@ -17168,7 +17183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>99</v>
       </c>
@@ -17197,7 +17212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>99</v>
       </c>
@@ -17226,7 +17241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>99</v>
       </c>
@@ -17255,7 +17270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>99</v>
       </c>
@@ -17284,7 +17299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>99</v>
       </c>
@@ -17313,7 +17328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>99</v>
       </c>
@@ -17342,7 +17357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>99</v>
       </c>
@@ -17371,7 +17386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>99</v>
       </c>
@@ -17400,7 +17415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>99</v>
       </c>
@@ -17429,7 +17444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>99</v>
       </c>
@@ -17458,7 +17473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>99</v>
       </c>
@@ -17487,7 +17502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>99</v>
       </c>
@@ -17516,7 +17531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>99</v>
       </c>
@@ -17545,7 +17560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>99</v>
       </c>
@@ -17574,7 +17589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>99</v>
       </c>
@@ -17603,7 +17618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>99</v>
       </c>
@@ -17632,7 +17647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>99</v>
       </c>
@@ -17661,7 +17676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>99</v>
       </c>
@@ -17690,7 +17705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>99</v>
       </c>
@@ -17719,7 +17734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>99</v>
       </c>
@@ -17748,7 +17763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>99</v>
       </c>
@@ -17777,7 +17792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>99</v>
       </c>
@@ -17806,7 +17821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>99</v>
       </c>
@@ -17835,7 +17850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>99</v>
       </c>
@@ -17864,7 +17879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>99</v>
       </c>
@@ -17893,7 +17908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>99</v>
       </c>
@@ -17922,7 +17937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>99</v>
       </c>
@@ -17951,7 +17966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>99</v>
       </c>
@@ -17980,7 +17995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>99</v>
       </c>
@@ -18009,7 +18024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>99</v>
       </c>
@@ -18038,7 +18053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>99</v>
       </c>
@@ -18067,7 +18082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>99</v>
       </c>
@@ -18096,7 +18111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>99</v>
       </c>
@@ -18125,7 +18140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>99</v>
       </c>
@@ -18154,7 +18169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>99</v>
       </c>
@@ -18183,7 +18198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>99</v>
       </c>
@@ -18212,7 +18227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>99</v>
       </c>
@@ -18241,7 +18256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>99</v>
       </c>
@@ -18270,7 +18285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>99</v>
       </c>
@@ -18299,7 +18314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>99</v>
       </c>
@@ -18328,7 +18343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>99</v>
       </c>
@@ -18357,7 +18372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>99</v>
       </c>
@@ -18386,7 +18401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>99</v>
       </c>
@@ -18415,7 +18430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>99</v>
       </c>
@@ -18444,7 +18459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>99</v>
       </c>
@@ -18473,7 +18488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>99</v>
       </c>
@@ -18502,7 +18517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>99</v>
       </c>
@@ -18531,7 +18546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>99</v>
       </c>
@@ -18560,7 +18575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>99</v>
       </c>
@@ -18589,7 +18604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>99</v>
       </c>
@@ -18618,7 +18633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>108</v>
       </c>
@@ -18628,13 +18643,13 @@
       <c r="C367" t="s">
         <v>23</v>
       </c>
-      <c r="D367" s="16">
+      <c r="D367" s="15">
         <v>0.75</v>
       </c>
       <c r="E367" t="s">
         <v>34</v>
       </c>
-      <c r="F367" s="16">
+      <c r="F367" s="15">
         <v>0.25</v>
       </c>
       <c r="G367" t="s">
@@ -18647,7 +18662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>108</v>
       </c>
@@ -18657,13 +18672,13 @@
       <c r="C368" t="s">
         <v>40</v>
       </c>
-      <c r="D368" s="16">
+      <c r="D368" s="15">
         <v>0.56999999999999995</v>
       </c>
       <c r="E368" t="s">
         <v>13</v>
       </c>
-      <c r="F368" s="16">
+      <c r="F368" s="15">
         <v>0.43</v>
       </c>
       <c r="G368" t="s">
@@ -18673,6 +18688,35 @@
         <v>84</v>
       </c>
       <c r="I368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
+        <v>108</v>
+      </c>
+      <c r="B369" s="1">
+        <v>45320</v>
+      </c>
+      <c r="C369" t="s">
+        <v>20</v>
+      </c>
+      <c r="D369" s="15">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E369" t="s">
+        <v>36</v>
+      </c>
+      <c r="F369" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="G369" t="s">
+        <v>64</v>
+      </c>
+      <c r="H369" t="s">
+        <v>84</v>
+      </c>
+      <c r="I369">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
historical back testing added
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F805017-830D-4194-BC72-639F5417717A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F49DA9-A53B-4152-B8C5-A25A326B68C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -964,7 +964,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45320.325966203702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="369" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45321.313462268517" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="371" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
@@ -983,7 +983,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-30T00:00:00" count="50">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-01-31T00:00:00" count="51">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1033,6 +1033,7 @@
         <d v="2024-01-27T00:00:00"/>
         <d v="2024-01-28T00:00:00"/>
         <d v="2024-01-29T00:00:00"/>
+        <d v="2024-01-30T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1040,7 +1041,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="661">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="663">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1393,6 +1394,8 @@
         <n v="0.75"/>
         <n v="0.56999999999999995"/>
         <n v="0.57999999999999996"/>
+        <n v="0.72299999999999998"/>
+        <n v="0.69799999999999995"/>
         <m/>
         <n v="0.87610539305886403" u="1"/>
         <n v="0.78056782297496197" u="1"/>
@@ -1740,7 +1743,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="369">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="371">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -5787,13 +5790,35 @@
     <n v="0.42"/>
     <s v="Playing At:  Ottawa Senators   Home"/>
     <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="49"/>
+    <s v="St. Louis Blues"/>
+    <x v="352"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.27700000000000002"/>
+    <s v="Playing At:  St. Louis Blues   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="49"/>
+    <s v="Seattle Kraken"/>
+    <x v="353"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.30199999999999999"/>
+    <s v="Playing At:  San Jose Sharks   Home"/>
+    <x v="2"/>
     <n v="1"/>
   </r>
   <r>
     <x v="8"/>
-    <x v="49"/>
+    <x v="50"/>
     <m/>
-    <x v="352"/>
+    <x v="354"/>
     <m/>
     <m/>
     <m/>
@@ -5804,6 +5829,190 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O37" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="8"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="34">
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
@@ -5822,7 +6031,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="51">
+      <items count="52">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -5862,7 +6071,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="49"/>
+        <item x="50"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -5873,15 +6082,14 @@
         <item x="46"/>
         <item x="47"/>
         <item x="48"/>
+        <item x="49"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="662">
-        <item x="352"/>
-        <item m="1" x="353"/>
-        <item m="1" x="354"/>
+      <items count="664">
+        <item x="354"/>
         <item m="1" x="355"/>
         <item m="1" x="356"/>
         <item m="1" x="357"/>
@@ -6182,14 +6390,16 @@
         <item m="1" x="652"/>
         <item m="1" x="653"/>
         <item m="1" x="654"/>
-        <item x="314"/>
         <item m="1" x="655"/>
         <item m="1" x="656"/>
+        <item x="314"/>
         <item m="1" x="657"/>
         <item m="1" x="658"/>
         <item m="1" x="659"/>
+        <item m="1" x="660"/>
+        <item m="1" x="661"/>
         <item x="9"/>
-        <item m="1" x="660"/>
+        <item m="1" x="662"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -6540,6 +6750,8 @@
         <item x="349"/>
         <item x="350"/>
         <item x="351"/>
+        <item x="352"/>
+        <item x="353"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6608,187 +6820,6 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O36" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="8"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="2"/>
-        <item x="6"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="33">
-    <i>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
@@ -7105,23 +7136,23 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -7129,7 +7160,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7137,7 +7168,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -7160,7 +7191,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L4" t="s">
         <v>86</v>
       </c>
@@ -7178,7 +7209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -7217,7 +7248,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
@@ -7233,11 +7264,11 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
@@ -7261,7 +7292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -7281,7 +7312,7 @@
       </c>
       <c r="F7" s="5">
         <f>SUM(C6:C9)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
@@ -7305,7 +7336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
@@ -7321,11 +7352,11 @@
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.55430711610486894</v>
+        <v>0.55223880597014929</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.69306930693069302</v>
+        <v>0.69607843137254899</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
@@ -7349,19 +7380,19 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="16">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="16">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>0.65909090909090906</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>107</v>
@@ -7392,35 +7423,35 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="16">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="16">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>0.59292035398230092</v>
+        <v>0.59649122807017541</v>
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.72554347826086951</v>
+        <v>0.72432432432432436</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" ref="F10:H10" si="2">F6/$B$13</f>
-        <v>0.27445652173913043</v>
+        <v>0.27567567567567569</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" si="2"/>
-        <v>0.15489130434782608</v>
+        <v>0.15405405405405406</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>4.0760869565217392E-2</v>
+        <v>4.0540540540540543E-2</v>
       </c>
       <c r="M10" t="s">
         <v>93</v>
@@ -7436,7 +7467,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
@@ -7444,11 +7475,11 @@
         <v>79</v>
       </c>
       <c r="C11" s="16">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0.51898734177215189</v>
+        <v>0.50632911392405067</v>
       </c>
       <c r="M11" t="s">
         <v>50</v>
@@ -7464,7 +7495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
@@ -7492,19 +7523,19 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="16">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C13" s="16">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0.59239130434782605</v>
+        <v>0.59189189189189184</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
@@ -7523,7 +7554,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
         <v>93</v>
       </c>
@@ -7538,7 +7569,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
         <v>50</v>
       </c>
@@ -7553,7 +7584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L16" t="s">
         <v>102</v>
       </c>
@@ -7568,7 +7599,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L17" t="s">
         <v>89</v>
       </c>
@@ -7586,7 +7617,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
         <v>93</v>
       </c>
@@ -7601,7 +7632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M19" t="s">
         <v>50</v>
       </c>
@@ -7616,7 +7647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
         <v>61</v>
       </c>
@@ -7631,7 +7662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L21" t="s">
         <v>103</v>
       </c>
@@ -7646,7 +7677,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="22" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L22" t="s">
         <v>91</v>
       </c>
@@ -7664,7 +7695,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
         <v>93</v>
       </c>
@@ -7679,7 +7710,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="24" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
         <v>50</v>
       </c>
@@ -7694,7 +7725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L25" t="s">
         <v>104</v>
       </c>
@@ -7709,7 +7740,7 @@
         <v>0.69230769230769229</v>
       </c>
     </row>
-    <row r="26" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L26" t="s">
         <v>90</v>
       </c>
@@ -7727,7 +7758,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>93</v>
       </c>
@@ -7742,7 +7773,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="28" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
         <v>61</v>
       </c>
@@ -7757,7 +7788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L29" t="s">
         <v>105</v>
       </c>
@@ -7772,7 +7803,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="30" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L30" t="s">
         <v>99</v>
       </c>
@@ -7790,7 +7821,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
         <v>93</v>
       </c>
@@ -7805,7 +7836,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="32" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M32" t="s">
         <v>50</v>
       </c>
@@ -7820,7 +7851,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L33" t="s">
         <v>106</v>
       </c>
@@ -7835,12 +7866,12 @@
         <v>0.73333333333333328</v>
       </c>
     </row>
-    <row r="34" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L34" t="s">
         <v>108</v>
       </c>
       <c r="M34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N34" s="16">
         <v>1</v>
@@ -7853,9 +7884,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="12:16" x14ac:dyDescent="0.35">
-      <c r="L35" t="s">
-        <v>109</v>
+    <row r="35" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>93</v>
       </c>
       <c r="N35" s="16">
         <v>1</v>
@@ -7868,67 +7899,76 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L36" t="s">
+        <v>109</v>
+      </c>
+      <c r="N36" s="16">
+        <v>2</v>
+      </c>
+      <c r="O36" s="16">
+        <v>2</v>
+      </c>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
         <v>53</v>
       </c>
-      <c r="N36" s="16">
-        <v>101</v>
-      </c>
-      <c r="O36" s="16">
-        <v>70</v>
-      </c>
-      <c r="P36" s="4"/>
-    </row>
-    <row r="37" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="N37" s="16">
+        <v>102</v>
+      </c>
+      <c r="O37" s="16">
+        <v>71</v>
+      </c>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="12:16" x14ac:dyDescent="0.25">
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P49" s="4"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P53" s="4"/>
     </row>
   </sheetData>
@@ -7999,27 +8039,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I369"/>
+  <dimension ref="A1:I371"/>
   <sheetViews>
     <sheetView topLeftCell="A351" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I370" sqref="I370"/>
+      <selection activeCell="I372" sqref="I372"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -8048,7 +8088,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -8077,7 +8117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -8106,7 +8146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -8135,7 +8175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -8164,7 +8204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -8193,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -8222,7 +8262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -8251,7 +8291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -8280,7 +8320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -8309,7 +8349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -8338,7 +8378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -8367,7 +8407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -8396,7 +8436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -8425,7 +8465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -8454,7 +8494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -8483,7 +8523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -8512,7 +8552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -8541,7 +8581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -8570,7 +8610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -8599,7 +8639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -8628,7 +8668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -8657,7 +8697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -8686,7 +8726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -8715,7 +8755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -8744,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -8773,7 +8813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -8802,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -8831,7 +8871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -8860,7 +8900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -8889,7 +8929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -8918,7 +8958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -8947,7 +8987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -8976,7 +9016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -9005,7 +9045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -9034,7 +9074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -9063,7 +9103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -9092,7 +9132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -9121,7 +9161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -9150,7 +9190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -9179,7 +9219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -9208,7 +9248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -9237,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -9266,7 +9306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -9295,7 +9335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -9324,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -9353,7 +9393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -9382,7 +9422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -9411,7 +9451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -9440,7 +9480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -9469,7 +9509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -9498,7 +9538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -9527,7 +9567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -9556,7 +9596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -9585,7 +9625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -9614,7 +9654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -9643,7 +9683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -9672,7 +9712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -9701,7 +9741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -9730,7 +9770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -9759,7 +9799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -9788,7 +9828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -9817,7 +9857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -9846,7 +9886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -9875,7 +9915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -9904,7 +9944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -9933,7 +9973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -9962,7 +10002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -9991,7 +10031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -10020,7 +10060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -10049,7 +10089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -10078,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -10107,7 +10147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -10136,7 +10176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -10165,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -10194,7 +10234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -10223,7 +10263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -10252,7 +10292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -10281,7 +10321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -10310,7 +10350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -10339,7 +10379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -10368,7 +10408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -10397,7 +10437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -10426,7 +10466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -10455,7 +10495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -10484,7 +10524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -10513,7 +10553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -10542,7 +10582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -10571,7 +10611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -10600,7 +10640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -10629,7 +10669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -10658,7 +10698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -10687,7 +10727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -10716,7 +10756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>87</v>
       </c>
@@ -10745,7 +10785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -10774,7 +10814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -10803,7 +10843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>87</v>
       </c>
@@ -10832,7 +10872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>87</v>
       </c>
@@ -10861,7 +10901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -10890,7 +10930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -10919,7 +10959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>87</v>
       </c>
@@ -10948,7 +10988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>87</v>
       </c>
@@ -10977,7 +11017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>87</v>
       </c>
@@ -11006,7 +11046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>87</v>
       </c>
@@ -11035,7 +11075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>87</v>
       </c>
@@ -11064,7 +11104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>87</v>
       </c>
@@ -11093,7 +11133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>87</v>
       </c>
@@ -11122,7 +11162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>87</v>
       </c>
@@ -11151,7 +11191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>87</v>
       </c>
@@ -11180,7 +11220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>87</v>
       </c>
@@ -11209,7 +11249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>87</v>
       </c>
@@ -11238,7 +11278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>87</v>
       </c>
@@ -11267,7 +11307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>87</v>
       </c>
@@ -11296,7 +11336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>87</v>
       </c>
@@ -11325,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>87</v>
       </c>
@@ -11354,7 +11394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>87</v>
       </c>
@@ -11383,7 +11423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>87</v>
       </c>
@@ -11412,7 +11452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>87</v>
       </c>
@@ -11441,7 +11481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>87</v>
       </c>
@@ -11470,7 +11510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>87</v>
       </c>
@@ -11499,7 +11539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>87</v>
       </c>
@@ -11528,7 +11568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>88</v>
       </c>
@@ -11557,7 +11597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -11586,7 +11626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>88</v>
       </c>
@@ -11615,7 +11655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>88</v>
       </c>
@@ -11644,7 +11684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>88</v>
       </c>
@@ -11673,7 +11713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>88</v>
       </c>
@@ -11702,7 +11742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>88</v>
       </c>
@@ -11731,7 +11771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>88</v>
       </c>
@@ -11760,7 +11800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>88</v>
       </c>
@@ -11789,7 +11829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>88</v>
       </c>
@@ -11818,7 +11858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>88</v>
       </c>
@@ -11847,7 +11887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>88</v>
       </c>
@@ -11876,7 +11916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>88</v>
       </c>
@@ -11905,7 +11945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>88</v>
       </c>
@@ -11934,7 +11974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>88</v>
       </c>
@@ -11963,7 +12003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>88</v>
       </c>
@@ -11992,7 +12032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>88</v>
       </c>
@@ -12021,7 +12061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>88</v>
       </c>
@@ -12050,7 +12090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>88</v>
       </c>
@@ -12079,7 +12119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>88</v>
       </c>
@@ -12108,7 +12148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>88</v>
       </c>
@@ -12137,7 +12177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>88</v>
       </c>
@@ -12166,7 +12206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>88</v>
       </c>
@@ -12195,7 +12235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>88</v>
       </c>
@@ -12224,7 +12264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>88</v>
       </c>
@@ -12253,7 +12293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>88</v>
       </c>
@@ -12282,7 +12322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>88</v>
       </c>
@@ -12311,7 +12351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>88</v>
       </c>
@@ -12340,7 +12380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>88</v>
       </c>
@@ -12369,7 +12409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -12398,7 +12438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>88</v>
       </c>
@@ -12427,7 +12467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>88</v>
       </c>
@@ -12456,7 +12496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>88</v>
       </c>
@@ -12485,7 +12525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>88</v>
       </c>
@@ -12514,7 +12554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>88</v>
       </c>
@@ -12543,7 +12583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>88</v>
       </c>
@@ -12572,7 +12612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>89</v>
       </c>
@@ -12601,7 +12641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>89</v>
       </c>
@@ -12630,7 +12670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>89</v>
       </c>
@@ -12659,7 +12699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>89</v>
       </c>
@@ -12688,7 +12728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -12717,7 +12757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>89</v>
       </c>
@@ -12746,7 +12786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>89</v>
       </c>
@@ -12775,7 +12815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>89</v>
       </c>
@@ -12804,7 +12844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>89</v>
       </c>
@@ -12833,7 +12873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>89</v>
       </c>
@@ -12862,7 +12902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>89</v>
       </c>
@@ -12891,7 +12931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>89</v>
       </c>
@@ -12920,7 +12960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>89</v>
       </c>
@@ -12949,7 +12989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>89</v>
       </c>
@@ -12978,7 +13018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>89</v>
       </c>
@@ -13007,7 +13047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>89</v>
       </c>
@@ -13036,7 +13076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>89</v>
       </c>
@@ -13065,7 +13105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>89</v>
       </c>
@@ -13094,7 +13134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>89</v>
       </c>
@@ -13123,7 +13163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>89</v>
       </c>
@@ -13152,7 +13192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>89</v>
       </c>
@@ -13181,7 +13221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>89</v>
       </c>
@@ -13210,7 +13250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>89</v>
       </c>
@@ -13239,7 +13279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>89</v>
       </c>
@@ -13268,7 +13308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>89</v>
       </c>
@@ -13297,7 +13337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>89</v>
       </c>
@@ -13326,7 +13366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>89</v>
       </c>
@@ -13355,7 +13395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>89</v>
       </c>
@@ -13384,7 +13424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>89</v>
       </c>
@@ -13413,7 +13453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>89</v>
       </c>
@@ -13442,7 +13482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>89</v>
       </c>
@@ -13471,7 +13511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>89</v>
       </c>
@@ -13500,7 +13540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>89</v>
       </c>
@@ -13529,7 +13569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>89</v>
       </c>
@@ -13558,7 +13598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>89</v>
       </c>
@@ -13587,7 +13627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>89</v>
       </c>
@@ -13616,7 +13656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>89</v>
       </c>
@@ -13645,7 +13685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>89</v>
       </c>
@@ -13674,7 +13714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>89</v>
       </c>
@@ -13703,7 +13743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>89</v>
       </c>
@@ -13732,7 +13772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>89</v>
       </c>
@@ -13761,7 +13801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>89</v>
       </c>
@@ -13790,7 +13830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>89</v>
       </c>
@@ -13819,7 +13859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>89</v>
       </c>
@@ -13848,7 +13888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>89</v>
       </c>
@@ -13877,7 +13917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>89</v>
       </c>
@@ -13906,7 +13946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>89</v>
       </c>
@@ -13935,7 +13975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>89</v>
       </c>
@@ -13964,7 +14004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>89</v>
       </c>
@@ -13993,7 +14033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>89</v>
       </c>
@@ -14022,7 +14062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>89</v>
       </c>
@@ -14051,7 +14091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>89</v>
       </c>
@@ -14080,7 +14120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>89</v>
       </c>
@@ -14109,7 +14149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>89</v>
       </c>
@@ -14138,7 +14178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>89</v>
       </c>
@@ -14167,7 +14207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>89</v>
       </c>
@@ -14196,7 +14236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>89</v>
       </c>
@@ -14225,7 +14265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>91</v>
       </c>
@@ -14254,7 +14294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>91</v>
       </c>
@@ -14283,7 +14323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>91</v>
       </c>
@@ -14312,7 +14352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>91</v>
       </c>
@@ -14341,7 +14381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>91</v>
       </c>
@@ -14370,7 +14410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -14399,7 +14439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>91</v>
       </c>
@@ -14428,7 +14468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>91</v>
       </c>
@@ -14457,7 +14497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>91</v>
       </c>
@@ -14486,7 +14526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>91</v>
       </c>
@@ -14515,7 +14555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>91</v>
       </c>
@@ -14544,7 +14584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>91</v>
       </c>
@@ -14573,7 +14613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>91</v>
       </c>
@@ -14602,7 +14642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>91</v>
       </c>
@@ -14631,7 +14671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>91</v>
       </c>
@@ -14660,7 +14700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>91</v>
       </c>
@@ -14689,7 +14729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>91</v>
       </c>
@@ -14718,7 +14758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>91</v>
       </c>
@@ -14747,7 +14787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>91</v>
       </c>
@@ -14776,7 +14816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>91</v>
       </c>
@@ -14805,7 +14845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>91</v>
       </c>
@@ -14834,7 +14874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>91</v>
       </c>
@@ -14863,7 +14903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>91</v>
       </c>
@@ -14892,7 +14932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>91</v>
       </c>
@@ -14921,7 +14961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>91</v>
       </c>
@@ -14950,7 +14990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>91</v>
       </c>
@@ -14979,7 +15019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>91</v>
       </c>
@@ -15008,7 +15048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>91</v>
       </c>
@@ -15037,7 +15077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>91</v>
       </c>
@@ -15066,7 +15106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>91</v>
       </c>
@@ -15095,7 +15135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>91</v>
       </c>
@@ -15124,7 +15164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>91</v>
       </c>
@@ -15153,7 +15193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>91</v>
       </c>
@@ -15182,7 +15222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>91</v>
       </c>
@@ -15211,7 +15251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>91</v>
       </c>
@@ -15240,7 +15280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>91</v>
       </c>
@@ -15269,7 +15309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>91</v>
       </c>
@@ -15298,7 +15338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>91</v>
       </c>
@@ -15327,7 +15367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>91</v>
       </c>
@@ -15356,7 +15396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>91</v>
       </c>
@@ -15385,7 +15425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>91</v>
       </c>
@@ -15414,7 +15454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>91</v>
       </c>
@@ -15443,7 +15483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>91</v>
       </c>
@@ -15472,7 +15512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>91</v>
       </c>
@@ -15501,7 +15541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>91</v>
       </c>
@@ -15530,7 +15570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>91</v>
       </c>
@@ -15559,7 +15599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>91</v>
       </c>
@@ -15588,7 +15628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>91</v>
       </c>
@@ -15617,7 +15657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>90</v>
       </c>
@@ -15646,7 +15686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>90</v>
       </c>
@@ -15675,7 +15715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>90</v>
       </c>
@@ -15704,7 +15744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>90</v>
       </c>
@@ -15733,7 +15773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>90</v>
       </c>
@@ -15762,7 +15802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>90</v>
       </c>
@@ -15791,7 +15831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>90</v>
       </c>
@@ -15820,7 +15860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>90</v>
       </c>
@@ -15849,7 +15889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>90</v>
       </c>
@@ -15878,7 +15918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>90</v>
       </c>
@@ -15907,7 +15947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>90</v>
       </c>
@@ -15936,7 +15976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>90</v>
       </c>
@@ -15965,7 +16005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>90</v>
       </c>
@@ -15994,7 +16034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>90</v>
       </c>
@@ -16023,7 +16063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>90</v>
       </c>
@@ -16052,7 +16092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>90</v>
       </c>
@@ -16081,7 +16121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>90</v>
       </c>
@@ -16110,7 +16150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>90</v>
       </c>
@@ -16139,7 +16179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>90</v>
       </c>
@@ -16168,7 +16208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>90</v>
       </c>
@@ -16197,7 +16237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>90</v>
       </c>
@@ -16226,7 +16266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>90</v>
       </c>
@@ -16255,7 +16295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>90</v>
       </c>
@@ -16284,7 +16324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>90</v>
       </c>
@@ -16313,7 +16353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>90</v>
       </c>
@@ -16342,7 +16382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>90</v>
       </c>
@@ -16371,7 +16411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>90</v>
       </c>
@@ -16400,7 +16440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>90</v>
       </c>
@@ -16429,7 +16469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>90</v>
       </c>
@@ -16458,7 +16498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>90</v>
       </c>
@@ -16487,7 +16527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>90</v>
       </c>
@@ -16516,7 +16556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>90</v>
       </c>
@@ -16545,7 +16585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>90</v>
       </c>
@@ -16574,7 +16614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>90</v>
       </c>
@@ -16603,7 +16643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>90</v>
       </c>
@@ -16632,7 +16672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>90</v>
       </c>
@@ -16661,7 +16701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>90</v>
       </c>
@@ -16690,7 +16730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>90</v>
       </c>
@@ -16719,7 +16759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>90</v>
       </c>
@@ -16748,7 +16788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>90</v>
       </c>
@@ -16777,7 +16817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>90</v>
       </c>
@@ -16806,7 +16846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>90</v>
       </c>
@@ -16835,7 +16875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>90</v>
       </c>
@@ -16864,7 +16904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>90</v>
       </c>
@@ -16893,7 +16933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>90</v>
       </c>
@@ -16922,7 +16962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>90</v>
       </c>
@@ -16951,7 +16991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>90</v>
       </c>
@@ -16980,7 +17020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>90</v>
       </c>
@@ -17009,7 +17049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>90</v>
       </c>
@@ -17038,7 +17078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>99</v>
       </c>
@@ -17067,7 +17107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>99</v>
       </c>
@@ -17096,7 +17136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>99</v>
       </c>
@@ -17125,7 +17165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>99</v>
       </c>
@@ -17154,7 +17194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>99</v>
       </c>
@@ -17183,7 +17223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>99</v>
       </c>
@@ -17212,7 +17252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>99</v>
       </c>
@@ -17241,7 +17281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>99</v>
       </c>
@@ -17270,7 +17310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>99</v>
       </c>
@@ -17299,7 +17339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>99</v>
       </c>
@@ -17328,7 +17368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>99</v>
       </c>
@@ -17357,7 +17397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>99</v>
       </c>
@@ -17386,7 +17426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>99</v>
       </c>
@@ -17415,7 +17455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>99</v>
       </c>
@@ -17444,7 +17484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>99</v>
       </c>
@@ -17473,7 +17513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>99</v>
       </c>
@@ -17502,7 +17542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>99</v>
       </c>
@@ -17531,7 +17571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>99</v>
       </c>
@@ -17560,7 +17600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>99</v>
       </c>
@@ -17589,7 +17629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>99</v>
       </c>
@@ -17618,7 +17658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>99</v>
       </c>
@@ -17647,7 +17687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>99</v>
       </c>
@@ -17676,7 +17716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>99</v>
       </c>
@@ -17705,7 +17745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>99</v>
       </c>
@@ -17734,7 +17774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>99</v>
       </c>
@@ -17763,7 +17803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>99</v>
       </c>
@@ -17792,7 +17832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>99</v>
       </c>
@@ -17821,7 +17861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>99</v>
       </c>
@@ -17850,7 +17890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>99</v>
       </c>
@@ -17879,7 +17919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>99</v>
       </c>
@@ -17908,7 +17948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>99</v>
       </c>
@@ -17937,7 +17977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>99</v>
       </c>
@@ -17966,7 +18006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>99</v>
       </c>
@@ -17995,7 +18035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>99</v>
       </c>
@@ -18024,7 +18064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>99</v>
       </c>
@@ -18053,7 +18093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>99</v>
       </c>
@@ -18082,7 +18122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>99</v>
       </c>
@@ -18111,7 +18151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>99</v>
       </c>
@@ -18140,7 +18180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>99</v>
       </c>
@@ -18169,7 +18209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>99</v>
       </c>
@@ -18198,7 +18238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>99</v>
       </c>
@@ -18227,7 +18267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>99</v>
       </c>
@@ -18256,7 +18296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>99</v>
       </c>
@@ -18285,7 +18325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>99</v>
       </c>
@@ -18314,7 +18354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>99</v>
       </c>
@@ -18343,7 +18383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>99</v>
       </c>
@@ -18372,7 +18412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>99</v>
       </c>
@@ -18401,7 +18441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>99</v>
       </c>
@@ -18430,7 +18470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>99</v>
       </c>
@@ -18459,7 +18499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>99</v>
       </c>
@@ -18488,7 +18528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>99</v>
       </c>
@@ -18517,7 +18557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>99</v>
       </c>
@@ -18546,7 +18586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>99</v>
       </c>
@@ -18575,7 +18615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>99</v>
       </c>
@@ -18604,7 +18644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>99</v>
       </c>
@@ -18633,7 +18673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>108</v>
       </c>
@@ -18662,7 +18702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>108</v>
       </c>
@@ -18691,7 +18731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>108</v>
       </c>
@@ -18717,6 +18757,64 @@
         <v>84</v>
       </c>
       <c r="I369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>108</v>
+      </c>
+      <c r="B370" s="1">
+        <v>45321</v>
+      </c>
+      <c r="C370" t="s">
+        <v>13</v>
+      </c>
+      <c r="D370" s="14">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="E370" t="s">
+        <v>34</v>
+      </c>
+      <c r="F370" s="14">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G370" t="s">
+        <v>65</v>
+      </c>
+      <c r="H370" t="s">
+        <v>94</v>
+      </c>
+      <c r="I370">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>108</v>
+      </c>
+      <c r="B371" s="1">
+        <v>45321</v>
+      </c>
+      <c r="C371" t="s">
+        <v>23</v>
+      </c>
+      <c r="D371" s="14">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="E371" t="s">
+        <v>56</v>
+      </c>
+      <c r="F371" s="14">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="G371" t="s">
+        <v>62</v>
+      </c>
+      <c r="H371" t="s">
+        <v>51</v>
+      </c>
+      <c r="I371">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated predictions and retrained model
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AF6BFC-919F-4B26-B4E8-CF8E97570427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAAB2AA-5305-42A6-A8E9-B55A0183A67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="14" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -976,7 +976,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45339.891772106479" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="456" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45340.360549305558" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="459" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
@@ -997,7 +997,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-02-18T00:00:00" count="65">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-02-19T00:00:00" count="66">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1062,6 +1062,7 @@
         <d v="2024-02-15T00:00:00"/>
         <d v="2024-02-16T00:00:00"/>
         <d v="2024-02-17T00:00:00"/>
+        <d v="2024-02-18T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1069,7 +1070,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="736">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="738">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1497,6 +1498,8 @@
         <n v="0.51239999999999997"/>
         <n v="0.51039999999999996"/>
         <n v="0.501"/>
+        <n v="0.72"/>
+        <n v="0.56899999999999995"/>
         <m/>
         <n v="0.87610539305886403" u="1"/>
         <n v="0.78056782297496197" u="1"/>
@@ -1844,7 +1847,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="456">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="459">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -6793,7 +6796,7 @@
     <n v="0.45910000000000001"/>
     <s v="Playing At:  San Jose Sharks   Home"/>
     <x v="4"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="9"/>
@@ -6826,7 +6829,7 @@
     <n v="0.48759999999999998"/>
     <s v="Playing At:  Vancouver Canucks   Home"/>
     <x v="4"/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <x v="9"/>
@@ -6851,10 +6854,43 @@
     <n v="1"/>
   </r>
   <r>
+    <x v="9"/>
+    <x v="64"/>
+    <s v="Colorado Avalanche"/>
+    <x v="427"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.28000000000000003"/>
+    <s v="Playing At:  Colorado Avalanche   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="64"/>
+    <s v="New York Rangers"/>
+    <x v="356"/>
+    <s v="New York Islanders"/>
+    <n v="0.375"/>
+    <s v="Playing At:  New York Islanders   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="64"/>
+    <s v="Los Angeles Kings"/>
+    <x v="428"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.43099999999999999"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="10"/>
-    <x v="64"/>
+    <x v="65"/>
     <m/>
-    <x v="427"/>
+    <x v="429"/>
     <m/>
     <m/>
     <m/>
@@ -6865,7 +6901,216 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O44" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="12">
+        <item h="1" x="10"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="41">
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -6885,7 +7130,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="66">
+      <items count="67">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -6925,7 +7170,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="64"/>
+        <item x="65"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -6951,15 +7196,14 @@
         <item x="61"/>
         <item x="62"/>
         <item x="63"/>
+        <item x="64"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="737">
-        <item x="427"/>
-        <item m="1" x="428"/>
-        <item m="1" x="429"/>
+      <items count="739">
+        <item x="429"/>
         <item m="1" x="430"/>
         <item m="1" x="431"/>
         <item m="1" x="432"/>
@@ -7260,14 +7504,16 @@
         <item m="1" x="727"/>
         <item m="1" x="728"/>
         <item m="1" x="729"/>
-        <item x="314"/>
         <item m="1" x="730"/>
         <item m="1" x="731"/>
+        <item x="314"/>
         <item m="1" x="732"/>
         <item m="1" x="733"/>
         <item m="1" x="734"/>
+        <item m="1" x="735"/>
+        <item m="1" x="736"/>
         <item x="9"/>
-        <item m="1" x="735"/>
+        <item m="1" x="737"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -7693,6 +7939,8 @@
         <item x="424"/>
         <item x="425"/>
         <item x="426"/>
+        <item x="427"/>
+        <item x="428"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -7761,215 +8009,6 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O44" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="12">
-        <item h="1" x="10"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="2"/>
-        <item x="6"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="41">
-    <i>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
@@ -8286,7 +8325,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8414,11 +8453,11 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
@@ -8458,11 +8497,11 @@
       </c>
       <c r="E7" s="7">
         <f>SUM(C10:C12)</f>
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F7" s="5">
         <f>SUM(C6:C9)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
@@ -8502,11 +8541,11 @@
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.54705882352941182</v>
+        <v>0.54678362573099415</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.68695652173913047</v>
+        <v>0.68965517241379315</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
@@ -8535,14 +8574,14 @@
         <v>94</v>
       </c>
       <c r="B9" s="16">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="16">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>0.6470588235294118</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>107</v>
@@ -8578,30 +8617,30 @@
         <v>51</v>
       </c>
       <c r="B10" s="16">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C10" s="16">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.60273972602739723</v>
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.74725274725274726</v>
+        <v>0.74672489082969429</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" ref="F10:H10" si="2">F6/$B$13</f>
-        <v>0.25274725274725274</v>
+        <v>0.25327510917030566</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" si="2"/>
-        <v>0.14065934065934066</v>
+        <v>0.13973799126637554</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>3.5164835164835165E-2</v>
+        <v>3.4934497816593885E-2</v>
       </c>
       <c r="M10" t="s">
         <v>93</v>
@@ -8622,14 +8661,14 @@
         <v>84</v>
       </c>
       <c r="B11" s="16">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C11" s="16">
         <v>48</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0.50526315789473686</v>
+        <v>0.5</v>
       </c>
       <c r="M11" t="s">
         <v>50</v>
@@ -8678,14 +8717,14 @@
         <v>53</v>
       </c>
       <c r="B13" s="16">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C13" s="16">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0.58241758241758246</v>
+        <v>0.58296943231441045</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
@@ -9120,14 +9159,14 @@
         <v>94</v>
       </c>
       <c r="N40" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O40" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P40" s="4">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="41" spans="12:16" x14ac:dyDescent="0.35">
@@ -9165,14 +9204,14 @@
         <v>113</v>
       </c>
       <c r="N43" s="16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O43" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P43" s="4">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="44" spans="12:16" x14ac:dyDescent="0.35">
@@ -9180,10 +9219,10 @@
         <v>53</v>
       </c>
       <c r="N44" s="16">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O44" s="16">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P44" s="4"/>
     </row>
@@ -9282,10 +9321,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I456"/>
+  <dimension ref="A1:I459"/>
   <sheetViews>
     <sheetView topLeftCell="A434" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I444" sqref="I444:I456"/>
+      <selection activeCell="I460" sqref="I460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22378,7 +22417,7 @@
         <v>85</v>
       </c>
       <c r="I451">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="452" spans="1:9" x14ac:dyDescent="0.35">
@@ -22465,7 +22504,7 @@
         <v>85</v>
       </c>
       <c r="I454">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="455" spans="1:9" x14ac:dyDescent="0.35">
@@ -22524,6 +22563,93 @@
       </c>
       <c r="I456">
         <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A457" t="s">
+        <v>112</v>
+      </c>
+      <c r="B457" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C457" t="s">
+        <v>7</v>
+      </c>
+      <c r="D457" s="14">
+        <v>0.72</v>
+      </c>
+      <c r="E457" t="s">
+        <v>5</v>
+      </c>
+      <c r="F457" s="14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G457" t="s">
+        <v>9</v>
+      </c>
+      <c r="H457" t="s">
+        <v>94</v>
+      </c>
+      <c r="I457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A458" t="s">
+        <v>112</v>
+      </c>
+      <c r="B458" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C458" t="s">
+        <v>25</v>
+      </c>
+      <c r="D458" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="E458" t="s">
+        <v>39</v>
+      </c>
+      <c r="F458" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="G458" t="s">
+        <v>41</v>
+      </c>
+      <c r="H458" t="s">
+        <v>51</v>
+      </c>
+      <c r="I458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A459" t="s">
+        <v>112</v>
+      </c>
+      <c r="B459" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C459" t="s">
+        <v>40</v>
+      </c>
+      <c r="D459" s="14">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="E459" t="s">
+        <v>66</v>
+      </c>
+      <c r="F459" s="14">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G459" t="s">
+        <v>67</v>
+      </c>
+      <c r="H459" t="s">
+        <v>84</v>
+      </c>
+      <c r="I459">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated model and predictions
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1917E19-2A77-4AFD-9923-987A85145CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DA0A5D-1FAB-4D6F-B57F-E50FB6DE13E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="14" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2634" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>PDA11</t>
+  </si>
+  <si>
+    <t>PDA12</t>
   </si>
 </sst>
 </file>
@@ -927,10 +930,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -991,13 +994,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45346.490324999999" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="509" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45347.636613773146" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="516" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Model Used" numFmtId="0">
-      <sharedItems containsBlank="1" count="12">
+      <sharedItems containsBlank="1" count="13">
         <s v="PDA1"/>
         <s v="PDA2"/>
         <s v="PDA3"/>
@@ -1009,11 +1012,12 @@
         <s v="PDA9"/>
         <s v="PDA10"/>
         <s v="PDA11"/>
+        <s v="PDA12"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-02-25T00:00:00" count="72">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-02-26T00:00:00" count="73">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1085,6 +1089,7 @@
         <d v="2024-02-22T00:00:00"/>
         <d v="2024-02-23T00:00:00"/>
         <d v="2024-02-24T00:00:00"/>
+        <d v="2024-02-25T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1092,7 +1097,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="779">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="786">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1561,6 +1566,13 @@
         <n v="0.58140000000000003"/>
         <n v="0.55349999999999999"/>
         <n v="0.50429999999999997"/>
+        <n v="0.76870000000000005"/>
+        <n v="0.68979999999999997"/>
+        <n v="0.67620000000000002"/>
+        <n v="0.66700000000000004"/>
+        <n v="0.66300000000000003"/>
+        <n v="0.63970000000000005"/>
+        <n v="0.55489999999999995"/>
         <m/>
         <n v="0.77869999999999995" u="1"/>
         <n v="0.63949999999999996" u="1"/>
@@ -1910,7 +1922,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="509">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="516">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -7387,7 +7399,7 @@
     <n v="0.28949999999999998"/>
     <s v="Playing At:  Edmonton Oilers   Home"/>
     <x v="6"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="10"/>
@@ -7431,7 +7443,7 @@
     <n v="0.3523"/>
     <s v="Playing At:  Ottawa Senators   Home"/>
     <x v="2"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="10"/>
@@ -7502,8 +7514,85 @@
   <r>
     <x v="11"/>
     <x v="71"/>
+    <s v="New York Rangers"/>
+    <x v="468"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.23130000000000001"/>
+    <s v="Playing At:  Columbus Blue Jackets   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="71"/>
+    <s v="Detroit Red Wings"/>
+    <x v="469"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.31019999999999998"/>
+    <s v="Playing At:  Chicago Blackhawks   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="71"/>
+    <s v="Nashville Predators"/>
+    <x v="470"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.32379999999999998"/>
+    <s v="Playing At:  Anaheim Ducks   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="71"/>
+    <s v="Winnipeg Jets"/>
+    <x v="471"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.33300000000000002"/>
+    <s v="Playing At:  Winnipeg Jets   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="71"/>
+    <s v="Carolina Hurricanes"/>
+    <x v="472"/>
+    <s v="Buffalo Sabres"/>
+    <n v="0.33700000000000002"/>
+    <s v="Playing At:  Buffalo Sabres   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="71"/>
+    <s v="Pittsburgh Penguins"/>
+    <x v="473"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.36030000000000001"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="71"/>
+    <s v="New Jersey Devils"/>
+    <x v="474"/>
+    <s v="Tampa Bay Lightning"/>
+    <n v="0.4451"/>
+    <s v="Playing At:  New Jersey Devils   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="72"/>
     <m/>
-    <x v="468"/>
+    <x v="475"/>
     <m/>
     <m/>
     <m/>
@@ -7514,222 +7603,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O44" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="13">
-        <item h="1" x="11"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item h="1" x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="2"/>
-        <item x="6"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="41">
-    <i>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="13">
-        <item x="11"/>
+      <items count="14">
+        <item x="12"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -7741,11 +7620,12 @@
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
+        <item x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="73">
+      <items count="74">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -7785,7 +7665,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="71"/>
+        <item x="72"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -7818,20 +7698,14 @@
         <item x="68"/>
         <item x="69"/>
         <item x="70"/>
+        <item x="71"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="780">
-        <item x="468"/>
-        <item m="1" x="471"/>
-        <item m="1" x="472"/>
-        <item m="1" x="473"/>
-        <item m="1" x="474"/>
-        <item m="1" x="475"/>
-        <item m="1" x="476"/>
-        <item m="1" x="477"/>
+      <items count="787">
+        <item x="475"/>
         <item m="1" x="478"/>
         <item m="1" x="479"/>
         <item m="1" x="480"/>
@@ -8127,14 +8001,21 @@
         <item m="1" x="770"/>
         <item m="1" x="771"/>
         <item m="1" x="772"/>
-        <item x="314"/>
         <item m="1" x="773"/>
         <item m="1" x="774"/>
         <item m="1" x="775"/>
         <item m="1" x="776"/>
         <item m="1" x="777"/>
+        <item m="1" x="778"/>
+        <item m="1" x="779"/>
+        <item x="314"/>
+        <item m="1" x="780"/>
+        <item m="1" x="781"/>
+        <item m="1" x="782"/>
+        <item m="1" x="783"/>
+        <item m="1" x="784"/>
         <item x="9"/>
-        <item m="1" x="778"/>
+        <item m="1" x="785"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -8588,8 +8469,8 @@
         <item x="452"/>
         <item x="453"/>
         <item x="454"/>
-        <item m="1" x="469"/>
-        <item m="1" x="470"/>
+        <item m="1" x="476"/>
+        <item m="1" x="477"/>
         <item x="455"/>
         <item x="456"/>
         <item x="457"/>
@@ -8603,6 +8484,13 @@
         <item x="465"/>
         <item x="466"/>
         <item x="467"/>
+        <item x="468"/>
+        <item x="469"/>
+        <item x="470"/>
+        <item x="471"/>
+        <item x="472"/>
+        <item x="473"/>
+        <item x="474"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8671,6 +8559,217 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O44" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="14">
+        <item h="1" x="12"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="41">
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
@@ -8987,7 +9086,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9049,10 +9148,10 @@
       <c r="M4" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="19">
         <v>5</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="19">
         <v>5</v>
       </c>
       <c r="P4" s="4">
@@ -9088,10 +9187,10 @@
       <c r="M5" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="19">
         <v>7</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="19">
         <v>4</v>
       </c>
       <c r="P5" s="4">
@@ -9103,10 +9202,10 @@
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="19">
         <v>4</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="19">
         <v>4</v>
       </c>
       <c r="D6" s="4">
@@ -9115,15 +9214,15 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="9">
         <f>SUM(B6:B7)</f>
@@ -9132,10 +9231,10 @@
       <c r="M6" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N6" s="19">
         <v>2</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6" s="19">
         <v>2</v>
       </c>
       <c r="P6" s="4">
@@ -9147,10 +9246,10 @@
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="19">
         <v>13</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="19">
         <v>12</v>
       </c>
       <c r="D7" s="4">
@@ -9159,7 +9258,7 @@
       </c>
       <c r="E7" s="7">
         <f>SUM(C10:C12)</f>
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F7" s="5">
         <f>SUM(C6:C9)</f>
@@ -9167,7 +9266,7 @@
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" s="9">
         <f>SUM(C6:C7)</f>
@@ -9176,10 +9275,10 @@
       <c r="M7" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="16">
-        <v>1</v>
-      </c>
-      <c r="O7" s="16">
+      <c r="N7" s="19">
+        <v>1</v>
+      </c>
+      <c r="O7" s="19">
         <v>1</v>
       </c>
       <c r="P7" s="4">
@@ -9191,27 +9290,27 @@
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="16">
-        <v>52</v>
-      </c>
-      <c r="C8" s="16">
-        <v>35</v>
+      <c r="B8" s="19">
+        <v>53</v>
+      </c>
+      <c r="C8" s="19">
+        <v>36</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>0.67307692307692313</v>
+        <v>0.67924528301886788</v>
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.54046997389033946</v>
+        <v>0.53984575835475579</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.71199999999999997</v>
+        <v>0.70634920634920639</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
-        <v>0.73913043478260865</v>
+        <v>0.74285714285714288</v>
       </c>
       <c r="H8" s="10">
         <f>H7/H6</f>
@@ -9220,10 +9319,10 @@
       <c r="L8" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="19">
         <v>15</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="19">
         <v>12</v>
       </c>
       <c r="P8" s="4">
@@ -9235,15 +9334,15 @@
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="19">
         <v>56</v>
       </c>
-      <c r="C9" s="16">
-        <v>38</v>
+      <c r="C9" s="19">
+        <v>37</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>0.6785714285714286</v>
+        <v>0.6607142857142857</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>107</v>
@@ -9263,10 +9362,10 @@
       <c r="M9" t="s">
         <v>94</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="19">
         <v>8</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="19">
         <v>5</v>
       </c>
       <c r="P9" s="4">
@@ -9278,39 +9377,39 @@
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="16">
-        <v>164</v>
-      </c>
-      <c r="C10" s="16">
-        <v>97</v>
+      <c r="B10" s="19">
+        <v>169</v>
+      </c>
+      <c r="C10" s="19">
+        <v>100</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="1"/>
-        <v>0.59146341463414631</v>
+        <v>0.59171597633136097</v>
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.75393700787401574</v>
+        <v>0.75533980582524274</v>
       </c>
       <c r="F10" s="6">
         <f>F6/$B$13</f>
-        <v>0.24606299212598426</v>
+        <v>0.24466019417475729</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" ref="F10:H10" si="2">G6/$B$13</f>
-        <v>0.13582677165354332</v>
+        <f t="shared" ref="G10:H10" si="2">G6/$B$13</f>
+        <v>0.13592233009708737</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>3.3464566929133861E-2</v>
+        <v>3.3009708737864081E-2</v>
       </c>
       <c r="M10" t="s">
         <v>93</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="19">
         <v>6</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="19">
         <v>1</v>
       </c>
       <c r="P10" s="4">
@@ -9322,23 +9421,23 @@
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="16">
-        <v>109</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="19">
+        <v>110</v>
+      </c>
+      <c r="C11" s="19">
         <v>57</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0.52293577981651373</v>
+        <v>0.51818181818181819</v>
       </c>
       <c r="M11" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="16">
-        <v>1</v>
-      </c>
-      <c r="O11" s="16">
+      <c r="N11" s="19">
+        <v>1</v>
+      </c>
+      <c r="O11" s="19">
         <v>1</v>
       </c>
       <c r="P11" s="4">
@@ -9350,10 +9449,10 @@
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="19">
         <v>110</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="19">
         <v>53</v>
       </c>
       <c r="D12" s="4">
@@ -9363,10 +9462,10 @@
       <c r="L12" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="19">
         <v>15</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="19">
         <v>7</v>
       </c>
       <c r="P12" s="4">
@@ -9378,15 +9477,15 @@
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="16">
-        <v>508</v>
-      </c>
-      <c r="C13" s="16">
-        <v>296</v>
+      <c r="B13" s="19">
+        <v>515</v>
+      </c>
+      <c r="C13" s="19">
+        <v>299</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0.58267716535433067</v>
+        <v>0.58058252427184465</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
@@ -9394,10 +9493,10 @@
       <c r="M13" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="19">
         <v>3</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O13" s="19">
         <v>2</v>
       </c>
       <c r="P13" s="4">
@@ -9409,10 +9508,10 @@
       <c r="M14" t="s">
         <v>93</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="19">
         <v>7</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="19">
         <v>4</v>
       </c>
       <c r="P14" s="4">
@@ -9424,10 +9523,10 @@
       <c r="M15" t="s">
         <v>50</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N15" s="19">
         <v>2</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="19">
         <v>2</v>
       </c>
       <c r="P15" s="4">
@@ -9439,10 +9538,10 @@
       <c r="L16" t="s">
         <v>102</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N16" s="19">
         <v>12</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="19">
         <v>8</v>
       </c>
       <c r="P16" s="4">
@@ -9457,10 +9556,10 @@
       <c r="M17" t="s">
         <v>94</v>
       </c>
-      <c r="N17" s="16">
+      <c r="N17" s="19">
         <v>9</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="19">
         <v>5</v>
       </c>
       <c r="P17" s="4">
@@ -9472,10 +9571,10 @@
       <c r="M18" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N18" s="19">
         <v>4</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="19">
         <v>4</v>
       </c>
       <c r="P18" s="4">
@@ -9487,10 +9586,10 @@
       <c r="M19" t="s">
         <v>50</v>
       </c>
-      <c r="N19" s="16">
+      <c r="N19" s="19">
         <v>3</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="19">
         <v>3</v>
       </c>
       <c r="P19" s="4">
@@ -9502,10 +9601,10 @@
       <c r="M20" t="s">
         <v>61</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N20" s="19">
         <v>2</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="19">
         <v>2</v>
       </c>
       <c r="P20" s="4">
@@ -9517,10 +9616,10 @@
       <c r="L21" t="s">
         <v>103</v>
       </c>
-      <c r="N21" s="16">
+      <c r="N21" s="19">
         <v>18</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="19">
         <v>14</v>
       </c>
       <c r="P21" s="4">
@@ -9535,10 +9634,10 @@
       <c r="M22" t="s">
         <v>94</v>
       </c>
-      <c r="N22" s="16">
+      <c r="N22" s="19">
         <v>6</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="19">
         <v>3</v>
       </c>
       <c r="P22" s="4">
@@ -9550,10 +9649,10 @@
       <c r="M23" t="s">
         <v>93</v>
       </c>
-      <c r="N23" s="16">
+      <c r="N23" s="19">
         <v>6</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23" s="19">
         <v>5</v>
       </c>
       <c r="P23" s="4">
@@ -9565,10 +9664,10 @@
       <c r="M24" t="s">
         <v>50</v>
       </c>
-      <c r="N24" s="16">
-        <v>1</v>
-      </c>
-      <c r="O24" s="16">
+      <c r="N24" s="19">
+        <v>1</v>
+      </c>
+      <c r="O24" s="19">
         <v>1</v>
       </c>
       <c r="P24" s="4">
@@ -9580,10 +9679,10 @@
       <c r="L25" t="s">
         <v>104</v>
       </c>
-      <c r="N25" s="16">
+      <c r="N25" s="19">
         <v>13</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="19">
         <v>9</v>
       </c>
       <c r="P25" s="4">
@@ -9598,10 +9697,10 @@
       <c r="M26" t="s">
         <v>94</v>
       </c>
-      <c r="N26" s="16">
+      <c r="N26" s="19">
         <v>8</v>
       </c>
-      <c r="O26" s="16">
+      <c r="O26" s="19">
         <v>6</v>
       </c>
       <c r="P26" s="4">
@@ -9613,10 +9712,10 @@
       <c r="M27" t="s">
         <v>93</v>
       </c>
-      <c r="N27" s="16">
+      <c r="N27" s="19">
         <v>3</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="19">
         <v>1</v>
       </c>
       <c r="P27" s="4">
@@ -9628,10 +9727,10 @@
       <c r="M28" t="s">
         <v>61</v>
       </c>
-      <c r="N28" s="16">
-        <v>1</v>
-      </c>
-      <c r="O28" s="16">
+      <c r="N28" s="19">
+        <v>1</v>
+      </c>
+      <c r="O28" s="19">
         <v>1</v>
       </c>
       <c r="P28" s="4">
@@ -9643,10 +9742,10 @@
       <c r="L29" t="s">
         <v>105</v>
       </c>
-      <c r="N29" s="16">
+      <c r="N29" s="19">
         <v>12</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="19">
         <v>8</v>
       </c>
       <c r="P29" s="4">
@@ -9661,10 +9760,10 @@
       <c r="M30" t="s">
         <v>94</v>
       </c>
-      <c r="N30" s="16">
+      <c r="N30" s="19">
         <v>5</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30" s="19">
         <v>3</v>
       </c>
       <c r="P30" s="4">
@@ -9676,10 +9775,10 @@
       <c r="M31" t="s">
         <v>93</v>
       </c>
-      <c r="N31" s="16">
+      <c r="N31" s="19">
         <v>8</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="19">
         <v>7</v>
       </c>
       <c r="P31" s="4">
@@ -9691,10 +9790,10 @@
       <c r="M32" t="s">
         <v>50</v>
       </c>
-      <c r="N32" s="16">
+      <c r="N32" s="19">
         <v>2</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32" s="19">
         <v>1</v>
       </c>
       <c r="P32" s="4">
@@ -9706,10 +9805,10 @@
       <c r="L33" t="s">
         <v>106</v>
       </c>
-      <c r="N33" s="16">
+      <c r="N33" s="19">
         <v>15</v>
       </c>
-      <c r="O33" s="16">
+      <c r="O33" s="19">
         <v>11</v>
       </c>
       <c r="P33" s="4">
@@ -9724,10 +9823,10 @@
       <c r="M34" t="s">
         <v>94</v>
       </c>
-      <c r="N34" s="16">
-        <v>1</v>
-      </c>
-      <c r="O34" s="16">
+      <c r="N34" s="19">
+        <v>1</v>
+      </c>
+      <c r="O34" s="19">
         <v>0</v>
       </c>
       <c r="P34" s="4">
@@ -9739,10 +9838,10 @@
       <c r="M35" t="s">
         <v>93</v>
       </c>
-      <c r="N35" s="16">
-        <v>1</v>
-      </c>
-      <c r="O35" s="16">
+      <c r="N35" s="19">
+        <v>1</v>
+      </c>
+      <c r="O35" s="19">
         <v>1</v>
       </c>
       <c r="P35" s="4">
@@ -9754,10 +9853,10 @@
       <c r="L36" t="s">
         <v>109</v>
       </c>
-      <c r="N36" s="16">
+      <c r="N36" s="19">
         <v>2</v>
       </c>
-      <c r="O36" s="16">
+      <c r="O36" s="19">
         <v>1</v>
       </c>
       <c r="P36" s="4">
@@ -9772,10 +9871,10 @@
       <c r="M37" t="s">
         <v>94</v>
       </c>
-      <c r="N37" s="16">
+      <c r="N37" s="19">
         <v>2</v>
       </c>
-      <c r="O37" s="16">
+      <c r="O37" s="19">
         <v>2</v>
       </c>
       <c r="P37" s="4">
@@ -9787,10 +9886,10 @@
       <c r="M38" t="s">
         <v>93</v>
       </c>
-      <c r="N38" s="16">
+      <c r="N38" s="19">
         <v>3</v>
       </c>
-      <c r="O38" s="16">
+      <c r="O38" s="19">
         <v>1</v>
       </c>
       <c r="P38" s="4">
@@ -9802,10 +9901,10 @@
       <c r="L39" t="s">
         <v>111</v>
       </c>
-      <c r="N39" s="16">
+      <c r="N39" s="19">
         <v>5</v>
       </c>
-      <c r="O39" s="16">
+      <c r="O39" s="19">
         <v>3</v>
       </c>
       <c r="P39" s="4">
@@ -9820,10 +9919,10 @@
       <c r="M40" t="s">
         <v>94</v>
       </c>
-      <c r="N40" s="16">
+      <c r="N40" s="19">
         <v>4</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O40" s="19">
         <v>2</v>
       </c>
       <c r="P40" s="4">
@@ -9835,10 +9934,10 @@
       <c r="M41" t="s">
         <v>93</v>
       </c>
-      <c r="N41" s="16">
+      <c r="N41" s="19">
         <v>3</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41" s="19">
         <v>3</v>
       </c>
       <c r="P41" s="4">
@@ -9850,10 +9949,10 @@
       <c r="M42" t="s">
         <v>50</v>
       </c>
-      <c r="N42" s="16">
-        <v>1</v>
-      </c>
-      <c r="O42" s="16">
+      <c r="N42" s="19">
+        <v>1</v>
+      </c>
+      <c r="O42" s="19">
         <v>1</v>
       </c>
       <c r="P42" s="4">
@@ -9865,10 +9964,10 @@
       <c r="L43" t="s">
         <v>113</v>
       </c>
-      <c r="N43" s="16">
+      <c r="N43" s="19">
         <v>8</v>
       </c>
-      <c r="O43" s="16">
+      <c r="O43" s="19">
         <v>6</v>
       </c>
       <c r="P43" s="4">
@@ -9880,10 +9979,10 @@
       <c r="L44" t="s">
         <v>53</v>
       </c>
-      <c r="N44" s="16">
+      <c r="N44" s="19">
         <v>115</v>
       </c>
-      <c r="O44" s="16">
+      <c r="O44" s="19">
         <v>79</v>
       </c>
       <c r="P44" s="4"/>
@@ -9983,10 +10082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I509"/>
+  <dimension ref="A1:I516"/>
   <sheetViews>
-    <sheetView topLeftCell="A471" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I510" sqref="I510"/>
+    <sheetView topLeftCell="A465" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I517" sqref="I517"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24387,32 +24486,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A497" s="17" t="s">
+    <row r="497" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A497" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B497" s="18">
+      <c r="B497" s="17">
         <v>45346</v>
       </c>
-      <c r="C497" s="17" t="s">
+      <c r="C497" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D497" s="19">
+      <c r="D497" s="18">
         <v>0.78380000000000005</v>
       </c>
-      <c r="E497" s="17" t="s">
+      <c r="E497" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F497" s="19">
+      <c r="F497" s="18">
         <v>0.2162</v>
       </c>
-      <c r="G497" s="17" t="s">
+      <c r="G497" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H497" s="17" t="s">
+      <c r="H497" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="I497" s="17">
+      <c r="I497" s="16">
         <v>1</v>
       </c>
     </row>
@@ -24471,7 +24570,7 @@
         <v>94</v>
       </c>
       <c r="I499">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="500" spans="1:9" x14ac:dyDescent="0.25">
@@ -24587,7 +24686,7 @@
         <v>51</v>
       </c>
       <c r="I503">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="504" spans="1:9" x14ac:dyDescent="0.25">
@@ -24761,6 +24860,209 @@
         <v>85</v>
       </c>
       <c r="I509">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>115</v>
+      </c>
+      <c r="B510" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C510" t="s">
+        <v>25</v>
+      </c>
+      <c r="D510" s="14">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="E510" t="s">
+        <v>34</v>
+      </c>
+      <c r="F510" s="14">
+        <v>0.23130000000000001</v>
+      </c>
+      <c r="G510" t="s">
+        <v>35</v>
+      </c>
+      <c r="H510" t="s">
+        <v>93</v>
+      </c>
+      <c r="I510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>115</v>
+      </c>
+      <c r="B511" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C511" t="s">
+        <v>37</v>
+      </c>
+      <c r="D511" s="14">
+        <v>0.68979999999999997</v>
+      </c>
+      <c r="E511" t="s">
+        <v>14</v>
+      </c>
+      <c r="F511" s="14">
+        <v>0.31019999999999998</v>
+      </c>
+      <c r="G511" t="s">
+        <v>15</v>
+      </c>
+      <c r="H511" t="s">
+        <v>51</v>
+      </c>
+      <c r="I511">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>115</v>
+      </c>
+      <c r="B512" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C512" t="s">
+        <v>20</v>
+      </c>
+      <c r="D512" s="14">
+        <v>0.67620000000000002</v>
+      </c>
+      <c r="E512" t="s">
+        <v>17</v>
+      </c>
+      <c r="F512" s="14">
+        <v>0.32379999999999998</v>
+      </c>
+      <c r="G512" t="s">
+        <v>18</v>
+      </c>
+      <c r="H512" t="s">
+        <v>51</v>
+      </c>
+      <c r="I512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>115</v>
+      </c>
+      <c r="B513" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C513" t="s">
+        <v>16</v>
+      </c>
+      <c r="D513" s="14">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E513" t="s">
+        <v>5</v>
+      </c>
+      <c r="F513" s="14">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G513" t="s">
+        <v>76</v>
+      </c>
+      <c r="H513" t="s">
+        <v>51</v>
+      </c>
+      <c r="I513">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>115</v>
+      </c>
+      <c r="B514" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C514" t="s">
+        <v>43</v>
+      </c>
+      <c r="D514" s="14">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="E514" t="s">
+        <v>46</v>
+      </c>
+      <c r="F514" s="14">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G514" t="s">
+        <v>47</v>
+      </c>
+      <c r="H514" t="s">
+        <v>51</v>
+      </c>
+      <c r="I514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>115</v>
+      </c>
+      <c r="B515" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C515" t="s">
+        <v>66</v>
+      </c>
+      <c r="D515" s="14">
+        <v>0.63970000000000005</v>
+      </c>
+      <c r="E515" t="s">
+        <v>8</v>
+      </c>
+      <c r="F515" s="14">
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="G515" t="s">
+        <v>67</v>
+      </c>
+      <c r="H515" t="s">
+        <v>51</v>
+      </c>
+      <c r="I515">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="516" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>115</v>
+      </c>
+      <c r="B516" s="1">
+        <v>45347</v>
+      </c>
+      <c r="C516" t="s">
+        <v>11</v>
+      </c>
+      <c r="D516" s="14">
+        <v>0.55489999999999995</v>
+      </c>
+      <c r="E516" t="s">
+        <v>22</v>
+      </c>
+      <c r="F516" s="14">
+        <v>0.4451</v>
+      </c>
+      <c r="G516" t="s">
+        <v>68</v>
+      </c>
+      <c r="H516" t="s">
+        <v>84</v>
+      </c>
+      <c r="I516">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated predictions - missed a line for 227 games
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E33793-0D44-446C-9121-84057161401A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F4D76-045A-415F-831F-B10384F250AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -994,7 +994,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45350.487995601849" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="534" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45350.490695370368" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="534" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
@@ -1100,7 +1100,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="802">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="804">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1590,9 +1590,11 @@
         <n v="0.56657800000000003"/>
         <n v="0.56054199999999998"/>
         <n v="0.55309900000000001"/>
-        <n v="0.8"/>
-        <n v="0.68"/>
+        <n v="0.79600000000000004"/>
+        <n v="0.7"/>
         <m/>
+        <n v="0.8" u="1"/>
+        <n v="0.68" u="1"/>
         <n v="0.77869999999999995" u="1"/>
         <n v="0.63949999999999996" u="1"/>
         <n v="0.87610539305886403" u="1"/>
@@ -7789,7 +7791,7 @@
     <s v="New York Rangers"/>
     <x v="489"/>
     <s v="Columbus Blue Jackets"/>
-    <n v="0.2"/>
+    <n v="0.20399999999999999"/>
     <s v="Playing At:  New York Rangers   Home"/>
     <x v="1"/>
     <n v="1"/>
@@ -7800,7 +7802,7 @@
     <s v="Edmonton Oilers"/>
     <x v="490"/>
     <s v="St. Louis Blues"/>
-    <n v="0.32"/>
+    <n v="0.3"/>
     <s v="Playing At:  Edmonton Oilers   Home"/>
     <x v="2"/>
     <n v="1"/>
@@ -7820,218 +7822,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L3:O44" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="14">
-        <item h="1" x="12"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="10">
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="2"/>
-        <item x="6"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="41">
-    <i>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -8135,10 +7926,8 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="803">
+      <items count="805">
         <item x="491"/>
-        <item m="1" x="494"/>
-        <item m="1" x="495"/>
         <item m="1" x="496"/>
         <item m="1" x="497"/>
         <item m="1" x="498"/>
@@ -8439,14 +8228,16 @@
         <item m="1" x="793"/>
         <item m="1" x="794"/>
         <item m="1" x="795"/>
-        <item x="314"/>
         <item m="1" x="796"/>
         <item m="1" x="797"/>
+        <item x="314"/>
         <item m="1" x="798"/>
         <item m="1" x="799"/>
         <item m="1" x="800"/>
+        <item m="1" x="801"/>
+        <item m="1" x="802"/>
         <item x="9"/>
-        <item m="1" x="801"/>
+        <item m="1" x="803"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -8900,8 +8691,8 @@
         <item x="452"/>
         <item x="453"/>
         <item x="454"/>
-        <item m="1" x="492"/>
-        <item m="1" x="493"/>
+        <item m="1" x="494"/>
+        <item m="1" x="495"/>
         <item x="455"/>
         <item x="456"/>
         <item x="457"/>
@@ -8936,6 +8727,8 @@
         <item x="486"/>
         <item x="487"/>
         <item x="488"/>
+        <item m="1" x="492"/>
+        <item m="1" x="493"/>
         <item x="489"/>
         <item x="490"/>
         <item t="default"/>
@@ -9006,6 +8799,217 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
+  <dataFields count="2">
+    <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80C3D042-980E-40EE-B50F-CF37801A1A1D}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L3:O44" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="14">
+        <item h="1" x="12"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="10">
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="41">
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner1" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="8" baseField="0" baseItem="0"/>
@@ -9322,7 +9326,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10321,7 +10325,7 @@
   <dimension ref="A1:I534"/>
   <sheetViews>
     <sheetView topLeftCell="A526" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D533" sqref="D533"/>
+      <selection activeCell="B554" sqref="B554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25776,14 +25780,14 @@
       <c r="C533" t="s">
         <v>25</v>
       </c>
-      <c r="D533" s="15">
-        <v>0.8</v>
+      <c r="D533" s="14">
+        <v>0.79600000000000004</v>
       </c>
       <c r="E533" t="s">
         <v>34</v>
       </c>
-      <c r="F533" s="15">
-        <v>0.2</v>
+      <c r="F533" s="14">
+        <v>0.20399999999999999</v>
       </c>
       <c r="G533" t="s">
         <v>60</v>
@@ -25805,14 +25809,14 @@
       <c r="C534" t="s">
         <v>10</v>
       </c>
-      <c r="D534" s="15">
-        <v>0.68</v>
+      <c r="D534" s="14">
+        <v>0.7</v>
       </c>
       <c r="E534" t="s">
         <v>13</v>
       </c>
-      <c r="F534" s="15">
-        <v>0.32</v>
+      <c r="F534" s="14">
+        <v>0.3</v>
       </c>
       <c r="G534" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
caught up on predictions
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5AC082-0CAD-4FF5-8AAB-A72B1FB07C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D5886-3879-4708-A1EC-64075CCB1120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3363" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>PDA13</t>
+  </si>
+  <si>
+    <t>PDA14</t>
   </si>
 </sst>
 </file>
@@ -967,13 +970,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45360.429782754632" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="615" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45366.954089120372" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="666" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Model Used" numFmtId="0">
-      <sharedItems containsBlank="1" count="14">
+      <sharedItems containsBlank="1" count="15">
         <s v="PDA1"/>
         <s v="PDA2"/>
         <s v="PDA3"/>
@@ -987,11 +990,12 @@
         <s v="PDA11"/>
         <s v="PDA12"/>
         <s v="PDA13"/>
+        <s v="PDA14"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-03-10T00:00:00" count="86">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-03-17T00:00:00" count="93">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1077,6 +1081,13 @@
         <d v="2024-03-07T00:00:00"/>
         <d v="2024-03-08T00:00:00"/>
         <d v="2024-03-09T00:00:00"/>
+        <d v="2024-03-10T00:00:00"/>
+        <d v="2024-03-11T00:00:00"/>
+        <d v="2024-03-12T00:00:00"/>
+        <d v="2024-03-13T00:00:00"/>
+        <d v="2024-03-14T00:00:00"/>
+        <d v="2024-03-15T00:00:00"/>
+        <d v="2024-03-16T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1084,7 +1095,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="874">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.87610539305886403" count="920">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1646,6 +1657,52 @@
         <n v="0.51585000000000003"/>
         <n v="0.51412000000000002"/>
         <n v="0.51246999999999998"/>
+        <n v="0.72140000000000004"/>
+        <n v="0.64580000000000004"/>
+        <n v="0.5605"/>
+        <n v="0.55900000000000005"/>
+        <n v="0.53700000000000003"/>
+        <n v="0.75109999999999999"/>
+        <n v="0.69410000000000005"/>
+        <n v="0.6704"/>
+        <n v="0.66579999999999995"/>
+        <n v="0.74167000000000005"/>
+        <n v="0.69716999999999996"/>
+        <n v="0.63897000000000004"/>
+        <n v="0.627"/>
+        <n v="0.56140000000000001"/>
+        <n v="0.53274999999999995"/>
+        <n v="0.53056999999999999"/>
+        <n v="0.52647999999999995"/>
+        <n v="0.52551000000000003"/>
+        <n v="0.51153999999999999"/>
+        <n v="0.50700000000000001"/>
+        <n v="0.84289999999999998"/>
+        <n v="0.74580000000000002"/>
+        <n v="0.72860000000000003"/>
+        <n v="0.6673"/>
+        <n v="0.65280000000000005"/>
+        <n v="0.63890000000000002"/>
+        <n v="0.6038"/>
+        <n v="0.58399999999999996"/>
+        <n v="0.56710000000000005"/>
+        <n v="0.53410000000000002"/>
+        <n v="0.77"/>
+        <n v="0.754"/>
+        <n v="0.71775"/>
+        <n v="0.65488000000000002"/>
+        <n v="0.64836000000000005"/>
+        <n v="0.64793999999999996"/>
+        <n v="0.63331999999999999"/>
+        <n v="0.63127999999999995"/>
+        <n v="0.61917999999999995"/>
+        <n v="0.59323000000000004"/>
+        <n v="0.58160000000000001"/>
+        <n v="0.55976000000000004"/>
+        <n v="0.54193999999999998"/>
+        <n v="0.52844000000000002"/>
+        <n v="0.52571000000000001"/>
+        <n v="0.51376999999999995"/>
         <m/>
         <n v="0.8" u="1"/>
         <n v="0.68" u="1"/>
@@ -1997,7 +2054,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="615">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="666">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -8755,8 +8812,569 @@
   <r>
     <x v="13"/>
     <x v="85"/>
+    <s v="Carolina Hurricanes"/>
+    <x v="561"/>
+    <s v="Calgary Flames"/>
+    <n v="0.27860000000000001"/>
+    <s v="Playing At:  Carolina Hurricanes   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="85"/>
+    <s v="Edmonton Oilers"/>
+    <x v="562"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.35420000000000001"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="85"/>
+    <s v="Arizona Coyotes"/>
+    <x v="563"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.4395"/>
+    <s v="Playing At:  Chicago Blackhawks   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="85"/>
+    <s v="New York Islanders"/>
+    <x v="564"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.441"/>
+    <s v="Playing At:  Anaheim Ducks   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="85"/>
+    <s v="Minnesota Wild"/>
+    <x v="565"/>
+    <s v="Nashville Predators"/>
+    <n v="0.46300000000000002"/>
+    <s v="Playing At:  Minnesota Wild   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="86"/>
+    <s v="Boston Bruins"/>
+    <x v="566"/>
+    <s v="St. Louis Blues"/>
+    <n v="0.24890000000000001"/>
+    <s v="Playing At:  Boston Bruins   Home"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="86"/>
+    <s v="Winnipeg Jets"/>
+    <x v="567"/>
+    <s v="Washington Capitals"/>
+    <n v="0.30590000000000001"/>
+    <s v="Playing At:  Winnipeg Jets   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="86"/>
+    <s v="Los Angeles Kings"/>
+    <x v="568"/>
+    <s v="New York Islanders"/>
+    <n v="0.3296"/>
+    <s v="Playing At:  Los Angeles Kings   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="86"/>
+    <s v="New York Rangers"/>
+    <x v="569"/>
+    <s v="New Jersey Devils"/>
+    <n v="0.3342"/>
+    <s v="Playing At:  New York Rangers   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Philadelphia Flyers"/>
+    <x v="570"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.25833"/>
+    <s v="Playing At:  Philadelphia Flyers   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Minnesota Wild"/>
+    <x v="571"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.30282999999999999"/>
+    <s v="Playing At:  Minnesota Wild   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Colorado Avalanche"/>
+    <x v="572"/>
+    <s v="Calgary Flames"/>
+    <n v="0.36103000000000002"/>
+    <s v="Playing At:  Calgary Flames   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Montreal Canadiens"/>
+    <x v="573"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.373"/>
+    <s v="Playing At:  Montreal Canadiens   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Vegas Golden Knights"/>
+    <x v="574"/>
+    <s v="Seattle Kraken"/>
+    <n v="0.43859999999999999"/>
+    <s v="Playing At:  Seattle Kraken   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="New York Rangers"/>
+    <x v="575"/>
+    <s v="Carolina Hurricanes"/>
+    <n v="0.46725"/>
+    <s v="Playing At:  Carolina Hurricanes   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Anaheim Ducks"/>
+    <x v="576"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.46943000000000001"/>
+    <s v="Playing At:  Chicago Blackhawks   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Buffalo Sabres"/>
+    <x v="577"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.47352"/>
+    <s v="Playing At:  Buffalo Sabres   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Ottawa Senators"/>
+    <x v="578"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.47449000000000002"/>
+    <s v="Playing At:  Ottawa Senators   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="87"/>
+    <s v="Dallas Stars"/>
+    <x v="579"/>
+    <s v="Florida Panthers"/>
+    <n v="0.48846000000000001"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="88"/>
+    <s v="Edmonton Oilers"/>
+    <x v="368"/>
+    <s v="Washington Capitals"/>
+    <n v="0.29099999999999998"/>
+    <s v="Playing At:  Edmonton Oilers   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="88"/>
+    <s v="Winnipeg Jets"/>
+    <x v="307"/>
+    <s v="Nashville Predators"/>
+    <n v="0.40300000000000002"/>
+    <s v="Playing At:  Winnipeg Jets   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="88"/>
+    <s v="Los Angeles Kings"/>
+    <x v="541"/>
+    <s v="St. Louis Blues"/>
+    <n v="0.438"/>
+    <s v="Playing At:  St. Louis Blues   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="88"/>
+    <s v="Colorado Avalanche"/>
+    <x v="580"/>
+    <s v="Vancouver Canucks"/>
+    <n v="0.49299999999999999"/>
+    <s v="Playing At:  Vancouver Canucks   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Boston Bruins"/>
+    <x v="581"/>
+    <s v="Montreal Canadiens"/>
+    <n v="0.15709999999999999"/>
+    <s v="Playing At:  Montreal Canadiens   Home"/>
+    <x v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Pittsburgh Penguins"/>
+    <x v="582"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.25419999999999998"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Minnesota Wild"/>
+    <x v="583"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.27139999999999997"/>
+    <s v="Playing At:  Minnesota Wild   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Detroit Red Wings"/>
+    <x v="36"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.32729999999999998"/>
+    <s v="Playing At:  Detroit Red Wings   Home"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Toronto Maple Leafs"/>
+    <x v="584"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.3327"/>
+    <s v="Playing At:  Philadelphia Flyers   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Ottawa Senators"/>
+    <x v="585"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.34720000000000001"/>
+    <s v="Playing At:  Columbus Blue Jackets   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Seattle Kraken"/>
+    <x v="586"/>
+    <s v="Washington Capitals"/>
+    <n v="0.36109999999999998"/>
+    <s v="Playing At:  Seattle Kraken   Home"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Dallas Stars"/>
+    <x v="573"/>
+    <s v="New Jersey Devils"/>
+    <n v="0.373"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <x v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Buffalo Sabres"/>
+    <x v="587"/>
+    <s v="New York Islanders"/>
+    <n v="0.3962"/>
+    <s v="Playing At:  Buffalo Sabres   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Vegas Golden Knights"/>
+    <x v="588"/>
+    <s v="Calgary Flames"/>
+    <n v="0.41599999999999998"/>
+    <s v="Playing At:  Calgary Flames   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="New York Rangers"/>
+    <x v="589"/>
+    <s v="Tampa Bay Lightning"/>
+    <n v="0.43290000000000001"/>
+    <s v="Playing At:  Tampa Bay Lightning   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="89"/>
+    <s v="Carolina Hurricanes"/>
+    <x v="590"/>
+    <s v="Florida Panthers"/>
+    <n v="0.46589999999999998"/>
+    <s v="Playing At:  Carolina Hurricanes   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="90"/>
+    <s v="Los Angeles Kings"/>
+    <x v="591"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.23"/>
+    <s v="Playing At:  Chicago Blackhawks   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="90"/>
+    <s v="Winnipeg Jets"/>
+    <x v="592"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.246"/>
+    <s v="Playing At:  Winnipeg Jets   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Boston Bruins"/>
+    <x v="593"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.28225"/>
+    <s v="Playing At:  Boston Bruins   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Calgary Flames"/>
+    <x v="594"/>
+    <s v="Montreal Canadiens"/>
+    <n v="0.34511999999999998"/>
+    <s v="Playing At:  Calgary Flames   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="New Jersey Devils"/>
+    <x v="595"/>
+    <s v="Arizona Coyotes"/>
+    <n v="0.35164000000000001"/>
+    <s v="Playing At:  Arizona Coyotes   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Dallas Stars"/>
+    <x v="596"/>
+    <s v="Los Angeles Kings"/>
+    <n v="0.35205999999999998"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="New York Rangers"/>
+    <x v="597"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.36668000000000001"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Florida Panthers"/>
+    <x v="598"/>
+    <s v="Tampa Bay Lightning"/>
+    <n v="0.36871999999999999"/>
+    <s v="Playing At:  Florida Panthers   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Vancouver Canucks"/>
+    <x v="599"/>
+    <s v="Washington Capitals"/>
+    <n v="0.38081999999999999"/>
+    <s v="Playing At:  Vancouver Canucks   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Edmonton Oilers"/>
+    <x v="600"/>
+    <s v="Colorado Avalanche"/>
+    <n v="0.40677000000000002"/>
+    <s v="Playing At:  Edmonton Oilers   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Columbus Blue Jackets"/>
+    <x v="601"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.41839999999999999"/>
+    <s v="Playing At:  Columbus Blue Jackets   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="New York Islanders"/>
+    <x v="602"/>
+    <s v="Ottawa Senators"/>
+    <n v="0.44024000000000002"/>
+    <s v="Playing At:  New York Islanders   Home"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Carolina Hurricanes"/>
+    <x v="603"/>
+    <s v="Toronto Maple Leafs"/>
+    <n v="0.45806000000000002"/>
+    <s v="Playing At:  Toronto Maple Leafs   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Detroit Red Wings"/>
+    <x v="604"/>
+    <s v="Buffalo Sabres"/>
+    <n v="0.47155999999999998"/>
+    <s v="Playing At:  Detroit Red Wings   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="Seattle Kraken"/>
+    <x v="605"/>
+    <s v="Nashville Predators"/>
+    <n v="0.47428999999999999"/>
+    <s v="Playing At:  Seattle Kraken   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="91"/>
+    <s v="St. Louis Blues"/>
+    <x v="606"/>
+    <s v="Minnesota Wild"/>
+    <n v="0.48623"/>
+    <s v="Playing At:  St. Louis Blues   Home"/>
+    <x v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="92"/>
     <m/>
-    <x v="561"/>
+    <x v="607"/>
     <m/>
     <m/>
     <m/>
@@ -8767,12 +9385,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="15">
-        <item x="13"/>
+      <items count="16">
+        <item x="14"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -8786,11 +9404,12 @@
         <item x="10"/>
         <item x="11"/>
         <item x="12"/>
+        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="87">
+      <items count="94">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -8830,7 +9449,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="85"/>
+        <item x="92"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -8877,59 +9496,20 @@
         <item x="82"/>
         <item x="83"/>
         <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="875">
-        <item x="561"/>
-        <item m="1" x="566"/>
-        <item m="1" x="567"/>
-        <item m="1" x="568"/>
-        <item m="1" x="569"/>
-        <item m="1" x="570"/>
-        <item m="1" x="571"/>
-        <item m="1" x="572"/>
-        <item m="1" x="573"/>
-        <item m="1" x="574"/>
-        <item m="1" x="575"/>
-        <item m="1" x="576"/>
-        <item m="1" x="577"/>
-        <item m="1" x="578"/>
-        <item m="1" x="579"/>
-        <item m="1" x="580"/>
-        <item m="1" x="581"/>
-        <item m="1" x="582"/>
-        <item m="1" x="583"/>
-        <item m="1" x="584"/>
-        <item m="1" x="585"/>
-        <item m="1" x="586"/>
-        <item m="1" x="587"/>
-        <item m="1" x="588"/>
-        <item m="1" x="589"/>
-        <item m="1" x="590"/>
-        <item m="1" x="591"/>
-        <item m="1" x="592"/>
-        <item m="1" x="593"/>
-        <item m="1" x="594"/>
-        <item m="1" x="595"/>
-        <item m="1" x="596"/>
-        <item m="1" x="597"/>
-        <item m="1" x="598"/>
-        <item m="1" x="599"/>
-        <item m="1" x="600"/>
-        <item m="1" x="601"/>
-        <item m="1" x="602"/>
-        <item m="1" x="603"/>
-        <item m="1" x="604"/>
-        <item m="1" x="605"/>
-        <item m="1" x="606"/>
-        <item m="1" x="607"/>
-        <item m="1" x="608"/>
-        <item m="1" x="609"/>
-        <item m="1" x="610"/>
-        <item m="1" x="611"/>
+      <items count="921">
+        <item x="607"/>
         <item m="1" x="612"/>
         <item m="1" x="613"/>
         <item m="1" x="614"/>
@@ -9186,14 +9766,60 @@
         <item m="1" x="865"/>
         <item m="1" x="866"/>
         <item m="1" x="867"/>
-        <item x="314"/>
         <item m="1" x="868"/>
         <item m="1" x="869"/>
         <item m="1" x="870"/>
         <item m="1" x="871"/>
         <item m="1" x="872"/>
+        <item m="1" x="873"/>
+        <item m="1" x="874"/>
+        <item m="1" x="875"/>
+        <item m="1" x="876"/>
+        <item m="1" x="877"/>
+        <item m="1" x="878"/>
+        <item m="1" x="879"/>
+        <item m="1" x="880"/>
+        <item m="1" x="881"/>
+        <item m="1" x="882"/>
+        <item m="1" x="883"/>
+        <item m="1" x="884"/>
+        <item m="1" x="885"/>
+        <item m="1" x="886"/>
+        <item m="1" x="887"/>
+        <item m="1" x="888"/>
+        <item m="1" x="889"/>
+        <item m="1" x="890"/>
+        <item m="1" x="891"/>
+        <item m="1" x="892"/>
+        <item m="1" x="893"/>
+        <item m="1" x="894"/>
+        <item m="1" x="895"/>
+        <item m="1" x="896"/>
+        <item m="1" x="897"/>
+        <item m="1" x="898"/>
+        <item m="1" x="899"/>
+        <item m="1" x="900"/>
+        <item m="1" x="901"/>
+        <item m="1" x="902"/>
+        <item m="1" x="903"/>
+        <item m="1" x="904"/>
+        <item m="1" x="905"/>
+        <item m="1" x="906"/>
+        <item m="1" x="907"/>
+        <item m="1" x="908"/>
+        <item m="1" x="909"/>
+        <item m="1" x="910"/>
+        <item m="1" x="911"/>
+        <item m="1" x="912"/>
+        <item m="1" x="913"/>
+        <item x="314"/>
+        <item m="1" x="914"/>
+        <item m="1" x="915"/>
+        <item m="1" x="916"/>
+        <item m="1" x="917"/>
+        <item m="1" x="918"/>
         <item x="9"/>
-        <item m="1" x="873"/>
+        <item m="1" x="919"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -9647,8 +10273,8 @@
         <item x="452"/>
         <item x="453"/>
         <item x="454"/>
-        <item m="1" x="564"/>
-        <item m="1" x="565"/>
+        <item m="1" x="610"/>
+        <item m="1" x="611"/>
         <item x="455"/>
         <item x="456"/>
         <item x="457"/>
@@ -9683,8 +10309,8 @@
         <item x="486"/>
         <item x="487"/>
         <item x="488"/>
-        <item m="1" x="562"/>
-        <item m="1" x="563"/>
+        <item m="1" x="608"/>
+        <item m="1" x="609"/>
         <item x="489"/>
         <item x="490"/>
         <item x="491"/>
@@ -9757,6 +10383,52 @@
         <item x="558"/>
         <item x="559"/>
         <item x="560"/>
+        <item x="561"/>
+        <item x="562"/>
+        <item x="563"/>
+        <item x="564"/>
+        <item x="565"/>
+        <item x="566"/>
+        <item x="567"/>
+        <item x="568"/>
+        <item x="569"/>
+        <item x="570"/>
+        <item x="571"/>
+        <item x="572"/>
+        <item x="573"/>
+        <item x="574"/>
+        <item x="575"/>
+        <item x="576"/>
+        <item x="577"/>
+        <item x="578"/>
+        <item x="579"/>
+        <item x="580"/>
+        <item x="581"/>
+        <item x="582"/>
+        <item x="583"/>
+        <item x="584"/>
+        <item x="585"/>
+        <item x="586"/>
+        <item x="587"/>
+        <item x="588"/>
+        <item x="589"/>
+        <item x="590"/>
+        <item x="591"/>
+        <item x="592"/>
+        <item x="593"/>
+        <item x="594"/>
+        <item x="595"/>
+        <item x="596"/>
+        <item x="597"/>
+        <item x="598"/>
+        <item x="599"/>
+        <item x="600"/>
+        <item x="601"/>
+        <item x="602"/>
+        <item x="603"/>
+        <item x="604"/>
+        <item x="605"/>
+        <item x="606"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -10141,7 +10813,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10223,19 +10895,19 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>466</v>
+        <v>507</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H6" s="9">
         <f>SUM(B6:B7)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -10243,30 +10915,30 @@
         <v>50</v>
       </c>
       <c r="B7" s="19">
+        <v>18</v>
+      </c>
+      <c r="C7" s="19">
         <v>17</v>
-      </c>
-      <c r="C7" s="19">
-        <v>16</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" ref="D7:D13" si="0">C7/B7</f>
-        <v>0.94117647058823528</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="E7" s="7">
         <f>SUM(C10:C12)</f>
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="F7" s="5">
         <f>SUM(C6:C9)</f>
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H7" s="9">
         <f>SUM(C6:C7)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -10274,10 +10946,10 @@
         <v>93</v>
       </c>
       <c r="B8" s="19">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C8" s="19">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
@@ -10285,19 +10957,19 @@
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.53862660944206009</v>
+        <v>0.54635108481262329</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.71621621621621623</v>
+        <v>0.72784810126582278</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
-        <v>0.7407407407407407</v>
+        <v>0.74117647058823533</v>
       </c>
       <c r="H8" s="10">
         <f>H7/H6</f>
-        <v>0.95238095238095233</v>
+        <v>0.95454545454545459</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -10305,14 +10977,14 @@
         <v>94</v>
       </c>
       <c r="B9" s="19">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C9" s="19">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>0.68656716417910446</v>
+        <v>0.71232876712328763</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>100</v>
@@ -10332,30 +11004,30 @@
         <v>51</v>
       </c>
       <c r="B10" s="19">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="C10" s="19">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>0.59024390243902436</v>
+        <v>0.6116071428571429</v>
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.75895765472312704</v>
+        <v>0.76240601503759398</v>
       </c>
       <c r="F10" s="6">
         <f>F6/$B$13</f>
-        <v>0.24104234527687296</v>
+        <v>0.23759398496240602</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" ref="G10:H10" si="1">G6/$B$13</f>
-        <v>0.13192182410423453</v>
+        <v>0.12781954887218044</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="1"/>
-        <v>3.4201954397394138E-2</v>
+        <v>3.308270676691729E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -10363,14 +11035,14 @@
         <v>84</v>
       </c>
       <c r="B11" s="19">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C11" s="19">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>0.5234375</v>
+        <v>0.51449275362318836</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -10378,14 +11050,14 @@
         <v>85</v>
       </c>
       <c r="B12" s="19">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C12" s="19">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>0.47368421052631576</v>
+        <v>0.47586206896551725</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -10393,14 +11065,14 @@
         <v>53</v>
       </c>
       <c r="B13" s="19">
-        <v>614</v>
+        <v>665</v>
       </c>
       <c r="C13" s="19">
-        <v>357</v>
+        <v>392</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="0"/>
-        <v>0.58143322475570036</v>
+        <v>0.58947368421052626</v>
       </c>
     </row>
     <row r="47" spans="16:16" x14ac:dyDescent="0.35">
@@ -10465,10 +11137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I615"/>
+  <dimension ref="A1:I666"/>
   <sheetViews>
-    <sheetView topLeftCell="A591" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I616" sqref="I616"/>
+    <sheetView topLeftCell="A638" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I667" sqref="I667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28320,6 +28992,1485 @@
         <v>0</v>
       </c>
     </row>
+    <row r="616" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A616" t="s">
+        <v>107</v>
+      </c>
+      <c r="B616" s="1">
+        <v>45361</v>
+      </c>
+      <c r="C616" t="s">
+        <v>43</v>
+      </c>
+      <c r="D616" s="14">
+        <v>0.72140000000000004</v>
+      </c>
+      <c r="E616" t="s">
+        <v>31</v>
+      </c>
+      <c r="F616" s="14">
+        <v>0.27860000000000001</v>
+      </c>
+      <c r="G616" t="s">
+        <v>74</v>
+      </c>
+      <c r="H616" t="s">
+        <v>94</v>
+      </c>
+      <c r="I616">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="617" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A617" t="s">
+        <v>107</v>
+      </c>
+      <c r="B617" s="1">
+        <v>45361</v>
+      </c>
+      <c r="C617" t="s">
+        <v>10</v>
+      </c>
+      <c r="D617" s="14">
+        <v>0.64580000000000004</v>
+      </c>
+      <c r="E617" t="s">
+        <v>66</v>
+      </c>
+      <c r="F617" s="14">
+        <v>0.35420000000000001</v>
+      </c>
+      <c r="G617" t="s">
+        <v>67</v>
+      </c>
+      <c r="H617" t="s">
+        <v>51</v>
+      </c>
+      <c r="I617">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="618" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A618" t="s">
+        <v>107</v>
+      </c>
+      <c r="B618" s="1">
+        <v>45361</v>
+      </c>
+      <c r="C618" t="s">
+        <v>5</v>
+      </c>
+      <c r="D618" s="14">
+        <v>0.5605</v>
+      </c>
+      <c r="E618" t="s">
+        <v>14</v>
+      </c>
+      <c r="F618" s="14">
+        <v>0.4395</v>
+      </c>
+      <c r="G618" t="s">
+        <v>15</v>
+      </c>
+      <c r="H618" t="s">
+        <v>84</v>
+      </c>
+      <c r="I618">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A619" t="s">
+        <v>107</v>
+      </c>
+      <c r="B619" s="1">
+        <v>45361</v>
+      </c>
+      <c r="C619" t="s">
+        <v>39</v>
+      </c>
+      <c r="D619" s="14">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="E619" t="s">
+        <v>17</v>
+      </c>
+      <c r="F619" s="14">
+        <v>0.441</v>
+      </c>
+      <c r="G619" t="s">
+        <v>18</v>
+      </c>
+      <c r="H619" t="s">
+        <v>84</v>
+      </c>
+      <c r="I619">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="620" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A620" t="s">
+        <v>107</v>
+      </c>
+      <c r="B620" s="1">
+        <v>45361</v>
+      </c>
+      <c r="C620" t="s">
+        <v>58</v>
+      </c>
+      <c r="D620" s="14">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="E620" t="s">
+        <v>20</v>
+      </c>
+      <c r="F620" s="14">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G620" t="s">
+        <v>72</v>
+      </c>
+      <c r="H620" t="s">
+        <v>85</v>
+      </c>
+      <c r="I620">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="621" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A621" t="s">
+        <v>107</v>
+      </c>
+      <c r="B621" s="1">
+        <v>45362</v>
+      </c>
+      <c r="C621" t="s">
+        <v>4</v>
+      </c>
+      <c r="D621" s="14">
+        <v>0.75109999999999999</v>
+      </c>
+      <c r="E621" t="s">
+        <v>13</v>
+      </c>
+      <c r="F621" s="14">
+        <v>0.24890000000000001</v>
+      </c>
+      <c r="G621" t="s">
+        <v>6</v>
+      </c>
+      <c r="H621" t="s">
+        <v>93</v>
+      </c>
+      <c r="I621">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A622" t="s">
+        <v>107</v>
+      </c>
+      <c r="B622" s="1">
+        <v>45362</v>
+      </c>
+      <c r="C622" t="s">
+        <v>16</v>
+      </c>
+      <c r="D622" s="14">
+        <v>0.69410000000000005</v>
+      </c>
+      <c r="E622" t="s">
+        <v>26</v>
+      </c>
+      <c r="F622" s="14">
+        <v>0.30590000000000001</v>
+      </c>
+      <c r="G622" t="s">
+        <v>76</v>
+      </c>
+      <c r="H622" t="s">
+        <v>51</v>
+      </c>
+      <c r="I622">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="623" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A623" t="s">
+        <v>107</v>
+      </c>
+      <c r="B623" s="1">
+        <v>45362</v>
+      </c>
+      <c r="C623" t="s">
+        <v>40</v>
+      </c>
+      <c r="D623" s="14">
+        <v>0.6704</v>
+      </c>
+      <c r="E623" t="s">
+        <v>39</v>
+      </c>
+      <c r="F623" s="14">
+        <v>0.3296</v>
+      </c>
+      <c r="G623" t="s">
+        <v>69</v>
+      </c>
+      <c r="H623" t="s">
+        <v>51</v>
+      </c>
+      <c r="I623">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="624" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A624" t="s">
+        <v>107</v>
+      </c>
+      <c r="B624" s="1">
+        <v>45362</v>
+      </c>
+      <c r="C624" t="s">
+        <v>25</v>
+      </c>
+      <c r="D624" s="14">
+        <v>0.66579999999999995</v>
+      </c>
+      <c r="E624" t="s">
+        <v>11</v>
+      </c>
+      <c r="F624" s="14">
+        <v>0.3342</v>
+      </c>
+      <c r="G624" t="s">
+        <v>60</v>
+      </c>
+      <c r="H624" t="s">
+        <v>51</v>
+      </c>
+      <c r="I624">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="625" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A625" t="s">
+        <v>107</v>
+      </c>
+      <c r="B625" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C625" t="s">
+        <v>8</v>
+      </c>
+      <c r="D625" s="14">
+        <v>0.74167000000000005</v>
+      </c>
+      <c r="E625" t="s">
+        <v>56</v>
+      </c>
+      <c r="F625" s="14">
+        <v>0.25833</v>
+      </c>
+      <c r="G625" t="s">
+        <v>73</v>
+      </c>
+      <c r="H625" t="s">
+        <v>94</v>
+      </c>
+      <c r="I625">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="626" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A626" t="s">
+        <v>107</v>
+      </c>
+      <c r="B626" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C626" t="s">
+        <v>58</v>
+      </c>
+      <c r="D626" s="14">
+        <v>0.69716999999999996</v>
+      </c>
+      <c r="E626" t="s">
+        <v>5</v>
+      </c>
+      <c r="F626" s="14">
+        <v>0.30282999999999999</v>
+      </c>
+      <c r="G626" t="s">
+        <v>72</v>
+      </c>
+      <c r="H626" t="s">
+        <v>51</v>
+      </c>
+      <c r="I626">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="627" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A627" t="s">
+        <v>107</v>
+      </c>
+      <c r="B627" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C627" t="s">
+        <v>7</v>
+      </c>
+      <c r="D627" s="14">
+        <v>0.63897000000000004</v>
+      </c>
+      <c r="E627" t="s">
+        <v>31</v>
+      </c>
+      <c r="F627" s="14">
+        <v>0.36103000000000002</v>
+      </c>
+      <c r="G627" t="s">
+        <v>32</v>
+      </c>
+      <c r="H627" t="s">
+        <v>51</v>
+      </c>
+      <c r="I627">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="628" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A628" t="s">
+        <v>107</v>
+      </c>
+      <c r="B628" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C628" t="s">
+        <v>45</v>
+      </c>
+      <c r="D628" s="14">
+        <v>0.627</v>
+      </c>
+      <c r="E628" t="s">
+        <v>34</v>
+      </c>
+      <c r="F628" s="14">
+        <v>0.373</v>
+      </c>
+      <c r="G628" t="s">
+        <v>59</v>
+      </c>
+      <c r="H628" t="s">
+        <v>51</v>
+      </c>
+      <c r="I628">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="629" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A629" t="s">
+        <v>107</v>
+      </c>
+      <c r="B629" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C629" t="s">
+        <v>29</v>
+      </c>
+      <c r="D629" s="14">
+        <v>0.56140000000000001</v>
+      </c>
+      <c r="E629" t="s">
+        <v>23</v>
+      </c>
+      <c r="F629" s="14">
+        <v>0.43859999999999999</v>
+      </c>
+      <c r="G629" t="s">
+        <v>24</v>
+      </c>
+      <c r="H629" t="s">
+        <v>84</v>
+      </c>
+      <c r="I629">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="630" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A630" t="s">
+        <v>107</v>
+      </c>
+      <c r="B630" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C630" t="s">
+        <v>25</v>
+      </c>
+      <c r="D630" s="14">
+        <v>0.53274999999999995</v>
+      </c>
+      <c r="E630" t="s">
+        <v>43</v>
+      </c>
+      <c r="F630" s="14">
+        <v>0.46725</v>
+      </c>
+      <c r="G630" t="s">
+        <v>74</v>
+      </c>
+      <c r="H630" t="s">
+        <v>85</v>
+      </c>
+      <c r="I630">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="631" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A631" t="s">
+        <v>107</v>
+      </c>
+      <c r="B631" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C631" t="s">
+        <v>17</v>
+      </c>
+      <c r="D631" s="14">
+        <v>0.53056999999999999</v>
+      </c>
+      <c r="E631" t="s">
+        <v>14</v>
+      </c>
+      <c r="F631" s="14">
+        <v>0.46943000000000001</v>
+      </c>
+      <c r="G631" t="s">
+        <v>15</v>
+      </c>
+      <c r="H631" t="s">
+        <v>85</v>
+      </c>
+      <c r="I631">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A632" t="s">
+        <v>107</v>
+      </c>
+      <c r="B632" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C632" t="s">
+        <v>46</v>
+      </c>
+      <c r="D632" s="14">
+        <v>0.52647999999999995</v>
+      </c>
+      <c r="E632" t="s">
+        <v>37</v>
+      </c>
+      <c r="F632" s="14">
+        <v>0.47352</v>
+      </c>
+      <c r="G632" t="s">
+        <v>47</v>
+      </c>
+      <c r="H632" t="s">
+        <v>85</v>
+      </c>
+      <c r="I632">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="633" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A633" t="s">
+        <v>107</v>
+      </c>
+      <c r="B633" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C633" t="s">
+        <v>36</v>
+      </c>
+      <c r="D633" s="14">
+        <v>0.52551000000000003</v>
+      </c>
+      <c r="E633" t="s">
+        <v>66</v>
+      </c>
+      <c r="F633" s="14">
+        <v>0.47449000000000002</v>
+      </c>
+      <c r="G633" t="s">
+        <v>64</v>
+      </c>
+      <c r="H633" t="s">
+        <v>85</v>
+      </c>
+      <c r="I633">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="634" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A634" t="s">
+        <v>107</v>
+      </c>
+      <c r="B634" s="1">
+        <v>45363</v>
+      </c>
+      <c r="C634" t="s">
+        <v>28</v>
+      </c>
+      <c r="D634" s="14">
+        <v>0.51153999999999999</v>
+      </c>
+      <c r="E634" t="s">
+        <v>33</v>
+      </c>
+      <c r="F634" s="14">
+        <v>0.48846000000000001</v>
+      </c>
+      <c r="G634" t="s">
+        <v>30</v>
+      </c>
+      <c r="H634" t="s">
+        <v>85</v>
+      </c>
+      <c r="I634">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A635" t="s">
+        <v>107</v>
+      </c>
+      <c r="B635" s="1">
+        <v>45364</v>
+      </c>
+      <c r="C635" t="s">
+        <v>10</v>
+      </c>
+      <c r="D635" s="14">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E635" t="s">
+        <v>26</v>
+      </c>
+      <c r="F635" s="14">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="G635" t="s">
+        <v>12</v>
+      </c>
+      <c r="H635" t="s">
+        <v>94</v>
+      </c>
+      <c r="I635">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="636" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A636" t="s">
+        <v>107</v>
+      </c>
+      <c r="B636" s="1">
+        <v>45364</v>
+      </c>
+      <c r="C636" t="s">
+        <v>16</v>
+      </c>
+      <c r="D636" s="14">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="E636" t="s">
+        <v>20</v>
+      </c>
+      <c r="F636" s="14">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="G636" t="s">
+        <v>76</v>
+      </c>
+      <c r="H636" t="s">
+        <v>84</v>
+      </c>
+      <c r="I636">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A637" t="s">
+        <v>107</v>
+      </c>
+      <c r="B637" s="1">
+        <v>45364</v>
+      </c>
+      <c r="C637" t="s">
+        <v>40</v>
+      </c>
+      <c r="D637" s="14">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="E637" t="s">
+        <v>13</v>
+      </c>
+      <c r="F637" s="14">
+        <v>0.438</v>
+      </c>
+      <c r="G637" t="s">
+        <v>65</v>
+      </c>
+      <c r="H637" t="s">
+        <v>84</v>
+      </c>
+      <c r="I637">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A638" t="s">
+        <v>107</v>
+      </c>
+      <c r="B638" s="1">
+        <v>45364</v>
+      </c>
+      <c r="C638" t="s">
+        <v>7</v>
+      </c>
+      <c r="D638" s="14">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E638" t="s">
+        <v>42</v>
+      </c>
+      <c r="F638" s="14">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="G638" t="s">
+        <v>44</v>
+      </c>
+      <c r="H638" t="s">
+        <v>85</v>
+      </c>
+      <c r="I638">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="639" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A639" t="s">
+        <v>107</v>
+      </c>
+      <c r="B639" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C639" t="s">
+        <v>4</v>
+      </c>
+      <c r="D639" s="14">
+        <v>0.84289999999999998</v>
+      </c>
+      <c r="E639" t="s">
+        <v>45</v>
+      </c>
+      <c r="F639" s="14">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="G639" t="s">
+        <v>59</v>
+      </c>
+      <c r="H639" t="s">
+        <v>50</v>
+      </c>
+      <c r="I639">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="640" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A640" t="s">
+        <v>107</v>
+      </c>
+      <c r="B640" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C640" t="s">
+        <v>66</v>
+      </c>
+      <c r="D640" s="14">
+        <v>0.74580000000000002</v>
+      </c>
+      <c r="E640" t="s">
+        <v>56</v>
+      </c>
+      <c r="F640" s="14">
+        <v>0.25419999999999998</v>
+      </c>
+      <c r="G640" t="s">
+        <v>67</v>
+      </c>
+      <c r="H640" t="s">
+        <v>94</v>
+      </c>
+      <c r="I640">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="641" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A641" t="s">
+        <v>107</v>
+      </c>
+      <c r="B641" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C641" t="s">
+        <v>58</v>
+      </c>
+      <c r="D641" s="14">
+        <v>0.72860000000000003</v>
+      </c>
+      <c r="E641" t="s">
+        <v>17</v>
+      </c>
+      <c r="F641" s="14">
+        <v>0.27139999999999997</v>
+      </c>
+      <c r="G641" t="s">
+        <v>72</v>
+      </c>
+      <c r="H641" t="s">
+        <v>94</v>
+      </c>
+      <c r="I641">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="642" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A642" t="s">
+        <v>107</v>
+      </c>
+      <c r="B642" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C642" t="s">
+        <v>37</v>
+      </c>
+      <c r="D642" s="14">
+        <v>0.67269999999999996</v>
+      </c>
+      <c r="E642" t="s">
+        <v>5</v>
+      </c>
+      <c r="F642" s="14">
+        <v>0.32729999999999998</v>
+      </c>
+      <c r="G642" t="s">
+        <v>38</v>
+      </c>
+      <c r="H642" t="s">
+        <v>51</v>
+      </c>
+      <c r="I642">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A643" t="s">
+        <v>107</v>
+      </c>
+      <c r="B643" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C643" t="s">
+        <v>19</v>
+      </c>
+      <c r="D643" s="14">
+        <v>0.6673</v>
+      </c>
+      <c r="E643" t="s">
+        <v>8</v>
+      </c>
+      <c r="F643" s="14">
+        <v>0.3327</v>
+      </c>
+      <c r="G643" t="s">
+        <v>73</v>
+      </c>
+      <c r="H643" t="s">
+        <v>51</v>
+      </c>
+      <c r="I643">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="644" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A644" t="s">
+        <v>107</v>
+      </c>
+      <c r="B644" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C644" t="s">
+        <v>36</v>
+      </c>
+      <c r="D644" s="14">
+        <v>0.65280000000000005</v>
+      </c>
+      <c r="E644" t="s">
+        <v>34</v>
+      </c>
+      <c r="F644" s="14">
+        <v>0.34720000000000001</v>
+      </c>
+      <c r="G644" t="s">
+        <v>35</v>
+      </c>
+      <c r="H644" t="s">
+        <v>51</v>
+      </c>
+      <c r="I644">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="645" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A645" t="s">
+        <v>107</v>
+      </c>
+      <c r="B645" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C645" t="s">
+        <v>23</v>
+      </c>
+      <c r="D645" s="14">
+        <v>0.63890000000000002</v>
+      </c>
+      <c r="E645" t="s">
+        <v>26</v>
+      </c>
+      <c r="F645" s="14">
+        <v>0.36109999999999998</v>
+      </c>
+      <c r="G645" t="s">
+        <v>24</v>
+      </c>
+      <c r="H645" t="s">
+        <v>51</v>
+      </c>
+      <c r="I645">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="646" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A646" t="s">
+        <v>107</v>
+      </c>
+      <c r="B646" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C646" t="s">
+        <v>28</v>
+      </c>
+      <c r="D646" s="14">
+        <v>0.627</v>
+      </c>
+      <c r="E646" t="s">
+        <v>11</v>
+      </c>
+      <c r="F646" s="14">
+        <v>0.373</v>
+      </c>
+      <c r="G646" t="s">
+        <v>30</v>
+      </c>
+      <c r="H646" t="s">
+        <v>51</v>
+      </c>
+      <c r="I646">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A647" t="s">
+        <v>107</v>
+      </c>
+      <c r="B647" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C647" t="s">
+        <v>46</v>
+      </c>
+      <c r="D647" s="14">
+        <v>0.6038</v>
+      </c>
+      <c r="E647" t="s">
+        <v>39</v>
+      </c>
+      <c r="F647" s="14">
+        <v>0.3962</v>
+      </c>
+      <c r="G647" t="s">
+        <v>47</v>
+      </c>
+      <c r="H647" t="s">
+        <v>51</v>
+      </c>
+      <c r="I647">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="648" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A648" t="s">
+        <v>107</v>
+      </c>
+      <c r="B648" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C648" t="s">
+        <v>29</v>
+      </c>
+      <c r="D648" s="14">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E648" t="s">
+        <v>31</v>
+      </c>
+      <c r="F648" s="14">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G648" t="s">
+        <v>32</v>
+      </c>
+      <c r="H648" t="s">
+        <v>84</v>
+      </c>
+      <c r="I648">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="649" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A649" t="s">
+        <v>107</v>
+      </c>
+      <c r="B649" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C649" t="s">
+        <v>25</v>
+      </c>
+      <c r="D649" s="14">
+        <v>0.56710000000000005</v>
+      </c>
+      <c r="E649" t="s">
+        <v>22</v>
+      </c>
+      <c r="F649" s="14">
+        <v>0.43290000000000001</v>
+      </c>
+      <c r="G649" t="s">
+        <v>77</v>
+      </c>
+      <c r="H649" t="s">
+        <v>84</v>
+      </c>
+      <c r="I649">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="650" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A650" t="s">
+        <v>107</v>
+      </c>
+      <c r="B650" s="1">
+        <v>45365</v>
+      </c>
+      <c r="C650" t="s">
+        <v>43</v>
+      </c>
+      <c r="D650" s="14">
+        <v>0.53410000000000002</v>
+      </c>
+      <c r="E650" t="s">
+        <v>33</v>
+      </c>
+      <c r="F650" s="14">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="G650" t="s">
+        <v>74</v>
+      </c>
+      <c r="H650" t="s">
+        <v>85</v>
+      </c>
+      <c r="I650">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="651" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A651" t="s">
+        <v>107</v>
+      </c>
+      <c r="B651" s="1">
+        <v>45366</v>
+      </c>
+      <c r="C651" t="s">
+        <v>40</v>
+      </c>
+      <c r="D651" s="14">
+        <v>0.77</v>
+      </c>
+      <c r="E651" t="s">
+        <v>14</v>
+      </c>
+      <c r="F651" s="14">
+        <v>0.23</v>
+      </c>
+      <c r="G651" t="s">
+        <v>15</v>
+      </c>
+      <c r="H651" t="s">
+        <v>93</v>
+      </c>
+      <c r="I651">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="652" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A652" t="s">
+        <v>107</v>
+      </c>
+      <c r="B652" s="1">
+        <v>45366</v>
+      </c>
+      <c r="C652" t="s">
+        <v>16</v>
+      </c>
+      <c r="D652" s="14">
+        <v>0.754</v>
+      </c>
+      <c r="E652" t="s">
+        <v>17</v>
+      </c>
+      <c r="F652" s="14">
+        <v>0.246</v>
+      </c>
+      <c r="G652" t="s">
+        <v>76</v>
+      </c>
+      <c r="H652" t="s">
+        <v>93</v>
+      </c>
+      <c r="I652">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="653" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A653" t="s">
+        <v>107</v>
+      </c>
+      <c r="B653" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C653" t="s">
+        <v>4</v>
+      </c>
+      <c r="D653" s="14">
+        <v>0.71775</v>
+      </c>
+      <c r="E653" t="s">
+        <v>8</v>
+      </c>
+      <c r="F653" s="14">
+        <v>0.28225</v>
+      </c>
+      <c r="G653" t="s">
+        <v>6</v>
+      </c>
+      <c r="H653" t="s">
+        <v>94</v>
+      </c>
+      <c r="I653">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="654" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A654" t="s">
+        <v>107</v>
+      </c>
+      <c r="B654" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C654" t="s">
+        <v>31</v>
+      </c>
+      <c r="D654" s="14">
+        <v>0.65488000000000002</v>
+      </c>
+      <c r="E654" t="s">
+        <v>45</v>
+      </c>
+      <c r="F654" s="14">
+        <v>0.34511999999999998</v>
+      </c>
+      <c r="G654" t="s">
+        <v>32</v>
+      </c>
+      <c r="H654" t="s">
+        <v>51</v>
+      </c>
+      <c r="I654">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="655" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A655" t="s">
+        <v>107</v>
+      </c>
+      <c r="B655" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C655" t="s">
+        <v>11</v>
+      </c>
+      <c r="D655" s="14">
+        <v>0.64836000000000005</v>
+      </c>
+      <c r="E655" t="s">
+        <v>5</v>
+      </c>
+      <c r="F655" s="14">
+        <v>0.35164000000000001</v>
+      </c>
+      <c r="G655" t="s">
+        <v>75</v>
+      </c>
+      <c r="H655" t="s">
+        <v>51</v>
+      </c>
+      <c r="I655">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="656" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A656" t="s">
+        <v>107</v>
+      </c>
+      <c r="B656" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C656" t="s">
+        <v>28</v>
+      </c>
+      <c r="D656" s="14">
+        <v>0.64793999999999996</v>
+      </c>
+      <c r="E656" t="s">
+        <v>40</v>
+      </c>
+      <c r="F656" s="14">
+        <v>0.35205999999999998</v>
+      </c>
+      <c r="G656" t="s">
+        <v>30</v>
+      </c>
+      <c r="H656" t="s">
+        <v>51</v>
+      </c>
+      <c r="I656">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="657" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A657" t="s">
+        <v>107</v>
+      </c>
+      <c r="B657" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C657" t="s">
+        <v>25</v>
+      </c>
+      <c r="D657" s="14">
+        <v>0.63331999999999999</v>
+      </c>
+      <c r="E657" t="s">
+        <v>66</v>
+      </c>
+      <c r="F657" s="14">
+        <v>0.36668000000000001</v>
+      </c>
+      <c r="G657" t="s">
+        <v>67</v>
+      </c>
+      <c r="H657" t="s">
+        <v>51</v>
+      </c>
+      <c r="I657">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="658" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A658" t="s">
+        <v>107</v>
+      </c>
+      <c r="B658" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C658" t="s">
+        <v>33</v>
+      </c>
+      <c r="D658" s="14">
+        <v>0.63127999999999995</v>
+      </c>
+      <c r="E658" t="s">
+        <v>22</v>
+      </c>
+      <c r="F658" s="14">
+        <v>0.36871999999999999</v>
+      </c>
+      <c r="G658" t="s">
+        <v>78</v>
+      </c>
+      <c r="H658" t="s">
+        <v>51</v>
+      </c>
+      <c r="I658">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="659" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A659" t="s">
+        <v>107</v>
+      </c>
+      <c r="B659" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C659" t="s">
+        <v>42</v>
+      </c>
+      <c r="D659" s="14">
+        <v>0.61917999999999995</v>
+      </c>
+      <c r="E659" t="s">
+        <v>26</v>
+      </c>
+      <c r="F659" s="14">
+        <v>0.38081999999999999</v>
+      </c>
+      <c r="G659" t="s">
+        <v>44</v>
+      </c>
+      <c r="H659" t="s">
+        <v>51</v>
+      </c>
+      <c r="I659">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="660" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A660" t="s">
+        <v>107</v>
+      </c>
+      <c r="B660" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C660" t="s">
+        <v>10</v>
+      </c>
+      <c r="D660" s="14">
+        <v>0.59323000000000004</v>
+      </c>
+      <c r="E660" t="s">
+        <v>7</v>
+      </c>
+      <c r="F660" s="14">
+        <v>0.40677000000000002</v>
+      </c>
+      <c r="G660" t="s">
+        <v>12</v>
+      </c>
+      <c r="H660" t="s">
+        <v>84</v>
+      </c>
+      <c r="I660">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A661" t="s">
+        <v>107</v>
+      </c>
+      <c r="B661" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C661" t="s">
+        <v>34</v>
+      </c>
+      <c r="D661" s="14">
+        <v>0.58160000000000001</v>
+      </c>
+      <c r="E661" t="s">
+        <v>56</v>
+      </c>
+      <c r="F661" s="14">
+        <v>0.41839999999999999</v>
+      </c>
+      <c r="G661" t="s">
+        <v>35</v>
+      </c>
+      <c r="H661" t="s">
+        <v>84</v>
+      </c>
+      <c r="I661">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="662" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A662" t="s">
+        <v>107</v>
+      </c>
+      <c r="B662" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C662" t="s">
+        <v>39</v>
+      </c>
+      <c r="D662" s="14">
+        <v>0.55976000000000004</v>
+      </c>
+      <c r="E662" t="s">
+        <v>36</v>
+      </c>
+      <c r="F662" s="14">
+        <v>0.44024000000000002</v>
+      </c>
+      <c r="G662" t="s">
+        <v>41</v>
+      </c>
+      <c r="H662" t="s">
+        <v>84</v>
+      </c>
+      <c r="I662">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="663" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A663" t="s">
+        <v>107</v>
+      </c>
+      <c r="B663" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C663" t="s">
+        <v>43</v>
+      </c>
+      <c r="D663" s="14">
+        <v>0.54193999999999998</v>
+      </c>
+      <c r="E663" t="s">
+        <v>19</v>
+      </c>
+      <c r="F663" s="14">
+        <v>0.45806000000000002</v>
+      </c>
+      <c r="G663" t="s">
+        <v>21</v>
+      </c>
+      <c r="H663" t="s">
+        <v>85</v>
+      </c>
+      <c r="I663">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="664" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A664" t="s">
+        <v>107</v>
+      </c>
+      <c r="B664" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C664" t="s">
+        <v>37</v>
+      </c>
+      <c r="D664" s="14">
+        <v>0.52844000000000002</v>
+      </c>
+      <c r="E664" t="s">
+        <v>46</v>
+      </c>
+      <c r="F664" s="14">
+        <v>0.47155999999999998</v>
+      </c>
+      <c r="G664" t="s">
+        <v>38</v>
+      </c>
+      <c r="H664" t="s">
+        <v>85</v>
+      </c>
+      <c r="I664">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="665" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A665" t="s">
+        <v>107</v>
+      </c>
+      <c r="B665" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C665" t="s">
+        <v>23</v>
+      </c>
+      <c r="D665" s="14">
+        <v>0.52571000000000001</v>
+      </c>
+      <c r="E665" t="s">
+        <v>20</v>
+      </c>
+      <c r="F665" s="14">
+        <v>0.47428999999999999</v>
+      </c>
+      <c r="G665" t="s">
+        <v>24</v>
+      </c>
+      <c r="H665" t="s">
+        <v>85</v>
+      </c>
+      <c r="I665">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A666" t="s">
+        <v>107</v>
+      </c>
+      <c r="B666" s="1">
+        <v>45367</v>
+      </c>
+      <c r="C666" t="s">
+        <v>13</v>
+      </c>
+      <c r="D666" s="14">
+        <v>0.51376999999999995</v>
+      </c>
+      <c r="E666" t="s">
+        <v>58</v>
+      </c>
+      <c r="F666" s="14">
+        <v>0.48623</v>
+      </c>
+      <c r="G666" t="s">
+        <v>65</v>
+      </c>
+      <c r="H666" t="s">
+        <v>85</v>
+      </c>
+      <c r="I666">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated predictions and model
</commit_message>
<xml_diff>
--- a/PDA Lifetime Predictions.xlsx
+++ b/PDA Lifetime Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743541F4-68DD-4AFC-B9DC-B8C14479EBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1196F05D-1949-4D8B-B0F7-505B5F98C11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="14" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3898" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3943" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>PDA16</t>
+  </si>
+  <si>
+    <t>PDA17</t>
   </si>
 </sst>
 </file>
@@ -976,13 +979,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45381.393940856484" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="773" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45383.401314467592" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="782" xr:uid="{D3A71568-3061-40C8-A74B-8B86C64C3ADC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Model Used" numFmtId="0">
-      <sharedItems containsBlank="1" count="17">
+      <sharedItems containsBlank="1" count="18">
         <s v="PDA1"/>
         <s v="PDA2"/>
         <s v="PDA3"/>
@@ -999,11 +1002,12 @@
         <s v="PDA14"/>
         <s v="PDA15"/>
         <s v="PDA16"/>
+        <s v="PDA17"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-03-31T00:00:00" count="107">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-09T00:00:00" maxDate="2024-04-02T00:00:00" count="109">
         <d v="2023-12-09T00:00:00"/>
         <d v="2023-12-10T00:00:00"/>
         <d v="2023-12-11T00:00:00"/>
@@ -1110,6 +1114,8 @@
         <d v="2024-03-28T00:00:00"/>
         <d v="2024-03-29T00:00:00"/>
         <d v="2024-03-30T00:00:00"/>
+        <d v="2024-03-31T00:00:00"/>
+        <d v="2024-04-01T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1117,7 +1123,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.9" count="1011">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="0.9" count="1017">
         <n v="0.87609999999999999"/>
         <n v="0.78059999999999996"/>
         <n v="0.65859999999999996"/>
@@ -1816,6 +1822,12 @@
         <n v="0.54027999999999998"/>
         <n v="0.52869999999999995"/>
         <n v="0.50849999999999995"/>
+        <n v="0.73829999999999996"/>
+        <n v="0.6734"/>
+        <n v="0.64510000000000001"/>
+        <n v="0.55969999999999998"/>
+        <n v="0.55530000000000002"/>
+        <n v="0.53539999999999999"/>
         <m/>
         <n v="0.8" u="1"/>
         <n v="0.68" u="1"/>
@@ -2167,7 +2179,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="773">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="782">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -10515,7 +10527,7 @@
     <n v="0.24772"/>
     <s v="Playing At:  St. Louis Blues   Home"/>
     <x v="1"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="15"/>
@@ -10570,7 +10582,7 @@
     <n v="0.31448999999999999"/>
     <s v="Playing At:  Washington Capitals   Home"/>
     <x v="2"/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <x v="15"/>
@@ -10581,7 +10593,7 @@
     <n v="0.31818999999999997"/>
     <s v="Playing At:  Winnipeg Jets   Home"/>
     <x v="2"/>
-    <n v="1"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="15"/>
@@ -10647,7 +10659,7 @@
     <n v="0.4713"/>
     <s v="Playing At:  Calgary Flames   Home"/>
     <x v="4"/>
-    <n v="0"/>
+    <n v="1"/>
   </r>
   <r>
     <x v="15"/>
@@ -10663,8 +10675,107 @@
   <r>
     <x v="16"/>
     <x v="106"/>
+    <s v="Vancouver Canucks"/>
+    <x v="591"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.23"/>
+    <s v="Playing At:  Vancouver Canucks   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="New York Rangers"/>
+    <x v="566"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.24890000000000001"/>
+    <s v="Playing At:  New York Rangers   Home"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Colorado Avalanche"/>
+    <x v="698"/>
+    <s v="Columbus Blue Jackets"/>
+    <n v="0.26169999999999999"/>
+    <s v="Playing At:  Columbus Blue Jackets   Home"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Seattle Kraken"/>
+    <x v="699"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.3266"/>
+    <s v="Playing At:  San Jose Sharks   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Edmonton Oilers"/>
+    <x v="700"/>
+    <s v="St. Louis Blues"/>
+    <n v="0.35489999999999999"/>
+    <s v="Playing At:  St. Louis Blues   Home"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Philadelphia Flyers"/>
+    <x v="701"/>
+    <s v="New York Islanders"/>
+    <n v="0.44030000000000002"/>
+    <s v="Playing At:  Philadelphia Flyers   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Winnipeg Jets"/>
+    <x v="702"/>
+    <s v="Los Angeles Kings"/>
+    <n v="0.44469999999999998"/>
+    <s v="Playing At:  Winnipeg Jets   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Florida Panthers"/>
+    <x v="635"/>
+    <s v="Toronto Maple Leafs"/>
+    <n v="0.44979999999999998"/>
+    <s v="Playing At:  Toronto Maple Leafs   Home"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="107"/>
+    <s v="Tampa Bay Lightning"/>
+    <x v="703"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.46460000000000001"/>
+    <s v="Playing At:  Tampa Bay Lightning   Home"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="108"/>
     <m/>
-    <x v="698"/>
+    <x v="704"/>
     <m/>
     <m/>
     <m/>
@@ -10675,12 +10786,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1FB34DD3-8207-4009-92F5-73C183F63DF8}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="18">
-        <item x="16"/>
+      <items count="19">
+        <item x="17"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -10697,11 +10808,12 @@
         <item x="13"/>
         <item x="14"/>
         <item x="15"/>
+        <item x="16"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="108">
+      <items count="110">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -10741,7 +10853,7 @@
         <item x="36"/>
         <item x="37"/>
         <item x="38"/>
-        <item x="106"/>
+        <item x="108"/>
         <item x="39"/>
         <item x="40"/>
         <item x="41"/>
@@ -10809,19 +10921,15 @@
         <item x="103"/>
         <item x="104"/>
         <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="1012">
-        <item x="698"/>
-        <item m="1" x="703"/>
-        <item m="1" x="704"/>
-        <item m="1" x="705"/>
-        <item m="1" x="706"/>
-        <item m="1" x="707"/>
-        <item m="1" x="708"/>
+      <items count="1018">
+        <item x="704"/>
         <item m="1" x="709"/>
         <item m="1" x="710"/>
         <item m="1" x="711"/>
@@ -11118,14 +11226,20 @@
         <item m="1" x="1002"/>
         <item m="1" x="1003"/>
         <item m="1" x="1004"/>
-        <item x="314"/>
         <item m="1" x="1005"/>
         <item m="1" x="1006"/>
         <item m="1" x="1007"/>
         <item m="1" x="1008"/>
         <item m="1" x="1009"/>
+        <item m="1" x="1010"/>
+        <item x="314"/>
+        <item m="1" x="1011"/>
+        <item m="1" x="1012"/>
+        <item m="1" x="1013"/>
+        <item m="1" x="1014"/>
+        <item m="1" x="1015"/>
         <item x="9"/>
-        <item m="1" x="1010"/>
+        <item m="1" x="1016"/>
         <item x="286"/>
         <item x="287"/>
         <item x="288"/>
@@ -11579,8 +11693,8 @@
         <item x="452"/>
         <item x="453"/>
         <item x="454"/>
-        <item m="1" x="701"/>
-        <item m="1" x="702"/>
+        <item m="1" x="707"/>
+        <item m="1" x="708"/>
         <item x="455"/>
         <item x="456"/>
         <item x="457"/>
@@ -11615,8 +11729,8 @@
         <item x="486"/>
         <item x="487"/>
         <item x="488"/>
-        <item m="1" x="699"/>
-        <item m="1" x="700"/>
+        <item m="1" x="705"/>
+        <item m="1" x="706"/>
         <item x="489"/>
         <item x="490"/>
         <item x="491"/>
@@ -11826,6 +11940,12 @@
         <item x="695"/>
         <item x="696"/>
         <item x="697"/>
+        <item x="698"/>
+        <item x="699"/>
+        <item x="700"/>
+        <item x="701"/>
+        <item x="702"/>
+        <item x="703"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12210,7 +12330,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12292,15 +12412,15 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(B10:B12)</f>
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="F6" s="5">
         <f>SUM(B6:B9)</f>
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G6" s="11">
         <f>SUM(B6:B8)</f>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H6" s="9">
         <f>SUM(B6:B7)</f>
@@ -12323,15 +12443,15 @@
       </c>
       <c r="E7" s="7">
         <f>SUM(C10:C12)</f>
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="F7" s="5">
         <f>SUM(C6:C9)</f>
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G7" s="11">
         <f>SUM(C6:C8)</f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H7" s="9">
         <f>SUM(C6:C7)</f>
@@ -12343,26 +12463,26 @@
         <v>93</v>
       </c>
       <c r="B8" s="19">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" s="19">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>0.68918918918918914</v>
+        <v>0.68421052631578949</v>
       </c>
       <c r="E8" s="8">
         <f>E7/E6</f>
-        <v>0.54436860068259385</v>
+        <v>0.54560810810810811</v>
       </c>
       <c r="F8" s="6">
         <f>F7/F6</f>
-        <v>0.74193548387096775</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="G8" s="12">
         <f>G7/G6</f>
-        <v>0.76923076923076927</v>
+        <v>0.76415094339622647</v>
       </c>
       <c r="H8" s="10">
         <f>H7/H6</f>
@@ -12374,14 +12494,14 @@
         <v>94</v>
       </c>
       <c r="B9" s="19">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" s="19">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>0.70731707317073167</v>
+        <v>0.71084337349397586</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>100</v>
@@ -12401,30 +12521,30 @@
         <v>51</v>
       </c>
       <c r="B10" s="19">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C10" s="19">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>0.59541984732824427</v>
+        <v>0.59848484848484851</v>
       </c>
       <c r="E10" s="8">
         <f>E6/$B$13</f>
-        <v>0.7590673575129534</v>
+        <v>0.75800256081946227</v>
       </c>
       <c r="F10" s="6">
         <f>F6/$B$13</f>
-        <v>0.24093264248704663</v>
+        <v>0.24199743918053776</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" ref="G10:H10" si="1">G6/$B$13</f>
-        <v>0.13471502590673576</v>
+        <v>0.13572343149807939</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="1"/>
-        <v>3.8860103626943004E-2</v>
+        <v>3.8412291933418691E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -12432,14 +12552,14 @@
         <v>84</v>
       </c>
       <c r="B11" s="19">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C11" s="19">
         <v>85</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>0.5214723926380368</v>
+        <v>0.51204819277108438</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -12447,14 +12567,14 @@
         <v>85</v>
       </c>
       <c r="B12" s="19">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C12" s="19">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>0.48447204968944102</v>
+        <v>0.49382716049382713</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -12462,14 +12582,14 @@
         <v>53</v>
       </c>
       <c r="B13" s="19">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="C13" s="19">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="0"/>
-        <v>0.59196891191709844</v>
+        <v>0.59282970550576186</v>
       </c>
     </row>
     <row r="47" spans="16:16" x14ac:dyDescent="0.25">
@@ -12534,10 +12654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I773"/>
+  <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A734" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A759" sqref="A759:XFD762"/>
+    <sheetView tabSelected="1" topLeftCell="A725" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I783" sqref="I783"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34591,7 +34711,7 @@
         <v>93</v>
       </c>
       <c r="I760">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="761" spans="1:9" x14ac:dyDescent="0.25">
@@ -34736,7 +34856,7 @@
         <v>51</v>
       </c>
       <c r="I765">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="766" spans="1:9" x14ac:dyDescent="0.25">
@@ -34765,7 +34885,7 @@
         <v>51</v>
       </c>
       <c r="I766">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="767" spans="1:9" x14ac:dyDescent="0.25">
@@ -34939,7 +35059,7 @@
         <v>85</v>
       </c>
       <c r="I772">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="773" spans="1:9" x14ac:dyDescent="0.25">
@@ -34969,6 +35089,267 @@
       </c>
       <c r="I773">
         <v>0</v>
+      </c>
+    </row>
+    <row r="774" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>110</v>
+      </c>
+      <c r="B774" s="1">
+        <v>45382</v>
+      </c>
+      <c r="C774" t="s">
+        <v>42</v>
+      </c>
+      <c r="D774" s="15">
+        <v>0.77</v>
+      </c>
+      <c r="E774" t="s">
+        <v>17</v>
+      </c>
+      <c r="F774" s="15">
+        <v>0.23</v>
+      </c>
+      <c r="G774" t="s">
+        <v>44</v>
+      </c>
+      <c r="H774" t="s">
+        <v>93</v>
+      </c>
+      <c r="I774">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="775" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A775" t="s">
+        <v>110</v>
+      </c>
+      <c r="B775" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C775" t="s">
+        <v>25</v>
+      </c>
+      <c r="D775" s="14">
+        <v>0.75109999999999999</v>
+      </c>
+      <c r="E775" t="s">
+        <v>66</v>
+      </c>
+      <c r="F775" s="14">
+        <v>0.24890000000000001</v>
+      </c>
+      <c r="G775" t="s">
+        <v>60</v>
+      </c>
+      <c r="H775" t="s">
+        <v>93</v>
+      </c>
+      <c r="I775">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="776" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
+        <v>110</v>
+      </c>
+      <c r="B776" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C776" t="s">
+        <v>7</v>
+      </c>
+      <c r="D776" s="14">
+        <v>0.73829999999999996</v>
+      </c>
+      <c r="E776" t="s">
+        <v>34</v>
+      </c>
+      <c r="F776" s="14">
+        <v>0.26169999999999999</v>
+      </c>
+      <c r="G776" t="s">
+        <v>35</v>
+      </c>
+      <c r="H776" t="s">
+        <v>94</v>
+      </c>
+      <c r="I776">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="777" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A777" t="s">
+        <v>110</v>
+      </c>
+      <c r="B777" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C777" t="s">
+        <v>23</v>
+      </c>
+      <c r="D777" s="14">
+        <v>0.6734</v>
+      </c>
+      <c r="E777" t="s">
+        <v>56</v>
+      </c>
+      <c r="F777" s="14">
+        <v>0.3266</v>
+      </c>
+      <c r="G777" t="s">
+        <v>62</v>
+      </c>
+      <c r="H777" t="s">
+        <v>51</v>
+      </c>
+      <c r="I777">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="778" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A778" t="s">
+        <v>110</v>
+      </c>
+      <c r="B778" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C778" t="s">
+        <v>10</v>
+      </c>
+      <c r="D778" s="14">
+        <v>0.64510000000000001</v>
+      </c>
+      <c r="E778" t="s">
+        <v>13</v>
+      </c>
+      <c r="F778" s="14">
+        <v>0.35489999999999999</v>
+      </c>
+      <c r="G778" t="s">
+        <v>65</v>
+      </c>
+      <c r="H778" t="s">
+        <v>51</v>
+      </c>
+      <c r="I778">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="779" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A779" t="s">
+        <v>110</v>
+      </c>
+      <c r="B779" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C779" t="s">
+        <v>8</v>
+      </c>
+      <c r="D779" s="14">
+        <v>0.55969999999999998</v>
+      </c>
+      <c r="E779" t="s">
+        <v>39</v>
+      </c>
+      <c r="F779" s="14">
+        <v>0.44030000000000002</v>
+      </c>
+      <c r="G779" t="s">
+        <v>73</v>
+      </c>
+      <c r="H779" t="s">
+        <v>84</v>
+      </c>
+      <c r="I779">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="780" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A780" t="s">
+        <v>110</v>
+      </c>
+      <c r="B780" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C780" t="s">
+        <v>16</v>
+      </c>
+      <c r="D780" s="14">
+        <v>0.55530000000000002</v>
+      </c>
+      <c r="E780" t="s">
+        <v>40</v>
+      </c>
+      <c r="F780" s="14">
+        <v>0.44469999999999998</v>
+      </c>
+      <c r="G780" t="s">
+        <v>76</v>
+      </c>
+      <c r="H780" t="s">
+        <v>84</v>
+      </c>
+      <c r="I780">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="781" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A781" t="s">
+        <v>110</v>
+      </c>
+      <c r="B781" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C781" t="s">
+        <v>33</v>
+      </c>
+      <c r="D781" s="14">
+        <v>0.55020000000000002</v>
+      </c>
+      <c r="E781" t="s">
+        <v>19</v>
+      </c>
+      <c r="F781" s="14">
+        <v>0.44979999999999998</v>
+      </c>
+      <c r="G781" t="s">
+        <v>21</v>
+      </c>
+      <c r="H781" t="s">
+        <v>84</v>
+      </c>
+      <c r="I781">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="782" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A782" t="s">
+        <v>110</v>
+      </c>
+      <c r="B782" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C782" t="s">
+        <v>22</v>
+      </c>
+      <c r="D782" s="14">
+        <v>0.53539999999999999</v>
+      </c>
+      <c r="E782" t="s">
+        <v>37</v>
+      </c>
+      <c r="F782" s="14">
+        <v>0.46460000000000001</v>
+      </c>
+      <c r="G782" t="s">
+        <v>77</v>
+      </c>
+      <c r="H782" t="s">
+        <v>85</v>
+      </c>
+      <c r="I782">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>